<commit_message>
fix data related bugs
- fix lam-33, lam-34, lam-54
- fix upload not updating the data because the db was not deleted, not it is
- fix the Excel files having incorrect data
</commit_message>
<xml_diff>
--- a/resources/input_workbook/LAM_metadata_20200903_JKU.xlsx
+++ b/resources/input_workbook/LAM_metadata_20200903_JKU.xlsx
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5775" uniqueCount="2413">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5781" uniqueCount="2415">
   <si>
     <t xml:space="preserve">URI</t>
   </si>
@@ -192,7 +192,7 @@
     <t xml:space="preserve">skos:prefLabel@en</t>
   </si>
   <si>
-    <t xml:space="preserve">lamd:clas_EDIT</t>
+    <t xml:space="preserve">lamd:class_EDIT</t>
   </si>
   <si>
     <t xml:space="preserve">KEYWORD</t>
@@ -261,7 +261,7 @@
     <t xml:space="preserve">Class or subclass according to CDM.</t>
   </si>
   <si>
-    <t xml:space="preserve">lamd:clas_MIS</t>
+    <t xml:space="preserve">lamd:class_MIS</t>
   </si>
   <si>
     <t xml:space="preserve">AU</t>
@@ -809,7 +809,7 @@
     <t xml:space="preserve">Miscellaneous information</t>
   </si>
   <si>
-    <t xml:space="preserve">lamd:clas_ESI</t>
+    <t xml:space="preserve">lamd:class_ESI</t>
   </si>
   <si>
     <t xml:space="preserve">FM</t>
@@ -1101,7 +1101,7 @@
     <t xml:space="preserve">Celex number</t>
   </si>
   <si>
-    <t xml:space="preserve">lamd:clas_CLX</t>
+    <t xml:space="preserve">lamd:class_CLX</t>
   </si>
   <si>
     <t xml:space="preserve">DN_CLASS</t>
@@ -3585,7 +3585,7 @@
     <t xml:space="preserve">Classification</t>
   </si>
   <si>
-    <t xml:space="preserve">lamd:clas_CLAS</t>
+    <t xml:space="preserve">lamd:class_CLAS</t>
   </si>
   <si>
     <t xml:space="preserve">CT</t>
@@ -6090,7 +6090,7 @@
     <t xml:space="preserve">Dates</t>
   </si>
   <si>
-    <t xml:space="preserve">lamd:clas_DPROP</t>
+    <t xml:space="preserve">lamd:class_DPROP</t>
   </si>
   <si>
     <t xml:space="preserve">IF</t>
@@ -11881,7 +11881,7 @@
     <t xml:space="preserve">Legal basis</t>
   </si>
   <si>
-    <t xml:space="preserve">lamd:clas_RBD</t>
+    <t xml:space="preserve">lamd:class_RBD</t>
   </si>
   <si>
     <t xml:space="preserve">AMENDMENT</t>
@@ -11997,7 +11997,7 @@
 Earlier related instruments</t>
   </si>
   <si>
-    <t xml:space="preserve">lamd:clas_MSEA</t>
+    <t xml:space="preserve">lamd:class_MSEA</t>
   </si>
   <si>
     <t xml:space="preserve">ADDITION</t>
@@ -13221,7 +13221,7 @@
     <t xml:space="preserve">Related documents</t>
   </si>
   <si>
-    <t xml:space="preserve">lamd:clas_RD</t>
+    <t xml:space="preserve">lamd:class_RD</t>
   </si>
   <si>
     <t xml:space="preserve">ASSOCIATION</t>
@@ -13294,7 +13294,7 @@
     <t xml:space="preserve">Case law properties</t>
   </si>
   <si>
-    <t xml:space="preserve">lamd:clas_CDJ</t>
+    <t xml:space="preserve">lamd:class_CDJ</t>
   </si>
   <si>
     <t xml:space="preserve">DF</t>
@@ -13384,7 +13384,7 @@
     <t xml:space="preserve">Case affecting</t>
   </si>
   <si>
-    <t xml:space="preserve">lamd:clas_AJ</t>
+    <t xml:space="preserve">lamd:class_AJ</t>
   </si>
   <si>
     <t xml:space="preserve">FAILURE_REQ</t>
@@ -13519,7 +13519,7 @@
     <t xml:space="preserve">Annotations</t>
   </si>
   <si>
-    <t xml:space="preserve">lamd:clas_DANNOT</t>
+    <t xml:space="preserve">lamd:class_DANNOT</t>
   </si>
   <si>
     <t xml:space="preserve">ANN_TOD</t>
@@ -13556,7 +13556,7 @@
     <t xml:space="preserve">2019/06/25: Replacement of fd_370 by at:subdivision should be considered.</t>
   </si>
   <si>
-    <t xml:space="preserve">lamd:clas_RANNOT</t>
+    <t xml:space="preserve">lamd:class_RANNOT</t>
   </si>
   <si>
     <t xml:space="preserve">ANN_ART</t>
@@ -13824,7 +13824,7 @@
     <t xml:space="preserve">Publication reference</t>
   </si>
   <si>
-    <t xml:space="preserve">lamd:clas_OTHER_REF</t>
+    <t xml:space="preserve">lamd:class_OTHER_REF</t>
   </si>
   <si>
     <t xml:space="preserve">ELI</t>
@@ -16000,7 +16000,7 @@
     <t xml:space="preserve">Parliamentary questions (European Parliament)</t>
   </si>
   <si>
-    <t xml:space="preserve">1_/AFI/DCL</t>
+    <t xml:space="preserve">1_AFI_DCL</t>
   </si>
   <si>
     <t xml:space="preserve">Declaration annexed to the Final Act</t>
@@ -16017,7 +16017,7 @@
     <t xml:space="preserve">??</t>
   </si>
   <si>
-    <t xml:space="preserve">1_/PRO</t>
+    <t xml:space="preserve">1_PRO</t>
   </si>
   <si>
     <t xml:space="preserve">Protocol</t>
@@ -16029,7 +16029,7 @@
     <t xml:space="preserve">a separate work for each protocol</t>
   </si>
   <si>
-    <t xml:space="preserve">1_/TXT</t>
+    <t xml:space="preserve">1_TXT</t>
   </si>
   <si>
     <t xml:space="preserve">Treaty - full text</t>
@@ -18833,6 +18833,9 @@
     <t xml:space="preserve">lamd:</t>
   </si>
   <si>
+    <t xml:space="preserve">class_classif:</t>
+  </si>
+  <si>
     <t xml:space="preserve">cdm:</t>
   </si>
   <si>
@@ -18846,6 +18849,9 @@
   </si>
   <si>
     <t xml:space="preserve">http://publications.europa.eu/resources/authority/celex/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">celex_classif:</t>
   </si>
   <si>
     <t xml:space="preserve">sh:</t>
@@ -19347,7 +19353,7 @@
     <numFmt numFmtId="166" formatCode="[$-809]dd/mm/yyyy"/>
     <numFmt numFmtId="167" formatCode="0.00E+00"/>
   </numFmts>
-  <fonts count="32">
+  <fonts count="33">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -19572,6 +19578,12 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -19666,7 +19678,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -19779,6 +19791,10 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -19876,9 +19892,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>219960</xdr:colOff>
+      <xdr:colOff>219600</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>669600</xdr:rowOff>
+      <xdr:rowOff>669240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -19888,7 +19904,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="7830360" cy="8163720"/>
+          <a:ext cx="7830000" cy="8163360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -19921,9 +19937,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
-      <xdr:colOff>637200</xdr:colOff>
+      <xdr:colOff>636840</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>2037240</xdr:rowOff>
+      <xdr:rowOff>2036880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -19933,7 +19949,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="10040040" cy="9531360"/>
+          <a:ext cx="10038960" cy="9531000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -19971,7 +19987,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>453960</xdr:colOff>
+      <xdr:colOff>453600</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>173160</xdr:rowOff>
     </xdr:to>
@@ -19983,7 +19999,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="17856000" cy="5697360"/>
+          <a:ext cx="17856360" cy="4627440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -20025,7 +20041,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A85" activeCellId="0" sqref="A85"/>
+      <selection pane="bottomLeft" activeCell="AJ2" activeCellId="0" sqref="AJ2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="2"/>
@@ -28055,10 +28071,10 @@
   <dimension ref="A1:J49"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
+      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.18359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.19140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.7"/>
@@ -28097,16 +28113,16 @@
       <c r="I1" s="13"/>
       <c r="J1" s="13"/>
     </row>
-    <row r="2" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="str">
-        <f aca="false">CONCATENATE("lamd:clas_",B2)</f>
-        <v>lamd:clas_REF</v>
+        <f aca="false">CONCATENATE("lamd:class_",B2)</f>
+        <v>lamd:class_REF</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>780</v>
       </c>
       <c r="C2" s="2" t="str">
-        <f aca="false">IF(NOT(ISBLANK(D2)),CONCATENATE("lamd:clas_",D2),""  )</f>
+        <f aca="false">IF(NOT(ISBLANK(D2)),CONCATENATE("lamd:class_",D2),""  )</f>
         <v/>
       </c>
       <c r="E2" s="2" t="n">
@@ -28119,17 +28135,17 @@
         <v>781</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="str">
-        <f aca="false">CONCATENATE("lamd:clas_",B3)</f>
-        <v>lamd:clas_CLX</v>
+        <f aca="false">CONCATENATE("lamd:class_",B3)</f>
+        <v>lamd:class_CLX</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>782</v>
       </c>
-      <c r="C3" s="0" t="str">
-        <f aca="false">IF(NOT(ISBLANK(D3)),CONCATENATE("lamd:clas_",D3),""  )</f>
-        <v>lamd:clas_REF</v>
+      <c r="C3" s="2" t="str">
+        <f aca="false">IF(NOT(ISBLANK(D3)),CONCATENATE("lamd:class_",D3),""  )</f>
+        <v>lamd:class_REF</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>780</v>
@@ -28141,17 +28157,17 @@
         <v>95</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="str">
-        <f aca="false">CONCATENATE("lamd:clas_",B4)</f>
-        <v>lamd:clas_OTHER_REF</v>
+        <f aca="false">CONCATENATE("lamd:class_",B4)</f>
+        <v>lamd:class_OTHER_REF</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>783</v>
       </c>
-      <c r="C4" s="0" t="str">
-        <f aca="false">IF(NOT(ISBLANK(D4)),CONCATENATE("lamd:clas_",D4),""  )</f>
-        <v>lamd:clas_REF</v>
+      <c r="C4" s="2" t="str">
+        <f aca="false">IF(NOT(ISBLANK(D4)),CONCATENATE("lamd:class_",D4),""  )</f>
+        <v>lamd:class_REF</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>780</v>
@@ -28163,16 +28179,16 @@
         <v>784</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="str">
-        <f aca="false">CONCATENATE("lamd:clas_",B5)</f>
-        <v>lamd:clas_DATE</v>
+        <f aca="false">CONCATENATE("lamd:class_",B5)</f>
+        <v>lamd:class_DATE</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>785</v>
       </c>
-      <c r="C5" s="0" t="str">
-        <f aca="false">IF(NOT(ISBLANK(D5)),CONCATENATE("lamd:clas_",D5),""  )</f>
+      <c r="C5" s="2" t="str">
+        <f aca="false">IF(NOT(ISBLANK(D5)),CONCATENATE("lamd:class_",D5),""  )</f>
         <v/>
       </c>
       <c r="E5" s="0" t="n">
@@ -28185,17 +28201,17 @@
         <v>786</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="str">
-        <f aca="false">CONCATENATE("lamd:clas_",B6)</f>
-        <v>lamd:clas_DPROP</v>
+        <f aca="false">CONCATENATE("lamd:class_",B6)</f>
+        <v>lamd:class_DPROP</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>787</v>
       </c>
-      <c r="C6" s="0" t="str">
-        <f aca="false">IF(NOT(ISBLANK(D6)),CONCATENATE("lamd:clas_",D6),""  )</f>
-        <v>lamd:clas_DATE</v>
+      <c r="C6" s="2" t="str">
+        <f aca="false">IF(NOT(ISBLANK(D6)),CONCATENATE("lamd:class_",D6),""  )</f>
+        <v>lamd:class_DATE</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>785</v>
@@ -28207,17 +28223,17 @@
         <v>788</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="str">
-        <f aca="false">CONCATENATE("lamd:clas_",B7)</f>
-        <v>lamd:clas_DANNOT</v>
+        <f aca="false">CONCATENATE("lamd:class_",B7)</f>
+        <v>lamd:class_DANNOT</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>789</v>
       </c>
-      <c r="C7" s="0" t="str">
-        <f aca="false">IF(NOT(ISBLANK(D7)),CONCATENATE("lamd:clas_",D7),""  )</f>
-        <v>lamd:clas_DATE</v>
+      <c r="C7" s="2" t="str">
+        <f aca="false">IF(NOT(ISBLANK(D7)),CONCATENATE("lamd:class_",D7),""  )</f>
+        <v>lamd:class_DATE</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>785</v>
@@ -28229,16 +28245,16 @@
         <v>790</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="str">
-        <f aca="false">CONCATENATE("lamd:clas_",B8)</f>
-        <v>lamd:clas_CLAS</v>
+        <f aca="false">CONCATENATE("lamd:class_",B8)</f>
+        <v>lamd:class_CLAS</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>791</v>
       </c>
-      <c r="C8" s="0" t="str">
-        <f aca="false">IF(NOT(ISBLANK(D8)),CONCATENATE("lamd:clas_",D8),""  )</f>
+      <c r="C8" s="2" t="str">
+        <f aca="false">IF(NOT(ISBLANK(D8)),CONCATENATE("lamd:class_",D8),""  )</f>
         <v/>
       </c>
       <c r="E8" s="0" t="n">
@@ -28251,16 +28267,16 @@
         <v>793</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="str">
-        <f aca="false">CONCATENATE("lamd:clas_",B9)</f>
-        <v>lamd:clas_ESI</v>
+        <f aca="false">CONCATENATE("lamd:class_",B9)</f>
+        <v>lamd:class_ESI</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>794</v>
       </c>
-      <c r="C9" s="0" t="str">
-        <f aca="false">IF(NOT(ISBLANK(D9)),CONCATENATE("lamd:clas_",D9),""  )</f>
+      <c r="C9" s="2" t="str">
+        <f aca="false">IF(NOT(ISBLANK(D9)),CONCATENATE("lamd:class_",D9),""  )</f>
         <v/>
       </c>
       <c r="E9" s="0" t="n">
@@ -28273,17 +28289,17 @@
         <v>796</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="300" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="225.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="str">
-        <f aca="false">CONCATENATE("lamd:clas_",B10)</f>
-        <v>lamd:clas_RBD</v>
+        <f aca="false">CONCATENATE("lamd:class_",B10)</f>
+        <v>lamd:class_RBD</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>797</v>
       </c>
-      <c r="C10" s="0" t="str">
-        <f aca="false">IF(NOT(ISBLANK(D10)),CONCATENATE("lamd:clas_",D10),""  )</f>
-        <v>lamd:clas_RBD</v>
+      <c r="C10" s="2" t="str">
+        <f aca="false">IF(NOT(ISBLANK(D10)),CONCATENATE("lamd:class_",D10),""  )</f>
+        <v>lamd:class_RBD</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>797</v>
@@ -28298,17 +28314,17 @@
         <v>799</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="str">
-        <f aca="false">CONCATENATE("lamd:clas_",B11)</f>
-        <v>lamd:clas_MSEA</v>
+        <f aca="false">CONCATENATE("lamd:class_",B11)</f>
+        <v>lamd:class_MSEA</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>800</v>
       </c>
-      <c r="C11" s="0" t="str">
-        <f aca="false">IF(NOT(ISBLANK(D11)),CONCATENATE("lamd:clas_",D11),""  )</f>
-        <v>lamd:clas_RBD</v>
+      <c r="C11" s="2" t="str">
+        <f aca="false">IF(NOT(ISBLANK(D11)),CONCATENATE("lamd:class_",D11),""  )</f>
+        <v>lamd:class_RBD</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>797</v>
@@ -28320,17 +28336,17 @@
         <v>801</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="str">
-        <f aca="false">CONCATENATE("lamd:clas_",B12)</f>
-        <v>lamd:clas_RD</v>
+        <f aca="false">CONCATENATE("lamd:class_",B12)</f>
+        <v>lamd:class_RD</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>802</v>
       </c>
-      <c r="C12" s="0" t="str">
-        <f aca="false">IF(NOT(ISBLANK(D12)),CONCATENATE("lamd:clas_",D12),""  )</f>
-        <v>lamd:clas_RBD</v>
+      <c r="C12" s="2" t="str">
+        <f aca="false">IF(NOT(ISBLANK(D12)),CONCATENATE("lamd:class_",D12),""  )</f>
+        <v>lamd:class_RBD</v>
       </c>
       <c r="D12" s="0" t="s">
         <v>797</v>
@@ -28342,17 +28358,17 @@
         <v>590</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="str">
-        <f aca="false">CONCATENATE("lamd:clas_",B13)</f>
-        <v>lamd:clas_AJ</v>
+        <f aca="false">CONCATENATE("lamd:class_",B13)</f>
+        <v>lamd:class_AJ</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>803</v>
       </c>
-      <c r="C13" s="0" t="str">
-        <f aca="false">IF(NOT(ISBLANK(D13)),CONCATENATE("lamd:clas_",D13),""  )</f>
-        <v>lamd:clas_RBD</v>
+      <c r="C13" s="2" t="str">
+        <f aca="false">IF(NOT(ISBLANK(D13)),CONCATENATE("lamd:class_",D13),""  )</f>
+        <v>lamd:class_RBD</v>
       </c>
       <c r="D13" s="0" t="s">
         <v>797</v>
@@ -28364,17 +28380,17 @@
         <v>635</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="str">
-        <f aca="false">CONCATENATE("lamd:clas_",B14)</f>
-        <v>lamd:clas_RANNOT</v>
+        <f aca="false">CONCATENATE("lamd:class_",B14)</f>
+        <v>lamd:class_RANNOT</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>804</v>
       </c>
-      <c r="C14" s="0" t="str">
-        <f aca="false">IF(NOT(ISBLANK(D14)),CONCATENATE("lamd:clas_",D14),""  )</f>
-        <v>lamd:clas_RBD</v>
+      <c r="C14" s="2" t="str">
+        <f aca="false">IF(NOT(ISBLANK(D14)),CONCATENATE("lamd:class_",D14),""  )</f>
+        <v>lamd:class_RBD</v>
       </c>
       <c r="D14" s="0" t="s">
         <v>797</v>
@@ -28386,16 +28402,16 @@
         <v>805</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="str">
-        <f aca="false">CONCATENATE("lamd:clas_",B15)</f>
-        <v>lamd:clas_MIS</v>
+        <f aca="false">CONCATENATE("lamd:class_",B15)</f>
+        <v>lamd:class_MIS</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>806</v>
       </c>
-      <c r="C15" s="0" t="str">
-        <f aca="false">IF(NOT(ISBLANK(D15)),CONCATENATE("lamd:clas_",D15),""  )</f>
+      <c r="C15" s="2" t="str">
+        <f aca="false">IF(NOT(ISBLANK(D15)),CONCATENATE("lamd:class_",D15),""  )</f>
         <v/>
       </c>
       <c r="E15" s="0" t="n">
@@ -28408,16 +28424,16 @@
         <v>807</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="str">
-        <f aca="false">CONCATENATE("lamd:clas_",B16)</f>
-        <v>lamd:clas_CDJ</v>
+        <f aca="false">CONCATENATE("lamd:class_",B16)</f>
+        <v>lamd:class_CDJ</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>808</v>
       </c>
-      <c r="C16" s="0" t="str">
-        <f aca="false">IF(NOT(ISBLANK(D16)),CONCATENATE("lamd:clas_",D16),""  )</f>
+      <c r="C16" s="2" t="str">
+        <f aca="false">IF(NOT(ISBLANK(D16)),CONCATENATE("lamd:class_",D16),""  )</f>
         <v/>
       </c>
       <c r="E16" s="0" t="n">
@@ -28430,16 +28446,16 @@
         <v>810</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="str">
-        <f aca="false">CONCATENATE("lamd:clas_",B17)</f>
-        <v>lamd:clas_EDIT</v>
+        <f aca="false">CONCATENATE("lamd:class_",B17)</f>
+        <v>lamd:class_EDIT</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>811</v>
       </c>
-      <c r="C17" s="0" t="str">
-        <f aca="false">IF(NOT(ISBLANK(D17)),CONCATENATE("lamd:clas_",D17),""  )</f>
+      <c r="C17" s="2" t="str">
+        <f aca="false">IF(NOT(ISBLANK(D17)),CONCATENATE("lamd:class_",D17),""  )</f>
         <v/>
       </c>
       <c r="E17" s="0" t="n">
@@ -28568,9 +28584,9 @@
   <dimension ref="A1:CX52"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="CW3" activeCellId="0" sqref="CW3"/>
+      <selection pane="bottomLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="1"/>
@@ -28978,7 +28994,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="180.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="23" t="s">
         <v>821</v>
       </c>
@@ -29113,11 +29129,11 @@
         <v>840</v>
       </c>
       <c r="CX2" s="23" t="str">
-        <f aca="false">IF(NOT(ISBLANK(CW2)),CONCATENATE("lamd:clc_",CW2),CONCATENATE("lamd:clc_",CV2)  )</f>
-        <v>lamd:clc_COM</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="180.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">IF(NOT(ISBLANK(CW2)),CONCATENATE("lamd:class_",CW2),CONCATENATE("lamd:class_",CV2)  )</f>
+        <v>lamd:class_COM</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="23" t="s">
         <v>841</v>
       </c>
@@ -29252,11 +29268,11 @@
         <v>840</v>
       </c>
       <c r="CX3" s="23" t="str">
-        <f aca="false">IF(NOT(ISBLANK(CW3)),CONCATENATE("lamd:clc_",CW3),CONCATENATE("lamd:clc_",CV3)  )</f>
-        <v>lamd:clc_COM</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="180.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">IF(NOT(ISBLANK(CW3)),CONCATENATE("lamd:class_",CW3),CONCATENATE("lamd:class_",CV3)  )</f>
+        <v>lamd:class_COM</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="23" t="s">
         <v>847</v>
       </c>
@@ -29391,11 +29407,11 @@
         <v>840</v>
       </c>
       <c r="CX4" s="23" t="str">
-        <f aca="false">IF(NOT(ISBLANK(CW4)),CONCATENATE("lamd:clc_",CW4),CONCATENATE("lamd:clc_",CV4)  )</f>
-        <v>lamd:clc_COM</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="180.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">IF(NOT(ISBLANK(CW4)),CONCATENATE("lamd:class_",CW4),CONCATENATE("lamd:class_",CV4)  )</f>
+        <v>lamd:class_COM</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="23" t="s">
         <v>855</v>
       </c>
@@ -29531,8 +29547,8 @@
         <v>840</v>
       </c>
       <c r="CX5" s="23" t="str">
-        <f aca="false">IF(NOT(ISBLANK(CW5)),CONCATENATE("lamd:clc_",CW5),CONCATENATE("lamd:clc_",CV5)  )</f>
-        <v>lamd:clc_COM</v>
+        <f aca="false">IF(NOT(ISBLANK(CW5)),CONCATENATE("lamd:class_",CW5),CONCATENATE("lamd:class_",CV5)  )</f>
+        <v>lamd:class_COM</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29650,11 +29666,11 @@
         <v>874</v>
       </c>
       <c r="CX6" s="23" t="str">
-        <f aca="false">IF(NOT(ISBLANK(CW6)),CONCATENATE("lamd:clc_",CW6),CONCATENATE("lamd:clc_",CV6)  )</f>
-        <v>lamd:clc_EESC</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="248.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">IF(NOT(ISBLANK(CW6)),CONCATENATE("lamd:class_",CW6),CONCATENATE("lamd:class_",CV6)  )</f>
+        <v>lamd:class_EESC</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="247.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="23" t="s">
         <v>875</v>
       </c>
@@ -29778,8 +29794,8 @@
         <v>874</v>
       </c>
       <c r="CX7" s="23" t="str">
-        <f aca="false">IF(NOT(ISBLANK(CW7)),CONCATENATE("lamd:clc_",CW7),CONCATENATE("lamd:clc_",CV7)  )</f>
-        <v>lamd:clc_EESC</v>
+        <f aca="false">IF(NOT(ISBLANK(CW7)),CONCATENATE("lamd:class_",CW7),CONCATENATE("lamd:class_",CV7)  )</f>
+        <v>lamd:class_EESC</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29903,8 +29919,8 @@
         <v>874</v>
       </c>
       <c r="CX8" s="23" t="str">
-        <f aca="false">IF(NOT(ISBLANK(CW8)),CONCATENATE("lamd:clc_",CW8),CONCATENATE("lamd:clc_",CV8)  )</f>
-        <v>lamd:clc_EESC</v>
+        <f aca="false">IF(NOT(ISBLANK(CW8)),CONCATENATE("lamd:class_",CW8),CONCATENATE("lamd:class_",CV8)  )</f>
+        <v>lamd:class_EESC</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30022,8 +30038,8 @@
         <v>874</v>
       </c>
       <c r="CX9" s="23" t="str">
-        <f aca="false">IF(NOT(ISBLANK(CW9)),CONCATENATE("lamd:clc_",CW9),CONCATENATE("lamd:clc_",CV9)  )</f>
-        <v>lamd:clc_EESC</v>
+        <f aca="false">IF(NOT(ISBLANK(CW9)),CONCATENATE("lamd:class_",CW9),CONCATENATE("lamd:class_",CV9)  )</f>
+        <v>lamd:class_EESC</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30141,11 +30157,11 @@
         <v>874</v>
       </c>
       <c r="CX10" s="23" t="str">
-        <f aca="false">IF(NOT(ISBLANK(CW10)),CONCATENATE("lamd:clc_",CW10),CONCATENATE("lamd:clc_",CV10)  )</f>
-        <v>lamd:clc_EESC</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="91.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">IF(NOT(ISBLANK(CW10)),CONCATENATE("lamd:class_",CW10),CONCATENATE("lamd:class_",CV10)  )</f>
+        <v>lamd:class_EESC</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="23" t="s">
         <v>904</v>
       </c>
@@ -30230,11 +30246,11 @@
         <v>914</v>
       </c>
       <c r="CX11" s="23" t="str">
-        <f aca="false">IF(NOT(ISBLANK(CW11)),CONCATENATE("lamd:clc_",CW11),CONCATENATE("lamd:clc_",CV11)  )</f>
-        <v>lamd:clc_CONSIL</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="203.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">IF(NOT(ISBLANK(CW11)),CONCATENATE("lamd:class_",CW11),CONCATENATE("lamd:class_",CV11)  )</f>
+        <v>lamd:class_CONSIL</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="23" t="s">
         <v>915</v>
       </c>
@@ -30343,11 +30359,11 @@
         <v>840</v>
       </c>
       <c r="CX12" s="23" t="str">
-        <f aca="false">IF(NOT(ISBLANK(CW12)),CONCATENATE("lamd:clc_",CW12),CONCATENATE("lamd:clc_",CV12)  )</f>
-        <v>lamd:clc_COM</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="203.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">IF(NOT(ISBLANK(CW12)),CONCATENATE("lamd:class_",CW12),CONCATENATE("lamd:class_",CV12)  )</f>
+        <v>lamd:class_COM</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="23" t="s">
         <v>928</v>
       </c>
@@ -30453,11 +30469,11 @@
         <v>840</v>
       </c>
       <c r="CX13" s="23" t="str">
-        <f aca="false">IF(NOT(ISBLANK(CW13)),CONCATENATE("lamd:clc_",CW13),CONCATENATE("lamd:clc_",CV13)  )</f>
-        <v>lamd:clc_COM</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="203.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">IF(NOT(ISBLANK(CW13)),CONCATENATE("lamd:class_",CW13),CONCATENATE("lamd:class_",CV13)  )</f>
+        <v>lamd:class_COM</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="23" t="s">
         <v>934</v>
       </c>
@@ -30570,11 +30586,11 @@
         <v>840</v>
       </c>
       <c r="CX14" s="23" t="str">
-        <f aca="false">IF(NOT(ISBLANK(CW14)),CONCATENATE("lamd:clc_",CW14),CONCATENATE("lamd:clc_",CV14)  )</f>
-        <v>lamd:clc_COM</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="203.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">IF(NOT(ISBLANK(CW14)),CONCATENATE("lamd:class_",CW14),CONCATENATE("lamd:class_",CV14)  )</f>
+        <v>lamd:class_COM</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="23" t="s">
         <v>941</v>
       </c>
@@ -30677,11 +30693,11 @@
         <v>884</v>
       </c>
       <c r="CX15" s="23" t="str">
-        <f aca="false">IF(NOT(ISBLANK(CW15)),CONCATENATE("lamd:clc_",CW15),CONCATENATE("lamd:clc_",CV15)  )</f>
-        <v>lamd:clc_</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="203.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">IF(NOT(ISBLANK(CW15)),CONCATENATE("lamd:class_",CW15),CONCATENATE("lamd:class_",CV15)  )</f>
+        <v>lamd:class_</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="23" t="s">
         <v>949</v>
       </c>
@@ -30787,11 +30803,11 @@
         <v>840</v>
       </c>
       <c r="CX16" s="23" t="str">
-        <f aca="false">IF(NOT(ISBLANK(CW16)),CONCATENATE("lamd:clc_",CW16),CONCATENATE("lamd:clc_",CV16)  )</f>
-        <v>lamd:clc_COM</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="203.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">IF(NOT(ISBLANK(CW16)),CONCATENATE("lamd:class_",CW16),CONCATENATE("lamd:class_",CV16)  )</f>
+        <v>lamd:class_COM</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="23" t="s">
         <v>955</v>
       </c>
@@ -30904,11 +30920,11 @@
         <v>840</v>
       </c>
       <c r="CX17" s="23" t="str">
-        <f aca="false">IF(NOT(ISBLANK(CW17)),CONCATENATE("lamd:clc_",CW17),CONCATENATE("lamd:clc_",CV17)  )</f>
-        <v>lamd:clc_COM</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="91.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">IF(NOT(ISBLANK(CW17)),CONCATENATE("lamd:class_",CW17),CONCATENATE("lamd:class_",CV17)  )</f>
+        <v>lamd:class_COM</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="23" t="s">
         <v>962</v>
       </c>
@@ -30990,11 +31006,11 @@
         <v>973</v>
       </c>
       <c r="CX18" s="23" t="str">
-        <f aca="false">IF(NOT(ISBLANK(CW18)),CONCATENATE("lamd:clc_",CW18),CONCATENATE("lamd:clc_",CV18)  )</f>
-        <v>lamd:clc_CASE</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="91.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">IF(NOT(ISBLANK(CW18)),CONCATENATE("lamd:class_",CW18),CONCATENATE("lamd:class_",CV18)  )</f>
+        <v>lamd:class_CASE</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="23" t="s">
         <v>974</v>
       </c>
@@ -31076,11 +31092,11 @@
         <v>973</v>
       </c>
       <c r="CX19" s="23" t="str">
-        <f aca="false">IF(NOT(ISBLANK(CW19)),CONCATENATE("lamd:clc_",CW19),CONCATENATE("lamd:clc_",CV19)  )</f>
-        <v>lamd:clc_CASE</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">IF(NOT(ISBLANK(CW19)),CONCATENATE("lamd:class_",CW19),CONCATENATE("lamd:class_",CV19)  )</f>
+        <v>lamd:class_CASE</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="23" t="s">
         <v>981</v>
       </c>
@@ -31234,11 +31250,11 @@
         <v>996</v>
       </c>
       <c r="CX20" s="23" t="str">
-        <f aca="false">IF(NOT(ISBLANK(CW20)),CONCATENATE("lamd:clc_",CW20),CONCATENATE("lamd:clc_",CV20)  )</f>
-        <v>lamd:clc_AGREE</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">IF(NOT(ISBLANK(CW20)),CONCATENATE("lamd:class_",CW20),CONCATENATE("lamd:class_",CV20)  )</f>
+        <v>lamd:class_AGREE</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="23" t="s">
         <v>997</v>
       </c>
@@ -31317,11 +31333,11 @@
         <v>840</v>
       </c>
       <c r="CX21" s="23" t="str">
-        <f aca="false">IF(NOT(ISBLANK(CW21)),CONCATENATE("lamd:clc_",CW21),CONCATENATE("lamd:clc_",CV21)  )</f>
-        <v>lamd:clc_COM</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="69.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">IF(NOT(ISBLANK(CW21)),CONCATENATE("lamd:class_",CW21),CONCATENATE("lamd:class_",CV21)  )</f>
+        <v>lamd:class_COM</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="27" t="s">
         <v>1009</v>
       </c>
@@ -31474,11 +31490,11 @@
         <v>1023</v>
       </c>
       <c r="CX22" s="23" t="str">
-        <f aca="false">IF(NOT(ISBLANK(CW22)),CONCATENATE("lamd:clc_",CW22),CONCATENATE("lamd:clc_",CV22)  )</f>
-        <v>lamd:clc_STATEAID</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="57.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">IF(NOT(ISBLANK(CW22)),CONCATENATE("lamd:class_",CW22),CONCATENATE("lamd:class_",CV22)  )</f>
+        <v>lamd:class_STATEAID</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="27" t="s">
         <v>1024</v>
       </c>
@@ -31627,11 +31643,11 @@
         <v>1037</v>
       </c>
       <c r="CX23" s="23" t="str">
-        <f aca="false">IF(NOT(ISBLANK(CW23)),CONCATENATE("lamd:clc_",CW23),CONCATENATE("lamd:clc_",CV23)  )</f>
-        <v>lamd:clc_EFTA</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="69.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">IF(NOT(ISBLANK(CW23)),CONCATENATE("lamd:class_",CW23),CONCATENATE("lamd:class_",CV23)  )</f>
+        <v>lamd:class_EFTA</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="27" t="s">
         <v>1038</v>
       </c>
@@ -31781,11 +31797,11 @@
         <v>1037</v>
       </c>
       <c r="CX24" s="23" t="str">
-        <f aca="false">IF(NOT(ISBLANK(CW24)),CONCATENATE("lamd:clc_",CW24),CONCATENATE("lamd:clc_",CV24)  )</f>
-        <v>lamd:clc_EFTA</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="69.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">IF(NOT(ISBLANK(CW24)),CONCATENATE("lamd:class_",CW24),CONCATENATE("lamd:class_",CV24)  )</f>
+        <v>lamd:class_EFTA</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="27" t="s">
         <v>1045</v>
       </c>
@@ -31964,11 +31980,11 @@
         <v>1037</v>
       </c>
       <c r="CX25" s="23" t="str">
-        <f aca="false">IF(NOT(ISBLANK(CW25)),CONCATENATE("lamd:clc_",CW25),CONCATENATE("lamd:clc_",CV25)  )</f>
-        <v>lamd:clc_EFTA</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="57.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">IF(NOT(ISBLANK(CW25)),CONCATENATE("lamd:class_",CW25),CONCATENATE("lamd:class_",CV25)  )</f>
+        <v>lamd:class_EFTA</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="27" t="s">
         <v>1056</v>
       </c>
@@ -32116,8 +32132,8 @@
         <v>1037</v>
       </c>
       <c r="CX26" s="23" t="str">
-        <f aca="false">IF(NOT(ISBLANK(CW26)),CONCATENATE("lamd:clc_",CW26),CONCATENATE("lamd:clc_",CV26)  )</f>
-        <v>lamd:clc_EFTA</v>
+        <f aca="false">IF(NOT(ISBLANK(CW26)),CONCATENATE("lamd:class_",CW26),CONCATENATE("lamd:class_",CV26)  )</f>
+        <v>lamd:class_EFTA</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="76.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -32270,8 +32286,8 @@
         <v>1037</v>
       </c>
       <c r="CX27" s="23" t="str">
-        <f aca="false">IF(NOT(ISBLANK(CW27)),CONCATENATE("lamd:clc_",CW27),CONCATENATE("lamd:clc_",CV27)  )</f>
-        <v>lamd:clc_EFTA</v>
+        <f aca="false">IF(NOT(ISBLANK(CW27)),CONCATENATE("lamd:class_",CW27),CONCATENATE("lamd:class_",CV27)  )</f>
+        <v>lamd:class_EFTA</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32435,11 +32451,11 @@
         <v>1037</v>
       </c>
       <c r="CX28" s="23" t="str">
-        <f aca="false">IF(NOT(ISBLANK(CW28)),CONCATENATE("lamd:clc_",CW28),CONCATENATE("lamd:clc_",CV28)  )</f>
-        <v>lamd:clc_EFTA</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">IF(NOT(ISBLANK(CW28)),CONCATENATE("lamd:class_",CW28),CONCATENATE("lamd:class_",CV28)  )</f>
+        <v>lamd:class_EFTA</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="27" t="s">
         <v>1085</v>
       </c>
@@ -32591,11 +32607,11 @@
         <v>1037</v>
       </c>
       <c r="CX29" s="23" t="str">
-        <f aca="false">IF(NOT(ISBLANK(CW29)),CONCATENATE("lamd:clc_",CW29),CONCATENATE("lamd:clc_",CV29)  )</f>
-        <v>lamd:clc_EFTA</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="124.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">IF(NOT(ISBLANK(CW29)),CONCATENATE("lamd:class_",CW29),CONCATENATE("lamd:class_",CV29)  )</f>
+        <v>lamd:class_EFTA</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="27" t="s">
         <v>1094</v>
       </c>
@@ -32746,11 +32762,11 @@
         <v>1037</v>
       </c>
       <c r="CX30" s="23" t="str">
-        <f aca="false">IF(NOT(ISBLANK(CW30)),CONCATENATE("lamd:clc_",CW30),CONCATENATE("lamd:clc_",CV30)  )</f>
-        <v>lamd:clc_EFTA</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="69.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">IF(NOT(ISBLANK(CW30)),CONCATENATE("lamd:class_",CW30),CONCATENATE("lamd:class_",CV30)  )</f>
+        <v>lamd:class_EFTA</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="27" t="s">
         <v>1105</v>
       </c>
@@ -32909,11 +32925,11 @@
         <v>1118</v>
       </c>
       <c r="CX31" s="23" t="str">
-        <f aca="false">IF(NOT(ISBLANK(CW31)),CONCATENATE("lamd:clc_",CW31),CONCATENATE("lamd:clc_",CV31)  )</f>
-        <v>lamd:clc_COTHER</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="35.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">IF(NOT(ISBLANK(CW31)),CONCATENATE("lamd:class_",CW31),CONCATENATE("lamd:class_",CV31)  )</f>
+        <v>lamd:class_COTHER</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="27" t="s">
         <v>1119</v>
       </c>
@@ -33066,11 +33082,11 @@
         <v>1023</v>
       </c>
       <c r="CX32" s="23" t="str">
-        <f aca="false">IF(NOT(ISBLANK(CW32)),CONCATENATE("lamd:clc_",CW32),CONCATENATE("lamd:clc_",CV32)  )</f>
-        <v>lamd:clc_STATEAID</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="91.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">IF(NOT(ISBLANK(CW32)),CONCATENATE("lamd:class_",CW32),CONCATENATE("lamd:class_",CV32)  )</f>
+        <v>lamd:class_STATEAID</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="27" t="s">
         <v>1131</v>
       </c>
@@ -33230,11 +33246,11 @@
         <v>1148</v>
       </c>
       <c r="CX33" s="23" t="str">
-        <f aca="false">IF(NOT(ISBLANK(CW33)),CONCATENATE("lamd:clc_",CW33),CONCATENATE("lamd:clc_",CV33)  )</f>
-        <v>lamd:clc_3OTHER</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="69.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">IF(NOT(ISBLANK(CW33)),CONCATENATE("lamd:class_",CW33),CONCATENATE("lamd:class_",CV33)  )</f>
+        <v>lamd:class_3OTHER</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="27" t="s">
         <v>1149</v>
       </c>
@@ -33405,11 +33421,11 @@
         <v>914</v>
       </c>
       <c r="CX34" s="23" t="str">
-        <f aca="false">IF(NOT(ISBLANK(CW34)),CONCATENATE("lamd:clc_",CW34),CONCATENATE("lamd:clc_",CV34)  )</f>
-        <v>lamd:clc_CONSIL</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="57.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">IF(NOT(ISBLANK(CW34)),CONCATENATE("lamd:class_",CW34),CONCATENATE("lamd:class_",CV34)  )</f>
+        <v>lamd:class_CONSIL</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="27" t="s">
         <v>1159</v>
       </c>
@@ -33580,11 +33596,11 @@
         <v>914</v>
       </c>
       <c r="CX35" s="23" t="str">
-        <f aca="false">IF(NOT(ISBLANK(CW35)),CONCATENATE("lamd:clc_",CW35),CONCATENATE("lamd:clc_",CV35)  )</f>
-        <v>lamd:clc_CONSIL</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="35.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">IF(NOT(ISBLANK(CW35)),CONCATENATE("lamd:class_",CW35),CONCATENATE("lamd:class_",CV35)  )</f>
+        <v>lamd:class_CONSIL</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="27" t="s">
         <v>1165</v>
       </c>
@@ -33755,11 +33771,11 @@
         <v>1176</v>
       </c>
       <c r="CX36" s="23" t="str">
-        <f aca="false">IF(NOT(ISBLANK(CW36)),CONCATENATE("lamd:clc_",CW36),CONCATENATE("lamd:clc_",CV36)  )</f>
-        <v>lamd:clc_5OTHER</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="57.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">IF(NOT(ISBLANK(CW36)),CONCATENATE("lamd:class_",CW36),CONCATENATE("lamd:class_",CV36)  )</f>
+        <v>lamd:class_5OTHER</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="27" t="s">
         <v>1177</v>
       </c>
@@ -33924,11 +33940,11 @@
         <v>1037</v>
       </c>
       <c r="CX37" s="23" t="str">
-        <f aca="false">IF(NOT(ISBLANK(CW37)),CONCATENATE("lamd:clc_",CW37),CONCATENATE("lamd:clc_",CV37)  )</f>
-        <v>lamd:clc_EFTA</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="69.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">IF(NOT(ISBLANK(CW37)),CONCATENATE("lamd:class_",CW37),CONCATENATE("lamd:class_",CV37)  )</f>
+        <v>lamd:class_EFTA</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="27" t="s">
         <v>1189</v>
       </c>
@@ -34083,11 +34099,11 @@
         <v>1023</v>
       </c>
       <c r="CX38" s="23" t="str">
-        <f aca="false">IF(NOT(ISBLANK(CW38)),CONCATENATE("lamd:clc_",CW38),CONCATENATE("lamd:clc_",CV38)  )</f>
-        <v>lamd:clc_STATEAID</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="57.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">IF(NOT(ISBLANK(CW38)),CONCATENATE("lamd:class_",CW38),CONCATENATE("lamd:class_",CV38)  )</f>
+        <v>lamd:class_STATEAID</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="27" t="s">
         <v>1198</v>
       </c>
@@ -34265,11 +34281,11 @@
         <v>1208</v>
       </c>
       <c r="CX39" s="23" t="str">
-        <f aca="false">IF(NOT(ISBLANK(CW39)),CONCATENATE("lamd:clc_",CW39),CONCATENATE("lamd:clc_",CV39)  )</f>
-        <v>lamd:clc_CRDS</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="136.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">IF(NOT(ISBLANK(CW39)),CONCATENATE("lamd:class_",CW39),CONCATENATE("lamd:class_",CV39)  )</f>
+        <v>lamd:class_CRDS</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="27" t="s">
         <v>1209</v>
       </c>
@@ -34446,11 +34462,11 @@
         <v>1208</v>
       </c>
       <c r="CX40" s="23" t="str">
-        <f aca="false">IF(NOT(ISBLANK(CW40)),CONCATENATE("lamd:clc_",CW40),CONCATENATE("lamd:clc_",CV40)  )</f>
-        <v>lamd:clc_CRDS</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="91.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">IF(NOT(ISBLANK(CW40)),CONCATENATE("lamd:class_",CW40),CONCATENATE("lamd:class_",CV40)  )</f>
+        <v>lamd:class_CRDS</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="27" t="s">
         <v>1217</v>
       </c>
@@ -34628,11 +34644,11 @@
         <v>1208</v>
       </c>
       <c r="CX41" s="23" t="str">
-        <f aca="false">IF(NOT(ISBLANK(CW41)),CONCATENATE("lamd:clc_",CW41),CONCATENATE("lamd:clc_",CV41)  )</f>
-        <v>lamd:clc_CRDS</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="69.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">IF(NOT(ISBLANK(CW41)),CONCATENATE("lamd:class_",CW41),CONCATENATE("lamd:class_",CV41)  )</f>
+        <v>lamd:class_CRDS</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="27" t="s">
         <v>1223</v>
       </c>
@@ -34796,11 +34812,11 @@
         <v>1208</v>
       </c>
       <c r="CX42" s="23" t="str">
-        <f aca="false">IF(NOT(ISBLANK(CW42)),CONCATENATE("lamd:clc_",CW42),CONCATENATE("lamd:clc_",CV42)  )</f>
-        <v>lamd:clc_CRDS</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="69.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">IF(NOT(ISBLANK(CW42)),CONCATENATE("lamd:class_",CW42),CONCATENATE("lamd:class_",CV42)  )</f>
+        <v>lamd:class_CRDS</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="27" t="s">
         <v>1232</v>
       </c>
@@ -34961,11 +34977,11 @@
         <v>1208</v>
       </c>
       <c r="CX43" s="23" t="str">
-        <f aca="false">IF(NOT(ISBLANK(CW43)),CONCATENATE("lamd:clc_",CW43),CONCATENATE("lamd:clc_",CV43)  )</f>
-        <v>lamd:clc_CRDS</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="124.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">IF(NOT(ISBLANK(CW43)),CONCATENATE("lamd:class_",CW43),CONCATENATE("lamd:class_",CV43)  )</f>
+        <v>lamd:class_CRDS</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="27" t="s">
         <v>1238</v>
       </c>
@@ -35139,11 +35155,11 @@
         <v>1251</v>
       </c>
       <c r="CX44" s="23" t="str">
-        <f aca="false">IF(NOT(ISBLANK(CW44)),CONCATENATE("lamd:clc_",CW44),CONCATENATE("lamd:clc_",CV44)  )</f>
-        <v>lamd:clc_NLEGIS</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">IF(NOT(ISBLANK(CW44)),CONCATENATE("lamd:class_",CW44),CONCATENATE("lamd:class_",CV44)  )</f>
+        <v>lamd:class_NLEGIS</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="27" t="s">
         <v>1252</v>
       </c>
@@ -35314,11 +35330,11 @@
         <v>1251</v>
       </c>
       <c r="CX45" s="23" t="str">
-        <f aca="false">IF(NOT(ISBLANK(CW45)),CONCATENATE("lamd:clc_",CW45),CONCATENATE("lamd:clc_",CV45)  )</f>
-        <v>lamd:clc_NLEGIS</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="124.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">IF(NOT(ISBLANK(CW45)),CONCATENATE("lamd:class_",CW45),CONCATENATE("lamd:class_",CV45)  )</f>
+        <v>lamd:class_NLEGIS</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="27" t="s">
         <v>1265</v>
       </c>
@@ -35475,8 +35491,8 @@
         <v>1023</v>
       </c>
       <c r="CX46" s="23" t="str">
-        <f aca="false">IF(NOT(ISBLANK(CW46)),CONCATENATE("lamd:clc_",CW46),CONCATENATE("lamd:clc_",CV46)  )</f>
-        <v>lamd:clc_STATEAID</v>
+        <f aca="false">IF(NOT(ISBLANK(CW46)),CONCATENATE("lamd:class_",CW46),CONCATENATE("lamd:class_",CV46)  )</f>
+        <v>lamd:class_STATEAID</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35634,11 +35650,11 @@
         <v>1023</v>
       </c>
       <c r="CX47" s="23" t="str">
-        <f aca="false">IF(NOT(ISBLANK(CW47)),CONCATENATE("lamd:clc_",CW47),CONCATENATE("lamd:clc_",CV47)  )</f>
-        <v>lamd:clc_STATEAID</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">IF(NOT(ISBLANK(CW47)),CONCATENATE("lamd:class_",CW47),CONCATENATE("lamd:class_",CV47)  )</f>
+        <v>lamd:class_STATEAID</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="27" t="s">
         <v>1281</v>
       </c>
@@ -35834,11 +35850,11 @@
         <v>996</v>
       </c>
       <c r="CX48" s="23" t="str">
-        <f aca="false">IF(NOT(ISBLANK(CW48)),CONCATENATE("lamd:clc_",CW48),CONCATENATE("lamd:clc_",CV48)  )</f>
-        <v>lamd:clc_AGREE</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="57.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">IF(NOT(ISBLANK(CW48)),CONCATENATE("lamd:class_",CW48),CONCATENATE("lamd:class_",CV48)  )</f>
+        <v>lamd:class_AGREE</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="27" t="s">
         <v>1292</v>
       </c>
@@ -36037,11 +36053,11 @@
         <v>996</v>
       </c>
       <c r="CX49" s="23" t="str">
-        <f aca="false">IF(NOT(ISBLANK(CW49)),CONCATENATE("lamd:clc_",CW49),CONCATENATE("lamd:clc_",CV49)  )</f>
-        <v>lamd:clc_AGREE</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">IF(NOT(ISBLANK(CW49)),CONCATENATE("lamd:class_",CW49),CONCATENATE("lamd:class_",CV49)  )</f>
+        <v>lamd:class_AGREE</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="27" t="s">
         <v>1301</v>
       </c>
@@ -36240,11 +36256,11 @@
         <v>996</v>
       </c>
       <c r="CX50" s="23" t="str">
-        <f aca="false">IF(NOT(ISBLANK(CW50)),CONCATENATE("lamd:clc_",CW50),CONCATENATE("lamd:clc_",CV50)  )</f>
-        <v>lamd:clc_AGREE</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">IF(NOT(ISBLANK(CW50)),CONCATENATE("lamd:class_",CW50),CONCATENATE("lamd:class_",CV50)  )</f>
+        <v>lamd:class_AGREE</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="27" t="s">
         <v>1308</v>
       </c>
@@ -36397,11 +36413,11 @@
         <v>1318</v>
       </c>
       <c r="CX51" s="23" t="str">
-        <f aca="false">IF(NOT(ISBLANK(CW51)),CONCATENATE("lamd:clc_",CW51),CONCATENATE("lamd:clc_",CV51)  )</f>
-        <v>lamd:clc_MA</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="57.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">IF(NOT(ISBLANK(CW51)),CONCATENATE("lamd:class_",CW51),CONCATENATE("lamd:class_",CV51)  )</f>
+        <v>lamd:class_MA</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="27" t="s">
         <v>1319</v>
       </c>
@@ -36555,8 +36571,8 @@
         <v>1318</v>
       </c>
       <c r="CX52" s="23" t="str">
-        <f aca="false">IF(NOT(ISBLANK(CW52)),CONCATENATE("lamd:clc_",CW52),CONCATENATE("lamd:clc_",CV52)  )</f>
-        <v>lamd:clc_MA</v>
+        <f aca="false">IF(NOT(ISBLANK(CW52)),CONCATENATE("lamd:class_",CW52),CONCATENATE("lamd:class_",CV52)  )</f>
+        <v>lamd:class_MA</v>
       </c>
     </row>
   </sheetData>
@@ -36577,22 +36593,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="18.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="58.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="58.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="18.71"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -36603,438 +36621,525 @@
         <v>769</v>
       </c>
       <c r="D1" s="5" t="s">
+        <v>779</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>772</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>776</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="str">
-        <f aca="false">CONCATENATE("class_classif:clc_",B2)</f>
-        <v>class_classif:clc_TREATY</v>
+        <f aca="false">CONCATENATE("class_classif:class_",B2)</f>
+        <v>class_classif:class_TREATY</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>1326</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5" t="n">
+      <c r="C2" s="28" t="str">
+        <f aca="false">IF(NOT(ISBLANK(D2)),CONCATENATE("class_classif:class_",D2),""  )</f>
+        <v/>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>1327</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>1328</v>
       </c>
-      <c r="G2" s="5"/>
-    </row>
-    <row r="3" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H2" s="5"/>
+    </row>
+    <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="str">
-        <f aca="false">CONCATENATE("class_classif:clc_",B3)</f>
-        <v>class_classif:clc_AGREE</v>
+        <f aca="false">CONCATENATE("class_classif:class_",B3)</f>
+        <v>class_classif:class_AGREE</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>996</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5" t="n">
+      <c r="C3" s="28" t="str">
+        <f aca="false">IF(NOT(ISBLANK(D3)),CONCATENATE("class_classif:class_",D3),""  )</f>
+        <v/>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="F3" s="5" t="s">
         <v>1329</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="G3" s="5" t="s">
         <v>1330</v>
       </c>
-      <c r="G3" s="5"/>
-    </row>
-    <row r="4" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H3" s="5"/>
+    </row>
+    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="str">
-        <f aca="false">CONCATENATE("class_classif:clc_",B4)</f>
-        <v>class_classif:clc_LEGAL</v>
+        <f aca="false">CONCATENATE("class_classif:class_",B4)</f>
+        <v>class_classif:class_LEGAL</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>1147</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5" t="n">
+      <c r="C4" s="28" t="str">
+        <f aca="false">IF(NOT(ISBLANK(D4)),CONCATENATE("class_classif:class_",D4),""  )</f>
+        <v/>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="F4" s="5" t="s">
         <v>1331</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="G4" s="5" t="s">
         <v>1332</v>
       </c>
-      <c r="G4" s="5"/>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H4" s="5"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="str">
-        <f aca="false">CONCATENATE("class_classif:clc_",B5)</f>
-        <v>class_classif:clc_LEGIS</v>
+        <f aca="false">CONCATENATE("class_classif:class_",B5)</f>
+        <v>class_classif:class_LEGIS</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>1333</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="28" t="str">
+        <f aca="false">IF(NOT(ISBLANK(D5)),CONCATENATE("class_classif:class_",D5),""  )</f>
+        <v>class_classif:class_LEGAL</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>1147</v>
       </c>
-      <c r="D5" s="5" t="n">
+      <c r="E5" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>1334</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="G5" s="5" t="s">
         <v>1335</v>
       </c>
-      <c r="G5" s="5"/>
-    </row>
-    <row r="6" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H5" s="5"/>
+    </row>
+    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="str">
-        <f aca="false">CONCATENATE("class_classif:clc_",B6)</f>
-        <v>class_classif:clc_NLEGIS</v>
+        <f aca="false">CONCATENATE("class_classif:class_",B6)</f>
+        <v>class_classif:class_NLEGIS</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>1251</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="28" t="str">
+        <f aca="false">IF(NOT(ISBLANK(D6)),CONCATENATE("class_classif:class_",D6),""  )</f>
+        <v>class_classif:class_LEGAL</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>1147</v>
       </c>
-      <c r="D6" s="5" t="n">
+      <c r="E6" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>1336</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="G6" s="5" t="s">
         <v>1337</v>
       </c>
-      <c r="G6" s="5"/>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="str">
-        <f aca="false">CONCATENATE("class_classif:clc_",B7)</f>
-        <v>class_classif:clc_3OTHER</v>
+        <f aca="false">CONCATENATE("class_classif:class_",B7)</f>
+        <v>class_classif:class_3OTHER</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>1148</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="28" t="str">
+        <f aca="false">IF(NOT(ISBLANK(D7)),CONCATENATE("class_classif:class_",D7),""  )</f>
+        <v>class_classif:class_LEGAL</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>1147</v>
       </c>
-      <c r="D7" s="5" t="n">
+      <c r="E7" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>1338</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="G7" s="5" t="s">
         <v>1339</v>
       </c>
-      <c r="G7" s="5"/>
-    </row>
-    <row r="8" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="str">
-        <f aca="false">CONCATENATE("class_classif:clc_",B8)</f>
-        <v>class_classif:clc_PREPDOC</v>
+        <f aca="false">CONCATENATE("class_classif:class_",B8)</f>
+        <v>class_classif:class_PREPDOC</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>839</v>
       </c>
-      <c r="D8" s="5" t="n">
+      <c r="C8" s="28" t="str">
+        <f aca="false">IF(NOT(ISBLANK(D8)),CONCATENATE("class_classif:class_",D8),""  )</f>
+        <v/>
+      </c>
+      <c r="E8" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="F8" s="0" t="s">
         <v>1340</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="G8" s="5" t="s">
         <v>1341</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="str">
-        <f aca="false">CONCATENATE("class_classif:clc_",B9)</f>
-        <v>class_classif:clc_COM</v>
+        <f aca="false">CONCATENATE("class_classif:class_",B9)</f>
+        <v>class_classif:class_COM</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>840</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="28" t="str">
+        <f aca="false">IF(NOT(ISBLANK(D9)),CONCATENATE("class_classif:class_",D9),""  )</f>
+        <v>class_classif:class_PREPDOC</v>
+      </c>
+      <c r="D9" s="0" t="s">
         <v>839</v>
       </c>
-      <c r="D9" s="5" t="n">
+      <c r="E9" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="E9" s="0" t="s">
+      <c r="F9" s="0" t="s">
         <v>1342</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="G9" s="5" t="s">
         <v>1343</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="str">
-        <f aca="false">CONCATENATE("class_classif:clc_",B10)</f>
-        <v>class_classif:clc_CONSIL</v>
+        <f aca="false">CONCATENATE("class_classif:class_",B10)</f>
+        <v>class_classif:class_CONSIL</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>914</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="28" t="str">
+        <f aca="false">IF(NOT(ISBLANK(D10)),CONCATENATE("class_classif:class_",D10),""  )</f>
+        <v>class_classif:class_PREPDOC</v>
+      </c>
+      <c r="D10" s="0" t="s">
         <v>839</v>
       </c>
-      <c r="D10" s="5" t="n">
+      <c r="E10" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="E10" s="0" t="s">
+      <c r="F10" s="0" t="s">
         <v>1344</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="G10" s="5" t="s">
         <v>1345</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="str">
-        <f aca="false">CONCATENATE("class_classif:clc_",B11)</f>
-        <v>class_classif:clc_EP</v>
+        <f aca="false">CONCATENATE("class_classif:class_",B11)</f>
+        <v>class_classif:class_EP</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>1346</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="28" t="str">
+        <f aca="false">IF(NOT(ISBLANK(D11)),CONCATENATE("class_classif:class_",D11),""  )</f>
+        <v>class_classif:class_PREPDOC</v>
+      </c>
+      <c r="D11" s="0" t="s">
         <v>839</v>
       </c>
-      <c r="D11" s="5" t="n">
+      <c r="E11" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="F11" s="2" t="s">
         <v>1347</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="G11" s="5" t="s">
         <v>1348</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="str">
-        <f aca="false">CONCATENATE("class_classif:clc_",B12)</f>
-        <v>class_classif:clc_EESC</v>
+        <f aca="false">CONCATENATE("class_classif:class_",B12)</f>
+        <v>class_classif:class_EESC</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>874</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" s="28" t="str">
+        <f aca="false">IF(NOT(ISBLANK(D12)),CONCATENATE("class_classif:class_",D12),""  )</f>
+        <v>class_classif:class_PREPDOC</v>
+      </c>
+      <c r="D12" s="0" t="s">
         <v>839</v>
       </c>
-      <c r="D12" s="5" t="n">
+      <c r="E12" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="F12" s="2" t="s">
         <v>1349</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="G12" s="5" t="s">
         <v>1350</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="str">
-        <f aca="false">CONCATENATE("class_classif:clc_",B13)</f>
-        <v>class_classif:clc_COR</v>
+        <f aca="false">CONCATENATE("class_classif:class_",B13)</f>
+        <v>class_classif:class_COR</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>1351</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" s="28" t="str">
+        <f aca="false">IF(NOT(ISBLANK(D13)),CONCATENATE("class_classif:class_",D13),""  )</f>
+        <v>class_classif:class_PREPDOC</v>
+      </c>
+      <c r="D13" s="0" t="s">
         <v>839</v>
       </c>
-      <c r="D13" s="5" t="n">
+      <c r="E13" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="F13" s="2" t="s">
         <v>1352</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="G13" s="5" t="s">
         <v>1353</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="str">
-        <f aca="false">CONCATENATE("class_classif:clc_",B14)</f>
-        <v>class_classif:clc_ECB</v>
+        <f aca="false">CONCATENATE("class_classif:class_",B14)</f>
+        <v>class_classif:class_ECB</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>1354</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C14" s="28" t="str">
+        <f aca="false">IF(NOT(ISBLANK(D14)),CONCATENATE("class_classif:class_",D14),""  )</f>
+        <v>class_classif:class_PREPDOC</v>
+      </c>
+      <c r="D14" s="0" t="s">
         <v>839</v>
       </c>
-      <c r="D14" s="5" t="n">
+      <c r="E14" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="F14" s="2" t="s">
         <v>1355</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="G14" s="5" t="s">
         <v>1356</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="str">
-        <f aca="false">CONCATENATE("class_classif:clc_",B15)</f>
-        <v>class_classif:clc_5OTHER</v>
+        <f aca="false">CONCATENATE("class_classif:class_",B15)</f>
+        <v>class_classif:class_5OTHER</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>1176</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="C15" s="28" t="str">
+        <f aca="false">IF(NOT(ISBLANK(D15)),CONCATENATE("class_classif:class_",D15),""  )</f>
+        <v>class_classif:class_PREPDOC</v>
+      </c>
+      <c r="D15" s="0" t="s">
         <v>839</v>
       </c>
-      <c r="D15" s="5" t="n">
+      <c r="E15" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="F15" s="2" t="s">
         <v>1338</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="G15" s="5" t="s">
         <v>1357</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="str">
-        <f aca="false">CONCATENATE("class_classif:clc_",B16)</f>
-        <v>class_classif:clc_CASE</v>
+        <f aca="false">CONCATENATE("class_classif:class_",B16)</f>
+        <v>class_classif:class_CASE</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>973</v>
       </c>
-      <c r="D16" s="5" t="n">
+      <c r="C16" s="28" t="str">
+        <f aca="false">IF(NOT(ISBLANK(D16)),CONCATENATE("class_classif:class_",D16),""  )</f>
+        <v/>
+      </c>
+      <c r="E16" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="F16" s="2" t="s">
         <v>1358</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="G16" s="5" t="s">
         <v>1359</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="str">
-        <f aca="false">CONCATENATE("class_classif:clc_",B17)</f>
-        <v>class_classif:clc_EFTA</v>
+        <f aca="false">CONCATENATE("class_classif:class_",B17)</f>
+        <v>class_classif:class_EFTA</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>1037</v>
       </c>
-      <c r="D17" s="5" t="n">
+      <c r="C17" s="28" t="str">
+        <f aca="false">IF(NOT(ISBLANK(D17)),CONCATENATE("class_classif:class_",D17),""  )</f>
+        <v/>
+      </c>
+      <c r="E17" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="F17" s="2" t="s">
         <v>1037</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="G17" s="5" t="s">
         <v>1360</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="str">
-        <f aca="false">CONCATENATE("class_classif:clc_",B18)</f>
-        <v>class_classif:clc_CDOC</v>
+        <f aca="false">CONCATENATE("class_classif:class_",B18)</f>
+        <v>class_classif:class_CDOC</v>
       </c>
       <c r="B18" s="0" t="s">
         <v>1022</v>
       </c>
-      <c r="D18" s="5" t="n">
+      <c r="C18" s="28" t="str">
+        <f aca="false">IF(NOT(ISBLANK(D18)),CONCATENATE("class_classif:class_",D18),""  )</f>
+        <v/>
+      </c>
+      <c r="E18" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="F18" s="2" t="s">
         <v>1361</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="G18" s="5" t="s">
         <v>1362</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="str">
-        <f aca="false">CONCATENATE("class_classif:clc_",B19)</f>
-        <v>class_classif:clc_STATEAID</v>
+        <f aca="false">CONCATENATE("class_classif:class_",B19)</f>
+        <v>class_classif:class_STATEAID</v>
       </c>
       <c r="B19" s="0" t="s">
         <v>1023</v>
       </c>
-      <c r="C19" s="0" t="s">
+      <c r="C19" s="28" t="str">
+        <f aca="false">IF(NOT(ISBLANK(D19)),CONCATENATE("class_classif:class_",D19),""  )</f>
+        <v>class_classif:class_CDOC</v>
+      </c>
+      <c r="D19" s="0" t="s">
         <v>1022</v>
       </c>
-      <c r="D19" s="5" t="n">
+      <c r="E19" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="F19" s="2" t="s">
         <v>1363</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="G19" s="5" t="s">
         <v>1364</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="str">
-        <f aca="false">CONCATENATE("class_classif:clc_",B20)</f>
-        <v>class_classif:clc_CRDS</v>
+        <f aca="false">CONCATENATE("class_classif:class_",B20)</f>
+        <v>class_classif:class_CRDS</v>
       </c>
       <c r="B20" s="0" t="s">
         <v>1208</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="C20" s="28" t="str">
+        <f aca="false">IF(NOT(ISBLANK(D20)),CONCATENATE("class_classif:class_",D20),""  )</f>
+        <v>class_classif:class_CDOC</v>
+      </c>
+      <c r="D20" s="0" t="s">
         <v>1022</v>
       </c>
-      <c r="D20" s="5" t="n">
+      <c r="E20" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="F20" s="2" t="s">
         <v>1365</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="str">
-        <f aca="false">CONCATENATE("class_classif:clc_",B21)</f>
-        <v>class_classif:clc_MA</v>
+        <f aca="false">CONCATENATE("class_classif:class_",B21)</f>
+        <v>class_classif:class_MA</v>
       </c>
       <c r="B21" s="0" t="s">
         <v>1318</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="C21" s="28" t="str">
+        <f aca="false">IF(NOT(ISBLANK(D21)),CONCATENATE("class_classif:class_",D21),""  )</f>
+        <v>class_classif:class_CDOC</v>
+      </c>
+      <c r="D21" s="0" t="s">
         <v>1022</v>
       </c>
-      <c r="D21" s="5" t="n">
+      <c r="E21" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="E21" s="5" t="s">
+      <c r="F21" s="5" t="s">
         <v>1366</v>
       </c>
-      <c r="F21" s="5" t="s">
+      <c r="G21" s="5" t="s">
         <v>1367</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="str">
-        <f aca="false">CONCATENATE("class_classif:clc_",B22)</f>
-        <v>class_classif:clc_COTHER</v>
+        <f aca="false">CONCATENATE("class_classif:class_",B22)</f>
+        <v>class_classif:class_COTHER</v>
       </c>
       <c r="B22" s="0" t="s">
         <v>1118</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="C22" s="28" t="str">
+        <f aca="false">IF(NOT(ISBLANK(D22)),CONCATENATE("class_classif:class_",D22),""  )</f>
+        <v>class_classif:class_CDOC</v>
+      </c>
+      <c r="D22" s="0" t="s">
         <v>1022</v>
       </c>
-      <c r="D22" s="5" t="n">
+      <c r="E22" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="F22" s="2" t="s">
         <v>1338</v>
       </c>
     </row>
@@ -37059,7 +37164,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E282" activeCellId="0" sqref="E282"/>
+      <selection pane="bottomLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="1"/>
@@ -37401,7 +37506,7 @@
     <row r="12" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="str">
         <f aca="false">CONCATENATE("celexd:c_",B12)</f>
-        <v>celexd:c_1_/AFI/DCL</v>
+        <v>celexd:c_1_AFI_DCL</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>1382</v>
@@ -37439,7 +37544,7 @@
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="str">
         <f aca="false">CONCATENATE("celexd:c_",B13)</f>
-        <v>celexd:c_1_/PRO</v>
+        <v>celexd:c_1_PRO</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>1387</v>
@@ -37477,7 +37582,7 @@
     <row r="14" customFormat="false" ht="314.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="str">
         <f aca="false">CONCATENATE("celexd:c_",B14)</f>
-        <v>celexd:c_1_/TXT</v>
+        <v>celexd:c_1_TXT</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>1391</v>
@@ -38576,7 +38681,7 @@
       <c r="E41" s="2" t="s">
         <v>1488</v>
       </c>
-      <c r="F41" s="28" t="s">
+      <c r="F41" s="29" t="s">
         <v>1489</v>
       </c>
       <c r="H41" s="2" t="n">
@@ -46801,7 +46906,7 @@
       <c r="E252" s="2" t="s">
         <v>2131</v>
       </c>
-      <c r="F252" s="28" t="s">
+      <c r="F252" s="29" t="s">
         <v>2132</v>
       </c>
       <c r="H252" s="2" t="n">
@@ -47712,437 +47817,538 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="29" width="23.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="23.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="37.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="23.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="30" width="23.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="37.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="23.42"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="31" t="s">
         <v>37</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>769</v>
       </c>
       <c r="D1" s="5" t="s">
+        <v>779</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>772</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>776</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="str">
-        <f aca="false">CONCATENATE("celex_classif:clc_",B2)</f>
-        <v>celex_classif:clc_1</v>
-      </c>
-      <c r="B2" s="29" t="n">
+        <f aca="false">CONCATENATE("celex_classif:class_",B2)</f>
+        <v>celex_classif:class_1</v>
+      </c>
+      <c r="B2" s="30" t="n">
         <v>1</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="C2" s="28" t="str">
+        <f aca="false">IF(NOT(ISBLANK(D2)),CONCATENATE("celex_classif:class_",D2),""  )</f>
+        <v/>
+      </c>
+      <c r="E2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="F2" s="0" t="s">
         <v>2193</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="str">
-        <f aca="false">CONCATENATE("celex_classif:clc_",B3)</f>
-        <v>celex_classif:clc_2</v>
-      </c>
-      <c r="B3" s="29" t="n">
+        <f aca="false">CONCATENATE("celex_classif:class_",B3)</f>
+        <v>celex_classif:class_2</v>
+      </c>
+      <c r="B3" s="30" t="n">
         <v>2</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="C3" s="28" t="str">
+        <f aca="false">IF(NOT(ISBLANK(D3)),CONCATENATE("celex_classif:class_",D3),""  )</f>
+        <v/>
+      </c>
+      <c r="E3" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="F3" s="0" t="s">
         <v>2194</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="str">
-        <f aca="false">CONCATENATE("celex_classif:clc_",B4)</f>
-        <v>celex_classif:clc_3</v>
-      </c>
-      <c r="B4" s="29" t="n">
+        <f aca="false">CONCATENATE("celex_classif:class_",B4)</f>
+        <v>celex_classif:class_3</v>
+      </c>
+      <c r="B4" s="30" t="n">
         <v>3</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="C4" s="28" t="str">
+        <f aca="false">IF(NOT(ISBLANK(D4)),CONCATENATE("celex_classif:class_",D4),""  )</f>
+        <v/>
+      </c>
+      <c r="E4" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="F4" s="0" t="s">
         <v>2195</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="str">
-        <f aca="false">CONCATENATE("celex_classif:clc_",B5)</f>
-        <v>celex_classif:clc_5</v>
-      </c>
-      <c r="B5" s="29" t="n">
+        <f aca="false">CONCATENATE("celex_classif:class_",B5)</f>
+        <v>celex_classif:class_5</v>
+      </c>
+      <c r="B5" s="30" t="n">
         <v>5</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="C5" s="28" t="str">
+        <f aca="false">IF(NOT(ISBLANK(D5)),CONCATENATE("celex_classif:class_",D5),""  )</f>
+        <v/>
+      </c>
+      <c r="E5" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="F5" s="0" t="s">
         <v>2196</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="str">
-        <f aca="false">CONCATENATE("celex_classif:clc_",B6)</f>
-        <v>celex_classif:clc_5</v>
-      </c>
-      <c r="B6" s="29" t="n">
+        <f aca="false">CONCATENATE("celex_classif:class_",B6)</f>
+        <v>celex_classif:class_5</v>
+      </c>
+      <c r="B6" s="30" t="n">
         <v>5</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="C6" s="28" t="str">
+        <f aca="false">IF(NOT(ISBLANK(D6)),CONCATENATE("celex_classif:class_",D6),""  )</f>
+        <v/>
+      </c>
+      <c r="E6" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="F6" s="0" t="s">
         <v>2197</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="str">
-        <f aca="false">CONCATENATE("celex_classif:clc_",B7)</f>
-        <v>celex_classif:clc_5_CONSIL</v>
-      </c>
-      <c r="B7" s="29" t="s">
+        <f aca="false">CONCATENATE("celex_classif:class_",B7)</f>
+        <v>celex_classif:class_5_CONSIL</v>
+      </c>
+      <c r="B7" s="30" t="s">
         <v>1650</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C7" s="28" t="str">
+        <f aca="false">IF(NOT(ISBLANK(D7)),CONCATENATE("celex_classif:class_",D7),""  )</f>
+        <v>celex_classif:class_5</v>
+      </c>
+      <c r="D7" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="E7" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="F7" s="0" t="s">
         <v>2198</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="str">
-        <f aca="false">CONCATENATE("celex_classif:clc_",B8)</f>
-        <v>celex_classif:clc_5_COM</v>
-      </c>
-      <c r="B8" s="29" t="s">
+        <f aca="false">CONCATENATE("celex_classif:class_",B8)</f>
+        <v>celex_classif:class_5_COM</v>
+      </c>
+      <c r="B8" s="30" t="s">
         <v>1709</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8" s="28" t="str">
+        <f aca="false">IF(NOT(ISBLANK(D8)),CONCATENATE("celex_classif:class_",D8),""  )</f>
+        <v>celex_classif:class_5</v>
+      </c>
+      <c r="D8" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="E8" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="F8" s="0" t="s">
         <v>2199</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="str">
-        <f aca="false">CONCATENATE("celex_classif:clc_",B9)</f>
-        <v>celex_classif:clc_5_EP</v>
-      </c>
-      <c r="B9" s="29" t="s">
+        <f aca="false">CONCATENATE("celex_classif:class_",B9)</f>
+        <v>celex_classif:class_5_EP</v>
+      </c>
+      <c r="B9" s="30" t="s">
         <v>1663</v>
       </c>
-      <c r="C9" s="0" t="n">
+      <c r="C9" s="28" t="str">
+        <f aca="false">IF(NOT(ISBLANK(D9)),CONCATENATE("celex_classif:class_",D9),""  )</f>
+        <v>celex_classif:class_5</v>
+      </c>
+      <c r="D9" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="E9" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="E9" s="0" t="s">
+      <c r="F9" s="0" t="s">
         <v>2200</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="str">
-        <f aca="false">CONCATENATE("celex_classif:clc_",B10)</f>
-        <v>celex_classif:clc_5_ECA</v>
-      </c>
-      <c r="B10" s="29" t="s">
+        <f aca="false">CONCATENATE("celex_classif:class_",B10)</f>
+        <v>celex_classif:class_5_ECA</v>
+      </c>
+      <c r="B10" s="30" t="s">
         <v>1617</v>
       </c>
-      <c r="C10" s="0" t="n">
+      <c r="C10" s="28" t="str">
+        <f aca="false">IF(NOT(ISBLANK(D10)),CONCATENATE("celex_classif:class_",D10),""  )</f>
+        <v>celex_classif:class_5</v>
+      </c>
+      <c r="D10" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="D10" s="0" t="n">
+      <c r="E10" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="E10" s="0" t="s">
+      <c r="F10" s="0" t="s">
         <v>2201</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="str">
-        <f aca="false">CONCATENATE("celex_classif:clc_",B11)</f>
-        <v>celex_classif:clc_5_ECB</v>
-      </c>
-      <c r="B11" s="29" t="s">
+        <f aca="false">CONCATENATE("celex_classif:class_",B11)</f>
+        <v>celex_classif:class_5_ECB</v>
+      </c>
+      <c r="B11" s="30" t="s">
         <v>1625</v>
       </c>
-      <c r="C11" s="0" t="n">
-        <v>5</v>
+      <c r="C11" s="28" t="str">
+        <f aca="false">IF(NOT(ISBLANK(D11)),CONCATENATE("celex_classif:class_",D11),""  )</f>
+        <v>celex_classif:class_5</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="E11" s="0" t="s">
+      <c r="E11" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="F11" s="0" t="s">
         <v>1355</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="str">
-        <f aca="false">CONCATENATE("celex_classif:clc_",B12)</f>
-        <v>celex_classif:clc_5_EESC</v>
-      </c>
-      <c r="B12" s="29" t="s">
+        <f aca="false">CONCATENATE("celex_classif:class_",B12)</f>
+        <v>celex_classif:class_5_EESC</v>
+      </c>
+      <c r="B12" s="30" t="s">
         <v>1633</v>
       </c>
-      <c r="C12" s="0" t="n">
+      <c r="C12" s="28" t="str">
+        <f aca="false">IF(NOT(ISBLANK(D12)),CONCATENATE("celex_classif:class_",D12),""  )</f>
+        <v>celex_classif:class_5</v>
+      </c>
+      <c r="D12" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="D12" s="0" t="n">
+      <c r="E12" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="E12" s="0" t="s">
+      <c r="F12" s="0" t="s">
         <v>1349</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="str">
-        <f aca="false">CONCATENATE("celex_classif:clc_",B13)</f>
-        <v>celex_classif:clc_5_COR</v>
-      </c>
-      <c r="B13" s="29" t="s">
+        <f aca="false">CONCATENATE("celex_classif:class_",B13)</f>
+        <v>celex_classif:class_5_COR</v>
+      </c>
+      <c r="B13" s="30" t="s">
         <v>1677</v>
       </c>
-      <c r="C13" s="0" t="n">
+      <c r="C13" s="28" t="str">
+        <f aca="false">IF(NOT(ISBLANK(D13)),CONCATENATE("celex_classif:class_",D13),""  )</f>
+        <v>celex_classif:class_5</v>
+      </c>
+      <c r="D13" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="D13" s="0" t="n">
+      <c r="E13" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="E13" s="0" t="s">
+      <c r="F13" s="0" t="s">
         <v>1352</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="str">
-        <f aca="false">CONCATENATE("celex_classif:clc_",B14)</f>
-        <v>celex_classif:clc_5_ECSC</v>
-      </c>
-      <c r="B14" s="29" t="s">
+        <f aca="false">CONCATENATE("celex_classif:class_",B14)</f>
+        <v>celex_classif:class_5_ECSC</v>
+      </c>
+      <c r="B14" s="30" t="s">
         <v>1657</v>
       </c>
-      <c r="C14" s="0" t="n">
+      <c r="C14" s="28" t="str">
+        <f aca="false">IF(NOT(ISBLANK(D14)),CONCATENATE("celex_classif:class_",D14),""  )</f>
+        <v>celex_classif:class_5</v>
+      </c>
+      <c r="D14" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="D14" s="0" t="n">
+      <c r="E14" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="E14" s="0" t="s">
+      <c r="F14" s="0" t="s">
         <v>2202</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="str">
-        <f aca="false">CONCATENATE("celex_classif:clc_",B15)</f>
-        <v>celex_classif:clc_5_OTHER</v>
-      </c>
-      <c r="B15" s="29" t="s">
+        <f aca="false">CONCATENATE("celex_classif:class_",B15)</f>
+        <v>celex_classif:class_5_OTHER</v>
+      </c>
+      <c r="B15" s="30" t="s">
         <v>1685</v>
       </c>
-      <c r="C15" s="0" t="n">
+      <c r="C15" s="28" t="str">
+        <f aca="false">IF(NOT(ISBLANK(D15)),CONCATENATE("celex_classif:class_",D15),""  )</f>
+        <v>celex_classif:class_5</v>
+      </c>
+      <c r="D15" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="D15" s="0" t="n">
+      <c r="E15" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="E15" s="0" t="s">
+      <c r="F15" s="0" t="s">
         <v>1338</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="str">
-        <f aca="false">CONCATENATE("celex_classif:clc_",B16)</f>
-        <v>celex_classif:clc_6</v>
-      </c>
-      <c r="B16" s="29" t="n">
+        <f aca="false">CONCATENATE("celex_classif:class_",B16)</f>
+        <v>celex_classif:class_6</v>
+      </c>
+      <c r="B16" s="30" t="n">
         <v>6</v>
       </c>
-      <c r="D16" s="0" t="n">
+      <c r="C16" s="28" t="str">
+        <f aca="false">IF(NOT(ISBLANK(D16)),CONCATENATE("celex_classif:class_",D16),""  )</f>
+        <v/>
+      </c>
+      <c r="E16" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="E16" s="0" t="s">
+      <c r="F16" s="0" t="s">
         <v>2203</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="str">
-        <f aca="false">CONCATENATE("celex_classif:clc_",B17)</f>
-        <v>celex_classif:clc_6_CJ</v>
-      </c>
-      <c r="B17" s="29" t="s">
+        <f aca="false">CONCATENATE("celex_classif:class_",B17)</f>
+        <v>celex_classif:class_6_CJ</v>
+      </c>
+      <c r="B17" s="30" t="s">
         <v>1908</v>
       </c>
-      <c r="C17" s="0" t="n">
+      <c r="C17" s="28" t="str">
+        <f aca="false">IF(NOT(ISBLANK(D17)),CONCATENATE("celex_classif:class_",D17),""  )</f>
+        <v>celex_classif:class_6</v>
+      </c>
+      <c r="D17" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="D17" s="0" t="n">
+      <c r="E17" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E17" s="0" t="s">
+      <c r="F17" s="0" t="s">
         <v>2204</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="str">
-        <f aca="false">CONCATENATE("celex_classif:clc_",B18)</f>
-        <v>celex_classif:clc_6_GCEU</v>
-      </c>
-      <c r="B18" s="29" t="s">
+        <f aca="false">CONCATENATE("celex_classif:class_",B18)</f>
+        <v>celex_classif:class_6_GCEU</v>
+      </c>
+      <c r="B18" s="30" t="s">
         <v>2016</v>
       </c>
-      <c r="C18" s="0" t="n">
+      <c r="C18" s="28" t="str">
+        <f aca="false">IF(NOT(ISBLANK(D18)),CONCATENATE("celex_classif:class_",D18),""  )</f>
+        <v>celex_classif:class_6</v>
+      </c>
+      <c r="D18" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="D18" s="0" t="n">
+      <c r="E18" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="E18" s="0" t="s">
+      <c r="F18" s="0" t="s">
         <v>2205</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="str">
-        <f aca="false">CONCATENATE("celex_classif:clc_",B19)</f>
-        <v>celex_classif:clc_6_CST</v>
-      </c>
-      <c r="B19" s="29" t="s">
+        <f aca="false">CONCATENATE("celex_classif:class_",B19)</f>
+        <v>celex_classif:class_6_CST</v>
+      </c>
+      <c r="B19" s="30" t="s">
         <v>1991</v>
       </c>
-      <c r="C19" s="0" t="n">
+      <c r="C19" s="28" t="str">
+        <f aca="false">IF(NOT(ISBLANK(D19)),CONCATENATE("celex_classif:class_",D19),""  )</f>
+        <v>celex_classif:class_6</v>
+      </c>
+      <c r="D19" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="D19" s="0" t="n">
+      <c r="E19" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="E19" s="0" t="s">
+      <c r="F19" s="0" t="s">
         <v>2206</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="str">
-        <f aca="false">CONCATENATE("celex_classif:clc_",B20)</f>
-        <v>celex_classif:clc_7</v>
-      </c>
-      <c r="B20" s="29" t="n">
+        <f aca="false">CONCATENATE("celex_classif:class_",B20)</f>
+        <v>celex_classif:class_7</v>
+      </c>
+      <c r="B20" s="30" t="n">
         <v>7</v>
       </c>
-      <c r="D20" s="0" t="n">
+      <c r="C20" s="28" t="str">
+        <f aca="false">IF(NOT(ISBLANK(D20)),CONCATENATE("celex_classif:class_",D20),""  )</f>
+        <v/>
+      </c>
+      <c r="E20" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="E20" s="0" t="s">
+      <c r="F20" s="0" t="s">
         <v>2207</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="str">
-        <f aca="false">CONCATENATE("celex_classif:clc_",B21)</f>
-        <v>celex_classif:clc_8</v>
-      </c>
-      <c r="B21" s="29" t="n">
+        <f aca="false">CONCATENATE("celex_classif:class_",B21)</f>
+        <v>celex_classif:class_8</v>
+      </c>
+      <c r="B21" s="30" t="n">
         <v>8</v>
       </c>
-      <c r="D21" s="0" t="n">
+      <c r="C21" s="28" t="str">
+        <f aca="false">IF(NOT(ISBLANK(D21)),CONCATENATE("celex_classif:class_",D21),""  )</f>
+        <v/>
+      </c>
+      <c r="E21" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="E21" s="0" t="s">
+      <c r="F21" s="0" t="s">
         <v>2208</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="str">
-        <f aca="false">CONCATENATE("celex_classif:clc_",B22)</f>
-        <v>celex_classif:clc_9</v>
-      </c>
-      <c r="B22" s="29" t="n">
+        <f aca="false">CONCATENATE("celex_classif:class_",B22)</f>
+        <v>celex_classif:class_9</v>
+      </c>
+      <c r="B22" s="30" t="n">
         <v>9</v>
       </c>
-      <c r="D22" s="0" t="n">
+      <c r="C22" s="28" t="str">
+        <f aca="false">IF(NOT(ISBLANK(D22)),CONCATENATE("celex_classif:class_",D22),""  )</f>
+        <v/>
+      </c>
+      <c r="E22" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="E22" s="0" t="s">
+      <c r="F22" s="0" t="s">
         <v>2209</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="str">
-        <f aca="false">CONCATENATE("celex_classif:clc_",B23)</f>
-        <v>celex_classif:clc_E</v>
-      </c>
-      <c r="B23" s="29" t="s">
+        <f aca="false">CONCATENATE("celex_classif:class_",B23)</f>
+        <v>celex_classif:class_E</v>
+      </c>
+      <c r="B23" s="30" t="s">
         <v>1486</v>
       </c>
-      <c r="D23" s="0" t="n">
+      <c r="C23" s="28" t="str">
+        <f aca="false">IF(NOT(ISBLANK(D23)),CONCATENATE("celex_classif:class_",D23),""  )</f>
+        <v/>
+      </c>
+      <c r="E23" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="E23" s="0" t="s">
+      <c r="F23" s="0" t="s">
         <v>2210</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="str">
-        <f aca="false">CONCATENATE("celex_classif:clc_",B24)</f>
-        <v>celex_classif:clc_C</v>
-      </c>
-      <c r="B24" s="29" t="s">
+        <f aca="false">CONCATENATE("celex_classif:class_",B24)</f>
+        <v>celex_classif:class_C</v>
+      </c>
+      <c r="B24" s="30" t="s">
         <v>1464</v>
       </c>
-      <c r="D24" s="0" t="n">
+      <c r="C24" s="28" t="str">
+        <f aca="false">IF(NOT(ISBLANK(D24)),CONCATENATE("celex_classif:class_",D24),""  )</f>
+        <v/>
+      </c>
+      <c r="E24" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="E24" s="0" t="s">
+      <c r="F24" s="0" t="s">
         <v>2211</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="str">
-        <f aca="false">CONCATENATE("celex_classif:clc_",B25)</f>
-        <v>celex_classif:clc_0</v>
-      </c>
-      <c r="B25" s="29" t="n">
+        <f aca="false">CONCATENATE("celex_classif:class_",B25)</f>
+        <v>celex_classif:class_0</v>
+      </c>
+      <c r="B25" s="30" t="n">
         <v>0</v>
       </c>
-      <c r="D25" s="0" t="n">
+      <c r="C25" s="28" t="str">
+        <f aca="false">IF(NOT(ISBLANK(D25)),CONCATENATE("celex_classif:class_",D25),""  )</f>
+        <v/>
+      </c>
+      <c r="E25" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="E25" s="0" t="s">
+      <c r="F25" s="0" t="s">
         <v>2212</v>
       </c>
     </row>
@@ -48162,15 +48368,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B52"/>
+  <dimension ref="A1:B1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.18359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.19140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="61.24"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -48306,20 +48513,20 @@
         <v>2215</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="28" t="s">
         <v>2245</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>2246</v>
+        <v>2215</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
+        <v>2246</v>
+      </c>
+      <c r="B19" s="0" t="s">
         <v>2247</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>2237</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -48327,265 +48534,282 @@
         <v>2248</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>2249</v>
+        <v>2237</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
+        <v>2249</v>
+      </c>
+      <c r="B21" s="0" t="s">
         <v>2250</v>
       </c>
-      <c r="B21" s="0" t="s">
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="28" t="s">
         <v>2251</v>
       </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
-        <v>2252</v>
-      </c>
       <c r="B22" s="0" t="s">
-        <v>2253</v>
+        <v>2250</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>2254</v>
+        <v>2252</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>2255</v>
+        <v>2253</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>2256</v>
+        <v>2254</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>2257</v>
+        <v>2255</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>2258</v>
+        <v>2256</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>2259</v>
+        <v>2257</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>2260</v>
+        <v>2258</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>2261</v>
+        <v>2259</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>2262</v>
+        <v>2260</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>2263</v>
+        <v>2261</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>2264</v>
+        <v>2262</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>2265</v>
+        <v>2263</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>2266</v>
+        <v>2264</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>2267</v>
+        <v>2265</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>2268</v>
+        <v>2266</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>2269</v>
+        <v>2267</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>2270</v>
+        <v>2268</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>2271</v>
+        <v>2269</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>2272</v>
+        <v>2270</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>2273</v>
+        <v>2271</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>2274</v>
+        <v>2272</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>2275</v>
+        <v>2273</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>2276</v>
+        <v>2274</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>2277</v>
+        <v>2275</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>2278</v>
+        <v>2276</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>2279</v>
+        <v>2277</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>2280</v>
+        <v>2278</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>2281</v>
+        <v>2279</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>2282</v>
+        <v>2280</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>2283</v>
+        <v>2281</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>2284</v>
+        <v>2282</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>2285</v>
+        <v>2283</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>2286</v>
+        <v>2284</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>2287</v>
+        <v>2285</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>2288</v>
+        <v>2286</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>2289</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>2290</v>
+        <v>2288</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>2291</v>
+        <v>2289</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>2292</v>
+        <v>2290</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>2253</v>
+        <v>2291</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
+        <v>2292</v>
+      </c>
+      <c r="B43" s="0" t="s">
         <v>2293</v>
-      </c>
-      <c r="B43" s="0" t="s">
-        <v>2294</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>2295</v>
+        <v>2294</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>2296</v>
+        <v>2255</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>2297</v>
+        <v>2295</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>2298</v>
+        <v>2296</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>2299</v>
+        <v>2297</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>2300</v>
+        <v>2298</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>2301</v>
+        <v>2299</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>2302</v>
+        <v>2300</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>2303</v>
+        <v>2301</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>2304</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>2305</v>
+        <v>2303</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>2255</v>
+        <v>2304</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
+        <v>2305</v>
+      </c>
+      <c r="B50" s="0" t="s">
         <v>2306</v>
-      </c>
-      <c r="B50" s="0" t="s">
-        <v>2307</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>2308</v>
+        <v>2307</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>2309</v>
+        <v>2257</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
+        <v>2308</v>
+      </c>
+      <c r="B52" s="0" t="s">
+        <v>2309</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
         <v>2310</v>
       </c>
-      <c r="B52" s="0" t="s">
+      <c r="B53" s="0" t="s">
         <v>2311</v>
       </c>
     </row>
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>2312</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>2313</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -48604,11 +48828,11 @@
   </sheetPr>
   <dimension ref="A1:B116"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A91" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A113" activeCellId="0" sqref="A113"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.18359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.19140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="80.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.28"/>
@@ -48627,23 +48851,23 @@
         <v>39</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>2312</v>
+        <v>2314</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>2313</v>
+        <v>2315</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>2314</v>
+        <v>2316</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>2313</v>
+        <v>2315</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>2315</v>
+        <v>2317</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -48651,7 +48875,7 @@
         <v>50</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>2316</v>
+        <v>2318</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -48659,7 +48883,7 @@
         <v>54</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>2317</v>
+        <v>2319</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -48667,7 +48891,7 @@
         <v>57</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>2318</v>
+        <v>2320</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -48675,7 +48899,7 @@
         <v>61</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>2319</v>
+        <v>2321</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -48683,7 +48907,7 @@
         <v>64</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>2320</v>
+        <v>2322</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -48691,7 +48915,7 @@
         <v>70</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>2321</v>
+        <v>2323</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -48699,7 +48923,7 @@
         <v>82</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>2322</v>
+        <v>2324</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -48707,7 +48931,7 @@
         <v>90</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>2323</v>
+        <v>2325</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -48715,7 +48939,7 @@
         <v>99</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>2324</v>
+        <v>2326</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -48723,7 +48947,7 @@
         <v>102</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>2325</v>
+        <v>2327</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -48731,7 +48955,7 @@
         <v>108</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>2326</v>
+        <v>2328</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -48739,7 +48963,7 @@
         <v>118</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>2327</v>
+        <v>2329</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -48747,7 +48971,7 @@
         <v>125</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>2328</v>
+        <v>2330</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -48755,7 +48979,7 @@
         <v>133</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>2329</v>
+        <v>2331</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -48763,7 +48987,7 @@
         <v>140</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>2330</v>
+        <v>2332</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -48771,7 +48995,7 @@
         <v>153</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>2331</v>
+        <v>2333</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -48779,7 +49003,7 @@
         <v>163</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>2332</v>
+        <v>2334</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -48787,7 +49011,7 @@
         <v>172</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>2333</v>
+        <v>2335</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -48795,7 +49019,7 @@
         <v>179</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>2334</v>
+        <v>2336</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -48803,7 +49027,7 @@
         <v>188</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>2335</v>
+        <v>2337</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -48811,7 +49035,7 @@
         <v>196</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>2336</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -48819,7 +49043,7 @@
         <v>203</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>2337</v>
+        <v>2339</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -48827,7 +49051,7 @@
         <v>211</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>2338</v>
+        <v>2340</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -48835,7 +49059,7 @@
         <v>218</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>2339</v>
+        <v>2341</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -48843,7 +49067,7 @@
         <v>226</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>2340</v>
+        <v>2342</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -48851,7 +49075,7 @@
         <v>232</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>2341</v>
+        <v>2343</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -48859,7 +49083,7 @@
         <v>239</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>2342</v>
+        <v>2344</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -48867,7 +49091,7 @@
         <v>247</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>2343</v>
+        <v>2345</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -48875,7 +49099,7 @@
         <v>256</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>2344</v>
+        <v>2346</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -48883,7 +49107,7 @@
         <v>265</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>2345</v>
+        <v>2347</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -48891,7 +49115,7 @@
         <v>273</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>2346</v>
+        <v>2348</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -48899,7 +49123,7 @@
         <v>279</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>2347</v>
+        <v>2349</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -48907,7 +49131,7 @@
         <v>287</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>2348</v>
+        <v>2350</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -48915,7 +49139,7 @@
         <v>295</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>2349</v>
+        <v>2351</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -48923,7 +49147,7 @@
         <v>301</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>2350</v>
+        <v>2352</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -48931,7 +49155,7 @@
         <v>310</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>2351</v>
+        <v>2353</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -48939,7 +49163,7 @@
         <v>319</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>2352</v>
+        <v>2354</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -48947,7 +49171,7 @@
         <v>326</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>2353</v>
+        <v>2355</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -48955,7 +49179,7 @@
         <v>335</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>2354</v>
+        <v>2356</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -48963,7 +49187,7 @@
         <v>343</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>2355</v>
+        <v>2357</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -48971,7 +49195,7 @@
         <v>351</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>2356</v>
+        <v>2358</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -48979,7 +49203,7 @@
         <v>359</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>2357</v>
+        <v>2359</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -48987,7 +49211,7 @@
         <v>367</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>2358</v>
+        <v>2360</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -48995,7 +49219,7 @@
         <v>387</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>2359</v>
+        <v>2361</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49003,7 +49227,7 @@
         <v>411</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>2360</v>
+        <v>2362</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49011,7 +49235,7 @@
         <v>417</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>2361</v>
+        <v>2363</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49019,7 +49243,7 @@
         <v>422</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>2362</v>
+        <v>2364</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49027,7 +49251,7 @@
         <v>428</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>2363</v>
+        <v>2365</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49035,7 +49259,7 @@
         <v>435</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>2364</v>
+        <v>2366</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49043,7 +49267,7 @@
         <v>441</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>2365</v>
+        <v>2367</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49051,7 +49275,7 @@
         <v>447</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>2366</v>
+        <v>2368</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49059,7 +49283,7 @@
         <v>454</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>2367</v>
+        <v>2369</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49067,7 +49291,7 @@
         <v>461</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>2368</v>
+        <v>2370</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49075,7 +49299,7 @@
         <v>468</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>2369</v>
+        <v>2371</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49083,7 +49307,7 @@
         <v>474</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>2370</v>
+        <v>2372</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49091,7 +49315,7 @@
         <v>480</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>2371</v>
+        <v>2373</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49099,7 +49323,7 @@
         <v>487</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>2372</v>
+        <v>2374</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49107,7 +49331,7 @@
         <v>493</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>2373</v>
+        <v>2375</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49115,7 +49339,7 @@
         <v>499</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>2374</v>
+        <v>2376</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49123,7 +49347,7 @@
         <v>504</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>2375</v>
+        <v>2377</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49131,7 +49355,7 @@
         <v>510</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>2376</v>
+        <v>2378</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49139,7 +49363,7 @@
         <v>516</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>2377</v>
+        <v>2379</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49147,7 +49371,7 @@
         <v>521</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>2378</v>
+        <v>2380</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49155,7 +49379,7 @@
         <v>527</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>2379</v>
+        <v>2381</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49163,7 +49387,7 @@
         <v>533</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>2380</v>
+        <v>2382</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49171,7 +49395,7 @@
         <v>539</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>2381</v>
+        <v>2383</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49179,7 +49403,7 @@
         <v>544</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>2382</v>
+        <v>2384</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49187,7 +49411,7 @@
         <v>550</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>2383</v>
+        <v>2385</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49195,7 +49419,7 @@
         <v>556</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>2384</v>
+        <v>2386</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49203,7 +49427,7 @@
         <v>560</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>2385</v>
+        <v>2387</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49211,7 +49435,7 @@
         <v>564</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>2386</v>
+        <v>2388</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49219,7 +49443,7 @@
         <v>569</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>2387</v>
+        <v>2389</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49227,7 +49451,7 @@
         <v>574</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>2388</v>
+        <v>2390</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49235,7 +49459,7 @@
         <v>585</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>2389</v>
+        <v>2391</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49243,7 +49467,7 @@
         <v>594</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>2390</v>
+        <v>2392</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49251,7 +49475,7 @@
         <v>600</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>2391</v>
+        <v>2393</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49259,7 +49483,7 @@
         <v>605</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>2392</v>
+        <v>2394</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49267,7 +49491,7 @@
         <v>614</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>2393</v>
+        <v>2395</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49275,7 +49499,7 @@
         <v>620</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>2394</v>
+        <v>2396</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49283,7 +49507,7 @@
         <v>627</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>2395</v>
+        <v>2397</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49291,7 +49515,7 @@
         <v>633</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>2396</v>
+        <v>2398</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49299,7 +49523,7 @@
         <v>639</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>2397</v>
+        <v>2399</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49307,7 +49531,7 @@
         <v>643</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>2398</v>
+        <v>2400</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49315,7 +49539,7 @@
         <v>647</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>2399</v>
+        <v>2401</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49323,7 +49547,7 @@
         <v>651</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>2400</v>
+        <v>2402</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49331,7 +49555,7 @@
         <v>655</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>2401</v>
+        <v>2403</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49339,7 +49563,7 @@
         <v>659</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>2402</v>
+        <v>2404</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49347,7 +49571,7 @@
         <v>663</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>2403</v>
+        <v>2405</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49475,7 +49699,7 @@
         <v>734</v>
       </c>
       <c r="B108" s="0" t="s">
-        <v>2404</v>
+        <v>2406</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49483,7 +49707,7 @@
         <v>740</v>
       </c>
       <c r="B109" s="0" t="s">
-        <v>2405</v>
+        <v>2407</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49491,7 +49715,7 @@
         <v>745</v>
       </c>
       <c r="B110" s="0" t="s">
-        <v>2406</v>
+        <v>2408</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49499,7 +49723,7 @@
         <v>751</v>
       </c>
       <c r="B111" s="0" t="s">
-        <v>2407</v>
+        <v>2409</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49507,7 +49731,7 @@
         <v>757</v>
       </c>
       <c r="B112" s="0" t="s">
-        <v>2408</v>
+        <v>2410</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49515,7 +49739,7 @@
         <v>765</v>
       </c>
       <c r="B113" s="0" t="s">
-        <v>2409</v>
+        <v>2411</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49523,7 +49747,7 @@
         <v>768</v>
       </c>
       <c r="B114" s="0" t="s">
-        <v>2410</v>
+        <v>2412</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49531,7 +49755,7 @@
         <v>771</v>
       </c>
       <c r="B115" s="0" t="s">
-        <v>2411</v>
+        <v>2413</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49539,7 +49763,7 @@
         <v>774</v>
       </c>
       <c r="B116" s="0" t="s">
-        <v>2412</v>
+        <v>2414</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix problem with RBD Document Property class self parent.
</commit_message>
<xml_diff>
--- a/resources/input_workbook/LAM_metadata_20200903_JKU.xlsx
+++ b/resources/input_workbook/LAM_metadata_20200903_JKU.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LAM properties" sheetId="1" state="visible" r:id="rId2"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5781" uniqueCount="2415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5780" uniqueCount="2415">
   <si>
     <t xml:space="preserve">URI</t>
   </si>
@@ -19353,7 +19353,7 @@
     <numFmt numFmtId="166" formatCode="[$-809]dd/mm/yyyy"/>
     <numFmt numFmtId="167" formatCode="0.00E+00"/>
   </numFmts>
-  <fonts count="33">
+  <fonts count="32">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -19578,12 +19578,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -19678,7 +19672,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -19791,10 +19785,6 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -19892,9 +19882,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>219600</xdr:colOff>
+      <xdr:colOff>219240</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>669240</xdr:rowOff>
+      <xdr:rowOff>668880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -19904,7 +19894,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="7830000" cy="8163360"/>
+          <a:ext cx="9809640" cy="8163000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -19937,9 +19927,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
-      <xdr:colOff>636840</xdr:colOff>
+      <xdr:colOff>636480</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>2036880</xdr:rowOff>
+      <xdr:rowOff>2036520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -19949,7 +19939,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="10038960" cy="9531000"/>
+          <a:ext cx="12485520" cy="9530640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -19987,9 +19977,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>453600</xdr:colOff>
+      <xdr:colOff>453240</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>173160</xdr:rowOff>
+      <xdr:rowOff>172800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -19999,7 +19989,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="17856360" cy="4627440"/>
+          <a:ext cx="22384800" cy="5195520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -20038,13 +20028,13 @@
   </sheetPr>
   <dimension ref="A1:AK118"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="AJ2" activeCellId="0" sqref="AJ2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9.12890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="2"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="23.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.57"/>
@@ -20058,7 +20048,7 @@
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="2" max="10" min="10" style="1" width="22.57"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="2" max="11" min="11" style="1" width="23.88"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="2" max="12" min="12" style="1" width="11.71"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="2" max="13" min="13" style="1" width="18.12"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="2" max="13" min="13" style="1" width="18.13"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="2" max="14" min="14" style="1" width="17.71"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="2" max="15" min="15" style="1" width="11.71"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="2" max="16" min="16" style="1" width="32.57"/>
@@ -28070,13 +28060,13 @@
   </sheetPr>
   <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.19140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.1953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.57"/>
@@ -28289,7 +28279,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="225.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="270.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="str">
         <f aca="false">CONCATENATE("lamd:class_",B10)</f>
         <v>lamd:class_RBD</v>
@@ -28299,10 +28289,7 @@
       </c>
       <c r="C10" s="2" t="str">
         <f aca="false">IF(NOT(ISBLANK(D10)),CONCATENATE("lamd:class_",D10),""  )</f>
-        <v>lamd:class_RBD</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>797</v>
+        <v/>
       </c>
       <c r="E10" s="0" t="n">
         <v>2</v>
@@ -28589,12 +28576,12 @@
       <selection pane="bottomLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9.12890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="1"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="23" width="10.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="23" width="40.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="23" width="67.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="5" min="5" style="23" width="67.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="23" width="67.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="5" min="5" style="23" width="67.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="6" min="6" style="23" width="80.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="7" min="7" style="23" width="23.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="8" min="8" style="23" width="31.15"/>
@@ -28616,7 +28603,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="27" min="27" style="23" width="3.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="28" min="28" style="23" width="13.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="29" min="29" style="23" width="3.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="30" min="30" style="23" width="3.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="30" min="30" style="23" width="3.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="31" min="31" style="23" width="3.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="32" min="32" style="23" width="3.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="33" min="33" style="23" width="3.42"/>
@@ -28630,7 +28617,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="42" min="42" style="23" width="3.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="43" min="43" style="23" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="44" min="44" style="23" width="3.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="45" min="45" style="23" width="3.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="45" min="45" style="23" width="3.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="46" min="46" style="23" width="3.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="47" min="47" style="23" width="11.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="48" min="48" style="23" width="2.85"/>
@@ -28654,7 +28641,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="67" min="67" style="23" width="17.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="68" min="68" style="23" width="15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="69" min="69" style="23" width="15.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="70" min="70" style="23" width="8.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="70" min="70" style="23" width="8.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="71" min="71" style="23" width="9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="72" min="72" style="23" width="13.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="73" min="73" style="23" width="17.13"/>
@@ -28674,7 +28661,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="90" min="90" style="23" width="15.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="91" min="91" style="23" width="12.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="92" min="92" style="23" width="15.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="93" min="93" style="23" width="22.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="93" min="93" style="23" width="22.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="94" min="94" style="23" width="11.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="95" min="95" style="23" width="16.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="98" min="96" style="23" width="20.57"/>
@@ -36644,7 +36631,7 @@
       <c r="B2" s="5" t="s">
         <v>1326</v>
       </c>
-      <c r="C2" s="28" t="str">
+      <c r="C2" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D2)),CONCATENATE("class_classif:class_",D2),""  )</f>
         <v/>
       </c>
@@ -36668,7 +36655,7 @@
       <c r="B3" s="5" t="s">
         <v>996</v>
       </c>
-      <c r="C3" s="28" t="str">
+      <c r="C3" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D3)),CONCATENATE("class_classif:class_",D3),""  )</f>
         <v/>
       </c>
@@ -36692,7 +36679,7 @@
       <c r="B4" s="5" t="s">
         <v>1147</v>
       </c>
-      <c r="C4" s="28" t="str">
+      <c r="C4" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D4)),CONCATENATE("class_classif:class_",D4),""  )</f>
         <v/>
       </c>
@@ -36716,7 +36703,7 @@
       <c r="B5" s="5" t="s">
         <v>1333</v>
       </c>
-      <c r="C5" s="28" t="str">
+      <c r="C5" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D5)),CONCATENATE("class_classif:class_",D5),""  )</f>
         <v>class_classif:class_LEGAL</v>
       </c>
@@ -36742,7 +36729,7 @@
       <c r="B6" s="5" t="s">
         <v>1251</v>
       </c>
-      <c r="C6" s="28" t="str">
+      <c r="C6" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D6)),CONCATENATE("class_classif:class_",D6),""  )</f>
         <v>class_classif:class_LEGAL</v>
       </c>
@@ -36768,7 +36755,7 @@
       <c r="B7" s="5" t="s">
         <v>1148</v>
       </c>
-      <c r="C7" s="28" t="str">
+      <c r="C7" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D7)),CONCATENATE("class_classif:class_",D7),""  )</f>
         <v>class_classif:class_LEGAL</v>
       </c>
@@ -36794,7 +36781,7 @@
       <c r="B8" s="0" t="s">
         <v>839</v>
       </c>
-      <c r="C8" s="28" t="str">
+      <c r="C8" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D8)),CONCATENATE("class_classif:class_",D8),""  )</f>
         <v/>
       </c>
@@ -36816,7 +36803,7 @@
       <c r="B9" s="0" t="s">
         <v>840</v>
       </c>
-      <c r="C9" s="28" t="str">
+      <c r="C9" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D9)),CONCATENATE("class_classif:class_",D9),""  )</f>
         <v>class_classif:class_PREPDOC</v>
       </c>
@@ -36841,7 +36828,7 @@
       <c r="B10" s="0" t="s">
         <v>914</v>
       </c>
-      <c r="C10" s="28" t="str">
+      <c r="C10" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D10)),CONCATENATE("class_classif:class_",D10),""  )</f>
         <v>class_classif:class_PREPDOC</v>
       </c>
@@ -36866,7 +36853,7 @@
       <c r="B11" s="0" t="s">
         <v>1346</v>
       </c>
-      <c r="C11" s="28" t="str">
+      <c r="C11" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D11)),CONCATENATE("class_classif:class_",D11),""  )</f>
         <v>class_classif:class_PREPDOC</v>
       </c>
@@ -36891,7 +36878,7 @@
       <c r="B12" s="0" t="s">
         <v>874</v>
       </c>
-      <c r="C12" s="28" t="str">
+      <c r="C12" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D12)),CONCATENATE("class_classif:class_",D12),""  )</f>
         <v>class_classif:class_PREPDOC</v>
       </c>
@@ -36916,7 +36903,7 @@
       <c r="B13" s="0" t="s">
         <v>1351</v>
       </c>
-      <c r="C13" s="28" t="str">
+      <c r="C13" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D13)),CONCATENATE("class_classif:class_",D13),""  )</f>
         <v>class_classif:class_PREPDOC</v>
       </c>
@@ -36941,7 +36928,7 @@
       <c r="B14" s="0" t="s">
         <v>1354</v>
       </c>
-      <c r="C14" s="28" t="str">
+      <c r="C14" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D14)),CONCATENATE("class_classif:class_",D14),""  )</f>
         <v>class_classif:class_PREPDOC</v>
       </c>
@@ -36966,7 +36953,7 @@
       <c r="B15" s="0" t="s">
         <v>1176</v>
       </c>
-      <c r="C15" s="28" t="str">
+      <c r="C15" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D15)),CONCATENATE("class_classif:class_",D15),""  )</f>
         <v>class_classif:class_PREPDOC</v>
       </c>
@@ -36991,7 +36978,7 @@
       <c r="B16" s="0" t="s">
         <v>973</v>
       </c>
-      <c r="C16" s="28" t="str">
+      <c r="C16" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D16)),CONCATENATE("class_classif:class_",D16),""  )</f>
         <v/>
       </c>
@@ -37013,7 +37000,7 @@
       <c r="B17" s="0" t="s">
         <v>1037</v>
       </c>
-      <c r="C17" s="28" t="str">
+      <c r="C17" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D17)),CONCATENATE("class_classif:class_",D17),""  )</f>
         <v/>
       </c>
@@ -37035,7 +37022,7 @@
       <c r="B18" s="0" t="s">
         <v>1022</v>
       </c>
-      <c r="C18" s="28" t="str">
+      <c r="C18" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D18)),CONCATENATE("class_classif:class_",D18),""  )</f>
         <v/>
       </c>
@@ -37057,7 +37044,7 @@
       <c r="B19" s="0" t="s">
         <v>1023</v>
       </c>
-      <c r="C19" s="28" t="str">
+      <c r="C19" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D19)),CONCATENATE("class_classif:class_",D19),""  )</f>
         <v>class_classif:class_CDOC</v>
       </c>
@@ -37082,7 +37069,7 @@
       <c r="B20" s="0" t="s">
         <v>1208</v>
       </c>
-      <c r="C20" s="28" t="str">
+      <c r="C20" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D20)),CONCATENATE("class_classif:class_",D20),""  )</f>
         <v>class_classif:class_CDOC</v>
       </c>
@@ -37104,7 +37091,7 @@
       <c r="B21" s="0" t="s">
         <v>1318</v>
       </c>
-      <c r="C21" s="28" t="str">
+      <c r="C21" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D21)),CONCATENATE("class_classif:class_",D21),""  )</f>
         <v>class_classif:class_CDOC</v>
       </c>
@@ -37129,7 +37116,7 @@
       <c r="B22" s="0" t="s">
         <v>1118</v>
       </c>
-      <c r="C22" s="28" t="str">
+      <c r="C22" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D22)),CONCATENATE("class_classif:class_",D22),""  )</f>
         <v>class_classif:class_CDOC</v>
       </c>
@@ -37167,7 +37154,7 @@
       <selection pane="bottomLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9.12890625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="1"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="27.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="16.14"/>
@@ -37175,7 +37162,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="40.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="6" min="6" style="2" width="93.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="7" min="7" style="2" width="123.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="7" min="7" style="2" width="123.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="8" min="8" style="2" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="9" min="9" style="2" width="22.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="10" min="10" style="2" width="22.57"/>
@@ -38681,7 +38668,7 @@
       <c r="E41" s="2" t="s">
         <v>1488</v>
       </c>
-      <c r="F41" s="29" t="s">
+      <c r="F41" s="28" t="s">
         <v>1489</v>
       </c>
       <c r="H41" s="2" t="n">
@@ -46906,7 +46893,7 @@
       <c r="E252" s="2" t="s">
         <v>2131</v>
       </c>
-      <c r="F252" s="29" t="s">
+      <c r="F252" s="28" t="s">
         <v>2132</v>
       </c>
       <c r="H252" s="2" t="n">
@@ -47826,19 +47813,19 @@
   <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="30" width="23.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="29" width="23.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="37.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="23.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="37.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="23.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="30" t="s">
         <v>37</v>
       </c>
       <c r="C1" s="5" t="s">
@@ -47865,10 +47852,10 @@
         <f aca="false">CONCATENATE("celex_classif:class_",B2)</f>
         <v>celex_classif:class_1</v>
       </c>
-      <c r="B2" s="30" t="n">
+      <c r="B2" s="29" t="n">
         <v>1</v>
       </c>
-      <c r="C2" s="28" t="str">
+      <c r="C2" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D2)),CONCATENATE("celex_classif:class_",D2),""  )</f>
         <v/>
       </c>
@@ -47884,10 +47871,10 @@
         <f aca="false">CONCATENATE("celex_classif:class_",B3)</f>
         <v>celex_classif:class_2</v>
       </c>
-      <c r="B3" s="30" t="n">
+      <c r="B3" s="29" t="n">
         <v>2</v>
       </c>
-      <c r="C3" s="28" t="str">
+      <c r="C3" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D3)),CONCATENATE("celex_classif:class_",D3),""  )</f>
         <v/>
       </c>
@@ -47903,10 +47890,10 @@
         <f aca="false">CONCATENATE("celex_classif:class_",B4)</f>
         <v>celex_classif:class_3</v>
       </c>
-      <c r="B4" s="30" t="n">
+      <c r="B4" s="29" t="n">
         <v>3</v>
       </c>
-      <c r="C4" s="28" t="str">
+      <c r="C4" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D4)),CONCATENATE("celex_classif:class_",D4),""  )</f>
         <v/>
       </c>
@@ -47922,10 +47909,10 @@
         <f aca="false">CONCATENATE("celex_classif:class_",B5)</f>
         <v>celex_classif:class_5</v>
       </c>
-      <c r="B5" s="30" t="n">
+      <c r="B5" s="29" t="n">
         <v>5</v>
       </c>
-      <c r="C5" s="28" t="str">
+      <c r="C5" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D5)),CONCATENATE("celex_classif:class_",D5),""  )</f>
         <v/>
       </c>
@@ -47941,10 +47928,10 @@
         <f aca="false">CONCATENATE("celex_classif:class_",B6)</f>
         <v>celex_classif:class_5</v>
       </c>
-      <c r="B6" s="30" t="n">
+      <c r="B6" s="29" t="n">
         <v>5</v>
       </c>
-      <c r="C6" s="28" t="str">
+      <c r="C6" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D6)),CONCATENATE("celex_classif:class_",D6),""  )</f>
         <v/>
       </c>
@@ -47960,10 +47947,10 @@
         <f aca="false">CONCATENATE("celex_classif:class_",B7)</f>
         <v>celex_classif:class_5_CONSIL</v>
       </c>
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="29" t="s">
         <v>1650</v>
       </c>
-      <c r="C7" s="28" t="str">
+      <c r="C7" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D7)),CONCATENATE("celex_classif:class_",D7),""  )</f>
         <v>celex_classif:class_5</v>
       </c>
@@ -47982,10 +47969,10 @@
         <f aca="false">CONCATENATE("celex_classif:class_",B8)</f>
         <v>celex_classif:class_5_COM</v>
       </c>
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="29" t="s">
         <v>1709</v>
       </c>
-      <c r="C8" s="28" t="str">
+      <c r="C8" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D8)),CONCATENATE("celex_classif:class_",D8),""  )</f>
         <v>celex_classif:class_5</v>
       </c>
@@ -48004,10 +47991,10 @@
         <f aca="false">CONCATENATE("celex_classif:class_",B9)</f>
         <v>celex_classif:class_5_EP</v>
       </c>
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="29" t="s">
         <v>1663</v>
       </c>
-      <c r="C9" s="28" t="str">
+      <c r="C9" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D9)),CONCATENATE("celex_classif:class_",D9),""  )</f>
         <v>celex_classif:class_5</v>
       </c>
@@ -48026,10 +48013,10 @@
         <f aca="false">CONCATENATE("celex_classif:class_",B10)</f>
         <v>celex_classif:class_5_ECA</v>
       </c>
-      <c r="B10" s="30" t="s">
+      <c r="B10" s="29" t="s">
         <v>1617</v>
       </c>
-      <c r="C10" s="28" t="str">
+      <c r="C10" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D10)),CONCATENATE("celex_classif:class_",D10),""  )</f>
         <v>celex_classif:class_5</v>
       </c>
@@ -48048,10 +48035,10 @@
         <f aca="false">CONCATENATE("celex_classif:class_",B11)</f>
         <v>celex_classif:class_5_ECB</v>
       </c>
-      <c r="B11" s="30" t="s">
+      <c r="B11" s="29" t="s">
         <v>1625</v>
       </c>
-      <c r="C11" s="28" t="str">
+      <c r="C11" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D11)),CONCATENATE("celex_classif:class_",D11),""  )</f>
         <v>celex_classif:class_5</v>
       </c>
@@ -48070,10 +48057,10 @@
         <f aca="false">CONCATENATE("celex_classif:class_",B12)</f>
         <v>celex_classif:class_5_EESC</v>
       </c>
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="29" t="s">
         <v>1633</v>
       </c>
-      <c r="C12" s="28" t="str">
+      <c r="C12" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D12)),CONCATENATE("celex_classif:class_",D12),""  )</f>
         <v>celex_classif:class_5</v>
       </c>
@@ -48092,10 +48079,10 @@
         <f aca="false">CONCATENATE("celex_classif:class_",B13)</f>
         <v>celex_classif:class_5_COR</v>
       </c>
-      <c r="B13" s="30" t="s">
+      <c r="B13" s="29" t="s">
         <v>1677</v>
       </c>
-      <c r="C13" s="28" t="str">
+      <c r="C13" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D13)),CONCATENATE("celex_classif:class_",D13),""  )</f>
         <v>celex_classif:class_5</v>
       </c>
@@ -48114,10 +48101,10 @@
         <f aca="false">CONCATENATE("celex_classif:class_",B14)</f>
         <v>celex_classif:class_5_ECSC</v>
       </c>
-      <c r="B14" s="30" t="s">
+      <c r="B14" s="29" t="s">
         <v>1657</v>
       </c>
-      <c r="C14" s="28" t="str">
+      <c r="C14" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D14)),CONCATENATE("celex_classif:class_",D14),""  )</f>
         <v>celex_classif:class_5</v>
       </c>
@@ -48136,10 +48123,10 @@
         <f aca="false">CONCATENATE("celex_classif:class_",B15)</f>
         <v>celex_classif:class_5_OTHER</v>
       </c>
-      <c r="B15" s="30" t="s">
+      <c r="B15" s="29" t="s">
         <v>1685</v>
       </c>
-      <c r="C15" s="28" t="str">
+      <c r="C15" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D15)),CONCATENATE("celex_classif:class_",D15),""  )</f>
         <v>celex_classif:class_5</v>
       </c>
@@ -48158,10 +48145,10 @@
         <f aca="false">CONCATENATE("celex_classif:class_",B16)</f>
         <v>celex_classif:class_6</v>
       </c>
-      <c r="B16" s="30" t="n">
+      <c r="B16" s="29" t="n">
         <v>6</v>
       </c>
-      <c r="C16" s="28" t="str">
+      <c r="C16" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D16)),CONCATENATE("celex_classif:class_",D16),""  )</f>
         <v/>
       </c>
@@ -48177,10 +48164,10 @@
         <f aca="false">CONCATENATE("celex_classif:class_",B17)</f>
         <v>celex_classif:class_6_CJ</v>
       </c>
-      <c r="B17" s="30" t="s">
+      <c r="B17" s="29" t="s">
         <v>1908</v>
       </c>
-      <c r="C17" s="28" t="str">
+      <c r="C17" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D17)),CONCATENATE("celex_classif:class_",D17),""  )</f>
         <v>celex_classif:class_6</v>
       </c>
@@ -48199,10 +48186,10 @@
         <f aca="false">CONCATENATE("celex_classif:class_",B18)</f>
         <v>celex_classif:class_6_GCEU</v>
       </c>
-      <c r="B18" s="30" t="s">
+      <c r="B18" s="29" t="s">
         <v>2016</v>
       </c>
-      <c r="C18" s="28" t="str">
+      <c r="C18" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D18)),CONCATENATE("celex_classif:class_",D18),""  )</f>
         <v>celex_classif:class_6</v>
       </c>
@@ -48221,10 +48208,10 @@
         <f aca="false">CONCATENATE("celex_classif:class_",B19)</f>
         <v>celex_classif:class_6_CST</v>
       </c>
-      <c r="B19" s="30" t="s">
+      <c r="B19" s="29" t="s">
         <v>1991</v>
       </c>
-      <c r="C19" s="28" t="str">
+      <c r="C19" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D19)),CONCATENATE("celex_classif:class_",D19),""  )</f>
         <v>celex_classif:class_6</v>
       </c>
@@ -48243,10 +48230,10 @@
         <f aca="false">CONCATENATE("celex_classif:class_",B20)</f>
         <v>celex_classif:class_7</v>
       </c>
-      <c r="B20" s="30" t="n">
+      <c r="B20" s="29" t="n">
         <v>7</v>
       </c>
-      <c r="C20" s="28" t="str">
+      <c r="C20" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D20)),CONCATENATE("celex_classif:class_",D20),""  )</f>
         <v/>
       </c>
@@ -48262,10 +48249,10 @@
         <f aca="false">CONCATENATE("celex_classif:class_",B21)</f>
         <v>celex_classif:class_8</v>
       </c>
-      <c r="B21" s="30" t="n">
+      <c r="B21" s="29" t="n">
         <v>8</v>
       </c>
-      <c r="C21" s="28" t="str">
+      <c r="C21" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D21)),CONCATENATE("celex_classif:class_",D21),""  )</f>
         <v/>
       </c>
@@ -48281,10 +48268,10 @@
         <f aca="false">CONCATENATE("celex_classif:class_",B22)</f>
         <v>celex_classif:class_9</v>
       </c>
-      <c r="B22" s="30" t="n">
+      <c r="B22" s="29" t="n">
         <v>9</v>
       </c>
-      <c r="C22" s="28" t="str">
+      <c r="C22" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D22)),CONCATENATE("celex_classif:class_",D22),""  )</f>
         <v/>
       </c>
@@ -48300,10 +48287,10 @@
         <f aca="false">CONCATENATE("celex_classif:class_",B23)</f>
         <v>celex_classif:class_E</v>
       </c>
-      <c r="B23" s="30" t="s">
+      <c r="B23" s="29" t="s">
         <v>1486</v>
       </c>
-      <c r="C23" s="28" t="str">
+      <c r="C23" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D23)),CONCATENATE("celex_classif:class_",D23),""  )</f>
         <v/>
       </c>
@@ -48319,10 +48306,10 @@
         <f aca="false">CONCATENATE("celex_classif:class_",B24)</f>
         <v>celex_classif:class_C</v>
       </c>
-      <c r="B24" s="30" t="s">
+      <c r="B24" s="29" t="s">
         <v>1464</v>
       </c>
-      <c r="C24" s="28" t="str">
+      <c r="C24" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D24)),CONCATENATE("celex_classif:class_",D24),""  )</f>
         <v/>
       </c>
@@ -48338,10 +48325,10 @@
         <f aca="false">CONCATENATE("celex_classif:class_",B25)</f>
         <v>celex_classif:class_0</v>
       </c>
-      <c r="B25" s="30" t="n">
+      <c r="B25" s="29" t="n">
         <v>0</v>
       </c>
-      <c r="C25" s="28" t="str">
+      <c r="C25" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D25)),CONCATENATE("celex_classif:class_",D25),""  )</f>
         <v/>
       </c>
@@ -48374,10 +48361,10 @@
       <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.19140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.1953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="61.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="61.23"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -48514,7 +48501,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="28" t="s">
+      <c r="A18" s="21" t="s">
         <v>2245</v>
       </c>
       <c r="B18" s="0" t="s">
@@ -48546,7 +48533,7 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="28" t="s">
+      <c r="A22" s="21" t="s">
         <v>2251</v>
       </c>
       <c r="B22" s="0" t="s">
@@ -48832,7 +48819,7 @@
       <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.19140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.1953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="80.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.28"/>

</xml_diff>

<commit_message>
fixed CELEX classes in the Excel file
</commit_message>
<xml_diff>
--- a/resources/input_workbook/LAM_metadata_20200903_JKU.xlsx
+++ b/resources/input_workbook/LAM_metadata_20200903_JKU.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="LAM properties" sheetId="1" state="visible" r:id="rId2"/>
@@ -19353,7 +19353,7 @@
     <numFmt numFmtId="166" formatCode="[$-809]dd/mm/yyyy"/>
     <numFmt numFmtId="167" formatCode="0.00E+00"/>
   </numFmts>
-  <fonts count="33">
+  <fonts count="32">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -19578,12 +19578,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -19678,7 +19672,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -19791,10 +19785,6 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -19892,9 +19882,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>219600</xdr:colOff>
+      <xdr:colOff>219240</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>669240</xdr:rowOff>
+      <xdr:rowOff>668880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -19904,7 +19894,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="7830000" cy="8163360"/>
+          <a:ext cx="7829640" cy="8163000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -19937,9 +19927,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
-      <xdr:colOff>636840</xdr:colOff>
+      <xdr:colOff>636480</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>2036880</xdr:rowOff>
+      <xdr:rowOff>2036520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -19949,7 +19939,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="10038960" cy="9531000"/>
+          <a:ext cx="10038600" cy="9530640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -19987,9 +19977,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>453600</xdr:colOff>
+      <xdr:colOff>453240</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>173160</xdr:rowOff>
+      <xdr:rowOff>172800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -19999,7 +19989,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="17856360" cy="4627440"/>
+          <a:ext cx="17857080" cy="4627080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -20038,7 +20028,7 @@
   </sheetPr>
   <dimension ref="A1:AK118"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="AJ2" activeCellId="0" sqref="AJ2"/>
@@ -28071,10 +28061,10 @@
   <dimension ref="A1:J49"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
+      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.19140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.2109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.7"/>
@@ -36596,13 +36586,13 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="25"/>
@@ -36644,7 +36634,7 @@
       <c r="B2" s="5" t="s">
         <v>1326</v>
       </c>
-      <c r="C2" s="28" t="str">
+      <c r="C2" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D2)),CONCATENATE("class_classif:class_",D2),""  )</f>
         <v/>
       </c>
@@ -36668,7 +36658,7 @@
       <c r="B3" s="5" t="s">
         <v>996</v>
       </c>
-      <c r="C3" s="28" t="str">
+      <c r="C3" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D3)),CONCATENATE("class_classif:class_",D3),""  )</f>
         <v/>
       </c>
@@ -36692,7 +36682,7 @@
       <c r="B4" s="5" t="s">
         <v>1147</v>
       </c>
-      <c r="C4" s="28" t="str">
+      <c r="C4" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D4)),CONCATENATE("class_classif:class_",D4),""  )</f>
         <v/>
       </c>
@@ -36716,7 +36706,7 @@
       <c r="B5" s="5" t="s">
         <v>1333</v>
       </c>
-      <c r="C5" s="28" t="str">
+      <c r="C5" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D5)),CONCATENATE("class_classif:class_",D5),""  )</f>
         <v>class_classif:class_LEGAL</v>
       </c>
@@ -36742,7 +36732,7 @@
       <c r="B6" s="5" t="s">
         <v>1251</v>
       </c>
-      <c r="C6" s="28" t="str">
+      <c r="C6" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D6)),CONCATENATE("class_classif:class_",D6),""  )</f>
         <v>class_classif:class_LEGAL</v>
       </c>
@@ -36768,7 +36758,7 @@
       <c r="B7" s="5" t="s">
         <v>1148</v>
       </c>
-      <c r="C7" s="28" t="str">
+      <c r="C7" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D7)),CONCATENATE("class_classif:class_",D7),""  )</f>
         <v>class_classif:class_LEGAL</v>
       </c>
@@ -36794,7 +36784,7 @@
       <c r="B8" s="0" t="s">
         <v>839</v>
       </c>
-      <c r="C8" s="28" t="str">
+      <c r="C8" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D8)),CONCATENATE("class_classif:class_",D8),""  )</f>
         <v/>
       </c>
@@ -36816,7 +36806,7 @@
       <c r="B9" s="0" t="s">
         <v>840</v>
       </c>
-      <c r="C9" s="28" t="str">
+      <c r="C9" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D9)),CONCATENATE("class_classif:class_",D9),""  )</f>
         <v>class_classif:class_PREPDOC</v>
       </c>
@@ -36841,7 +36831,7 @@
       <c r="B10" s="0" t="s">
         <v>914</v>
       </c>
-      <c r="C10" s="28" t="str">
+      <c r="C10" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D10)),CONCATENATE("class_classif:class_",D10),""  )</f>
         <v>class_classif:class_PREPDOC</v>
       </c>
@@ -36866,7 +36856,7 @@
       <c r="B11" s="0" t="s">
         <v>1346</v>
       </c>
-      <c r="C11" s="28" t="str">
+      <c r="C11" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D11)),CONCATENATE("class_classif:class_",D11),""  )</f>
         <v>class_classif:class_PREPDOC</v>
       </c>
@@ -36891,7 +36881,7 @@
       <c r="B12" s="0" t="s">
         <v>874</v>
       </c>
-      <c r="C12" s="28" t="str">
+      <c r="C12" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D12)),CONCATENATE("class_classif:class_",D12),""  )</f>
         <v>class_classif:class_PREPDOC</v>
       </c>
@@ -36916,7 +36906,7 @@
       <c r="B13" s="0" t="s">
         <v>1351</v>
       </c>
-      <c r="C13" s="28" t="str">
+      <c r="C13" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D13)),CONCATENATE("class_classif:class_",D13),""  )</f>
         <v>class_classif:class_PREPDOC</v>
       </c>
@@ -36941,7 +36931,7 @@
       <c r="B14" s="0" t="s">
         <v>1354</v>
       </c>
-      <c r="C14" s="28" t="str">
+      <c r="C14" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D14)),CONCATENATE("class_classif:class_",D14),""  )</f>
         <v>class_classif:class_PREPDOC</v>
       </c>
@@ -36966,7 +36956,7 @@
       <c r="B15" s="0" t="s">
         <v>1176</v>
       </c>
-      <c r="C15" s="28" t="str">
+      <c r="C15" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D15)),CONCATENATE("class_classif:class_",D15),""  )</f>
         <v>class_classif:class_PREPDOC</v>
       </c>
@@ -36991,7 +36981,7 @@
       <c r="B16" s="0" t="s">
         <v>973</v>
       </c>
-      <c r="C16" s="28" t="str">
+      <c r="C16" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D16)),CONCATENATE("class_classif:class_",D16),""  )</f>
         <v/>
       </c>
@@ -37013,7 +37003,7 @@
       <c r="B17" s="0" t="s">
         <v>1037</v>
       </c>
-      <c r="C17" s="28" t="str">
+      <c r="C17" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D17)),CONCATENATE("class_classif:class_",D17),""  )</f>
         <v/>
       </c>
@@ -37035,7 +37025,7 @@
       <c r="B18" s="0" t="s">
         <v>1022</v>
       </c>
-      <c r="C18" s="28" t="str">
+      <c r="C18" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D18)),CONCATENATE("class_classif:class_",D18),""  )</f>
         <v/>
       </c>
@@ -37057,7 +37047,7 @@
       <c r="B19" s="0" t="s">
         <v>1023</v>
       </c>
-      <c r="C19" s="28" t="str">
+      <c r="C19" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D19)),CONCATENATE("class_classif:class_",D19),""  )</f>
         <v>class_classif:class_CDOC</v>
       </c>
@@ -37082,7 +37072,7 @@
       <c r="B20" s="0" t="s">
         <v>1208</v>
       </c>
-      <c r="C20" s="28" t="str">
+      <c r="C20" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D20)),CONCATENATE("class_classif:class_",D20),""  )</f>
         <v>class_classif:class_CDOC</v>
       </c>
@@ -37104,7 +37094,7 @@
       <c r="B21" s="0" t="s">
         <v>1318</v>
       </c>
-      <c r="C21" s="28" t="str">
+      <c r="C21" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D21)),CONCATENATE("class_classif:class_",D21),""  )</f>
         <v>class_classif:class_CDOC</v>
       </c>
@@ -37129,7 +37119,7 @@
       <c r="B22" s="0" t="s">
         <v>1118</v>
       </c>
-      <c r="C22" s="28" t="str">
+      <c r="C22" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D22)),CONCATENATE("class_classif:class_",D22),""  )</f>
         <v>class_classif:class_CDOC</v>
       </c>
@@ -37161,10 +37151,10 @@
   </sheetPr>
   <dimension ref="A1:O276"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
+      <selection pane="bottomLeft" activeCell="N3" activeCellId="0" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="1"/>
@@ -37256,8 +37246,8 @@
         <v>0</v>
       </c>
       <c r="O2" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M2)</f>
-        <v>celexd:clc_0</v>
+        <f aca="false">CONCATENATE("celexd:class_",M2)</f>
+        <v>celexd:class_0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37282,8 +37272,8 @@
         <v>1</v>
       </c>
       <c r="O3" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M3)</f>
-        <v>celexd:clc_1</v>
+        <f aca="false">CONCATENATE("celexd:class_",M3)</f>
+        <v>celexd:class_1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37308,8 +37298,8 @@
         <v>2</v>
       </c>
       <c r="O4" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M4)</f>
-        <v>celexd:clc_2</v>
+        <f aca="false">CONCATENATE("celexd:class_",M4)</f>
+        <v>celexd:class_2</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37334,8 +37324,8 @@
         <v>3</v>
       </c>
       <c r="O5" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M5)</f>
-        <v>celexd:clc_3</v>
+        <f aca="false">CONCATENATE("celexd:class_",M5)</f>
+        <v>celexd:class_3</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37360,8 +37350,8 @@
         <v>4</v>
       </c>
       <c r="O6" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M6)</f>
-        <v>celexd:clc_4</v>
+        <f aca="false">CONCATENATE("celexd:class_",M6)</f>
+        <v>celexd:class_4</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37386,8 +37376,8 @@
         <v>5</v>
       </c>
       <c r="O7" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M7)</f>
-        <v>celexd:clc_5</v>
+        <f aca="false">CONCATENATE("celexd:class_",M7)</f>
+        <v>celexd:class_5</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37412,8 +37402,8 @@
         <v>6</v>
       </c>
       <c r="O8" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M8)</f>
-        <v>celexd:clc_6</v>
+        <f aca="false">CONCATENATE("celexd:class_",M8)</f>
+        <v>celexd:class_6</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37444,8 +37434,8 @@
         <v>7</v>
       </c>
       <c r="O9" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M9)</f>
-        <v>celexd:clc_7</v>
+        <f aca="false">CONCATENATE("celexd:class_",M9)</f>
+        <v>celexd:class_7</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37473,8 +37463,8 @@
         <v>8</v>
       </c>
       <c r="O10" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M10)</f>
-        <v>celexd:clc_8</v>
+        <f aca="false">CONCATENATE("celexd:class_",M10)</f>
+        <v>celexd:class_8</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37499,8 +37489,8 @@
         <v>9</v>
       </c>
       <c r="O11" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M11)</f>
-        <v>celexd:clc_9</v>
+        <f aca="false">CONCATENATE("celexd:class_",M11)</f>
+        <v>celexd:class_9</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37537,8 +37527,8 @@
         <v>1</v>
       </c>
       <c r="O12" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M12)</f>
-        <v>celexd:clc_1</v>
+        <f aca="false">CONCATENATE("celexd:class_",M12)</f>
+        <v>celexd:class_1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37575,8 +37565,8 @@
         <v>1</v>
       </c>
       <c r="O13" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M13)</f>
-        <v>celexd:clc_1</v>
+        <f aca="false">CONCATENATE("celexd:class_",M13)</f>
+        <v>celexd:class_1</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="314.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37619,8 +37609,8 @@
         <v>1</v>
       </c>
       <c r="O14" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M14)</f>
-        <v>celexd:clc_1</v>
+        <f aca="false">CONCATENATE("celexd:class_",M14)</f>
+        <v>celexd:class_1</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37657,8 +37647,8 @@
         <v>1</v>
       </c>
       <c r="O15" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M15)</f>
-        <v>celexd:clc_1</v>
+        <f aca="false">CONCATENATE("celexd:class_",M15)</f>
+        <v>celexd:class_1</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37695,8 +37685,8 @@
         <v>1</v>
       </c>
       <c r="O16" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M16)</f>
-        <v>celexd:clc_1</v>
+        <f aca="false">CONCATENATE("celexd:class_",M16)</f>
+        <v>celexd:class_1</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37730,8 +37720,8 @@
         <v>2</v>
       </c>
       <c r="O17" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M17)</f>
-        <v>celexd:clc_2</v>
+        <f aca="false">CONCATENATE("celexd:class_",M17)</f>
+        <v>celexd:class_2</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37776,8 +37766,8 @@
         <v>2</v>
       </c>
       <c r="O18" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M18)</f>
-        <v>celexd:clc_2</v>
+        <f aca="false">CONCATENATE("celexd:class_",M18)</f>
+        <v>celexd:class_2</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37819,8 +37809,8 @@
         <v>2</v>
       </c>
       <c r="O19" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M19)</f>
-        <v>celexd:clc_2</v>
+        <f aca="false">CONCATENATE("celexd:class_",M19)</f>
+        <v>celexd:class_2</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37854,8 +37844,8 @@
         <v>2</v>
       </c>
       <c r="O20" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M20)</f>
-        <v>celexd:clc_2</v>
+        <f aca="false">CONCATENATE("celexd:class_",M20)</f>
+        <v>celexd:class_2</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37898,8 +37888,8 @@
         <v>2</v>
       </c>
       <c r="O21" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M21)</f>
-        <v>celexd:clc_2</v>
+        <f aca="false">CONCATENATE("celexd:class_",M21)</f>
+        <v>celexd:class_2</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37942,8 +37932,8 @@
         <v>2</v>
       </c>
       <c r="O22" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M22)</f>
-        <v>celexd:clc_2</v>
+        <f aca="false">CONCATENATE("celexd:class_",M22)</f>
+        <v>celexd:class_2</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37977,8 +37967,8 @@
         <v>2</v>
       </c>
       <c r="O23" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M23)</f>
-        <v>celexd:clc_2</v>
+        <f aca="false">CONCATENATE("celexd:class_",M23)</f>
+        <v>celexd:class_2</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38021,8 +38011,8 @@
         <v>2</v>
       </c>
       <c r="O24" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M24)</f>
-        <v>celexd:clc_2</v>
+        <f aca="false">CONCATENATE("celexd:class_",M24)</f>
+        <v>celexd:class_2</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38056,8 +38046,8 @@
         <v>2</v>
       </c>
       <c r="O25" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M25)</f>
-        <v>celexd:clc_2</v>
+        <f aca="false">CONCATENATE("celexd:class_",M25)</f>
+        <v>celexd:class_2</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38100,8 +38090,8 @@
         <v>2</v>
       </c>
       <c r="O26" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M26)</f>
-        <v>celexd:clc_2</v>
+        <f aca="false">CONCATENATE("celexd:class_",M26)</f>
+        <v>celexd:class_2</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38144,8 +38134,8 @@
         <v>2</v>
       </c>
       <c r="O27" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M27)</f>
-        <v>celexd:clc_2</v>
+        <f aca="false">CONCATENATE("celexd:class_",M27)</f>
+        <v>celexd:class_2</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38176,8 +38166,8 @@
         <v>3</v>
       </c>
       <c r="O28" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M28)</f>
-        <v>celexd:clc_3</v>
+        <f aca="false">CONCATENATE("celexd:class_",M28)</f>
+        <v>celexd:class_3</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38223,8 +38213,8 @@
         <v>3</v>
       </c>
       <c r="O29" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M29)</f>
-        <v>celexd:clc_3</v>
+        <f aca="false">CONCATENATE("celexd:class_",M29)</f>
+        <v>celexd:class_3</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38261,8 +38251,8 @@
         <v>3</v>
       </c>
       <c r="O30" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M30)</f>
-        <v>celexd:clc_3</v>
+        <f aca="false">CONCATENATE("celexd:class_",M30)</f>
+        <v>celexd:class_3</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38293,8 +38283,8 @@
         <v>3</v>
       </c>
       <c r="O31" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M31)</f>
-        <v>celexd:clc_3</v>
+        <f aca="false">CONCATENATE("celexd:class_",M31)</f>
+        <v>celexd:class_3</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38337,8 +38327,8 @@
         <v>3</v>
       </c>
       <c r="O32" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M32)</f>
-        <v>celexd:clc_3</v>
+        <f aca="false">CONCATENATE("celexd:class_",M32)</f>
+        <v>celexd:class_3</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38378,8 +38368,8 @@
         <v>3</v>
       </c>
       <c r="O33" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M33)</f>
-        <v>celexd:clc_3</v>
+        <f aca="false">CONCATENATE("celexd:class_",M33)</f>
+        <v>celexd:class_3</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38410,8 +38400,8 @@
         <v>3</v>
       </c>
       <c r="O34" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M34)</f>
-        <v>celexd:clc_3</v>
+        <f aca="false">CONCATENATE("celexd:class_",M34)</f>
+        <v>celexd:class_3</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38454,8 +38444,8 @@
         <v>3</v>
       </c>
       <c r="O35" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M35)</f>
-        <v>celexd:clc_3</v>
+        <f aca="false">CONCATENATE("celexd:class_",M35)</f>
+        <v>celexd:class_3</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38501,8 +38491,8 @@
         <v>3</v>
       </c>
       <c r="O36" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M36)</f>
-        <v>celexd:clc_3</v>
+        <f aca="false">CONCATENATE("celexd:class_",M36)</f>
+        <v>celexd:class_3</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38536,8 +38526,8 @@
         <v>3</v>
       </c>
       <c r="O37" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M37)</f>
-        <v>celexd:clc_3</v>
+        <f aca="false">CONCATENATE("celexd:class_",M37)</f>
+        <v>celexd:class_3</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38580,8 +38570,8 @@
         <v>3</v>
       </c>
       <c r="O38" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M38)</f>
-        <v>celexd:clc_3</v>
+        <f aca="false">CONCATENATE("celexd:class_",M38)</f>
+        <v>celexd:class_3</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38624,8 +38614,8 @@
         <v>3</v>
       </c>
       <c r="O39" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M39)</f>
-        <v>celexd:clc_3</v>
+        <f aca="false">CONCATENATE("celexd:class_",M39)</f>
+        <v>celexd:class_3</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38659,8 +38649,8 @@
         <v>3</v>
       </c>
       <c r="O40" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M40)</f>
-        <v>celexd:clc_3</v>
+        <f aca="false">CONCATENATE("celexd:class_",M40)</f>
+        <v>celexd:class_3</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38681,7 +38671,7 @@
       <c r="E41" s="2" t="s">
         <v>1488</v>
       </c>
-      <c r="F41" s="29" t="s">
+      <c r="F41" s="28" t="s">
         <v>1489</v>
       </c>
       <c r="H41" s="2" t="n">
@@ -38700,8 +38690,8 @@
         <v>3</v>
       </c>
       <c r="O41" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M41)</f>
-        <v>celexd:clc_3</v>
+        <f aca="false">CONCATENATE("celexd:class_",M41)</f>
+        <v>celexd:class_3</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38735,8 +38725,8 @@
         <v>3</v>
       </c>
       <c r="O42" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M42)</f>
-        <v>celexd:clc_3</v>
+        <f aca="false">CONCATENATE("celexd:class_",M42)</f>
+        <v>celexd:class_3</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38776,8 +38766,8 @@
         <v>3</v>
       </c>
       <c r="O43" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M43)</f>
-        <v>celexd:clc_3</v>
+        <f aca="false">CONCATENATE("celexd:class_",M43)</f>
+        <v>celexd:class_3</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38817,8 +38807,8 @@
         <v>3</v>
       </c>
       <c r="O44" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M44)</f>
-        <v>celexd:clc_3</v>
+        <f aca="false">CONCATENATE("celexd:class_",M44)</f>
+        <v>celexd:class_3</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38852,8 +38842,8 @@
         <v>3</v>
       </c>
       <c r="O45" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M45)</f>
-        <v>celexd:clc_3</v>
+        <f aca="false">CONCATENATE("celexd:class_",M45)</f>
+        <v>celexd:class_3</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38896,8 +38886,8 @@
         <v>3</v>
       </c>
       <c r="O46" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M46)</f>
-        <v>celexd:clc_3</v>
+        <f aca="false">CONCATENATE("celexd:class_",M46)</f>
+        <v>celexd:class_3</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38940,8 +38930,8 @@
         <v>3</v>
       </c>
       <c r="O47" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M47)</f>
-        <v>celexd:clc_3</v>
+        <f aca="false">CONCATENATE("celexd:class_",M47)</f>
+        <v>celexd:class_3</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38972,8 +38962,8 @@
         <v>3</v>
       </c>
       <c r="O48" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M48)</f>
-        <v>celexd:clc_3</v>
+        <f aca="false">CONCATENATE("celexd:class_",M48)</f>
+        <v>celexd:class_3</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39016,8 +39006,8 @@
         <v>3</v>
       </c>
       <c r="O49" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M49)</f>
-        <v>celexd:clc_3</v>
+        <f aca="false">CONCATENATE("celexd:class_",M49)</f>
+        <v>celexd:class_3</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39060,8 +39050,8 @@
         <v>3</v>
       </c>
       <c r="O50" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M50)</f>
-        <v>celexd:clc_3</v>
+        <f aca="false">CONCATENATE("celexd:class_",M50)</f>
+        <v>celexd:class_3</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39092,8 +39082,8 @@
         <v>3</v>
       </c>
       <c r="O51" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M51)</f>
-        <v>celexd:clc_3</v>
+        <f aca="false">CONCATENATE("celexd:class_",M51)</f>
+        <v>celexd:class_3</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39136,8 +39126,8 @@
         <v>3</v>
       </c>
       <c r="O52" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M52)</f>
-        <v>celexd:clc_3</v>
+        <f aca="false">CONCATENATE("celexd:class_",M52)</f>
+        <v>celexd:class_3</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39171,8 +39161,8 @@
         <v>3</v>
       </c>
       <c r="O53" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M53)</f>
-        <v>celexd:clc_3</v>
+        <f aca="false">CONCATENATE("celexd:class_",M53)</f>
+        <v>celexd:class_3</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39215,8 +39205,8 @@
         <v>3</v>
       </c>
       <c r="O54" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M54)</f>
-        <v>celexd:clc_3</v>
+        <f aca="false">CONCATENATE("celexd:class_",M54)</f>
+        <v>celexd:class_3</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39247,8 +39237,8 @@
         <v>3</v>
       </c>
       <c r="O55" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M55)</f>
-        <v>celexd:clc_3</v>
+        <f aca="false">CONCATENATE("celexd:class_",M55)</f>
+        <v>celexd:class_3</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39291,8 +39281,8 @@
         <v>3</v>
       </c>
       <c r="O56" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M56)</f>
-        <v>celexd:clc_3</v>
+        <f aca="false">CONCATENATE("celexd:class_",M56)</f>
+        <v>celexd:class_3</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39323,8 +39313,8 @@
         <v>3</v>
       </c>
       <c r="O57" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M57)</f>
-        <v>celexd:clc_3</v>
+        <f aca="false">CONCATENATE("celexd:class_",M57)</f>
+        <v>celexd:class_3</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39370,8 +39360,8 @@
         <v>3</v>
       </c>
       <c r="O58" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M58)</f>
-        <v>celexd:clc_3</v>
+        <f aca="false">CONCATENATE("celexd:class_",M58)</f>
+        <v>celexd:class_3</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39402,8 +39392,8 @@
         <v>3</v>
       </c>
       <c r="O59" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M59)</f>
-        <v>celexd:clc_3</v>
+        <f aca="false">CONCATENATE("celexd:class_",M59)</f>
+        <v>celexd:class_3</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39446,8 +39436,8 @@
         <v>3</v>
       </c>
       <c r="O60" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M60)</f>
-        <v>celexd:clc_3</v>
+        <f aca="false">CONCATENATE("celexd:class_",M60)</f>
+        <v>celexd:class_3</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39490,8 +39480,8 @@
         <v>3</v>
       </c>
       <c r="O61" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M61)</f>
-        <v>celexd:clc_3</v>
+        <f aca="false">CONCATENATE("celexd:class_",M61)</f>
+        <v>celexd:class_3</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39522,8 +39512,8 @@
         <v>3</v>
       </c>
       <c r="O62" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M62)</f>
-        <v>celexd:clc_3</v>
+        <f aca="false">CONCATENATE("celexd:class_",M62)</f>
+        <v>celexd:class_3</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39566,8 +39556,8 @@
         <v>3</v>
       </c>
       <c r="O63" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M63)</f>
-        <v>celexd:clc_3</v>
+        <f aca="false">CONCATENATE("celexd:class_",M63)</f>
+        <v>celexd:class_3</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39610,8 +39600,8 @@
         <v>3</v>
       </c>
       <c r="O64" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M64)</f>
-        <v>celexd:clc_3</v>
+        <f aca="false">CONCATENATE("celexd:class_",M64)</f>
+        <v>celexd:class_3</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39642,8 +39632,8 @@
         <v>3</v>
       </c>
       <c r="O65" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M65)</f>
-        <v>celexd:clc_3</v>
+        <f aca="false">CONCATENATE("celexd:class_",M65)</f>
+        <v>celexd:class_3</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39686,8 +39676,8 @@
         <v>3</v>
       </c>
       <c r="O66" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M66)</f>
-        <v>celexd:clc_3</v>
+        <f aca="false">CONCATENATE("celexd:class_",M66)</f>
+        <v>celexd:class_3</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39730,8 +39720,8 @@
         <v>3</v>
       </c>
       <c r="O67" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M67)</f>
-        <v>celexd:clc_3</v>
+        <f aca="false">CONCATENATE("celexd:class_",M67)</f>
+        <v>celexd:class_3</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39765,8 +39755,8 @@
         <v>3</v>
       </c>
       <c r="O68" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M68)</f>
-        <v>celexd:clc_3</v>
+        <f aca="false">CONCATENATE("celexd:class_",M68)</f>
+        <v>celexd:class_3</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39809,8 +39799,8 @@
         <v>3</v>
       </c>
       <c r="O69" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M69)</f>
-        <v>celexd:clc_3</v>
+        <f aca="false">CONCATENATE("celexd:class_",M69)</f>
+        <v>celexd:class_3</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39841,8 +39831,8 @@
         <v>3</v>
       </c>
       <c r="O70" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M70)</f>
-        <v>celexd:clc_3</v>
+        <f aca="false">CONCATENATE("celexd:class_",M70)</f>
+        <v>celexd:class_3</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39888,8 +39878,8 @@
         <v>3</v>
       </c>
       <c r="O71" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M71)</f>
-        <v>celexd:clc_3</v>
+        <f aca="false">CONCATENATE("celexd:class_",M71)</f>
+        <v>celexd:class_3</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39920,8 +39910,8 @@
         <v>3</v>
       </c>
       <c r="O72" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M72)</f>
-        <v>celexd:clc_3</v>
+        <f aca="false">CONCATENATE("celexd:class_",M72)</f>
+        <v>celexd:class_3</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39964,8 +39954,8 @@
         <v>3</v>
       </c>
       <c r="O73" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M73)</f>
-        <v>celexd:clc_3</v>
+        <f aca="false">CONCATENATE("celexd:class_",M73)</f>
+        <v>celexd:class_3</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39999,8 +39989,8 @@
         <v>4</v>
       </c>
       <c r="O74" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M74)</f>
-        <v>celexd:clc_4</v>
+        <f aca="false">CONCATENATE("celexd:class_",M74)</f>
+        <v>celexd:class_4</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -40043,8 +40033,8 @@
         <v>4</v>
       </c>
       <c r="O75" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M75)</f>
-        <v>celexd:clc_4</v>
+        <f aca="false">CONCATENATE("celexd:class_",M75)</f>
+        <v>celexd:class_4</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -40087,8 +40077,8 @@
         <v>4</v>
       </c>
       <c r="O76" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M76)</f>
-        <v>celexd:clc_4</v>
+        <f aca="false">CONCATENATE("celexd:class_",M76)</f>
+        <v>celexd:class_4</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -40119,8 +40109,8 @@
         <v>4</v>
       </c>
       <c r="O77" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M77)</f>
-        <v>celexd:clc_4</v>
+        <f aca="false">CONCATENATE("celexd:class_",M77)</f>
+        <v>celexd:class_4</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -40163,8 +40153,8 @@
         <v>4</v>
       </c>
       <c r="O78" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M78)</f>
-        <v>celexd:clc_4</v>
+        <f aca="false">CONCATENATE("celexd:class_",M78)</f>
+        <v>celexd:class_4</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -40207,8 +40197,8 @@
         <v>4</v>
       </c>
       <c r="O79" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M79)</f>
-        <v>celexd:clc_4</v>
+        <f aca="false">CONCATENATE("celexd:class_",M79)</f>
+        <v>celexd:class_4</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -40242,8 +40232,8 @@
         <v>4</v>
       </c>
       <c r="O80" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M80)</f>
-        <v>celexd:clc_4</v>
+        <f aca="false">CONCATENATE("celexd:class_",M80)</f>
+        <v>celexd:class_4</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -40289,8 +40279,8 @@
         <v>4</v>
       </c>
       <c r="O81" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M81)</f>
-        <v>celexd:clc_4</v>
+        <f aca="false">CONCATENATE("celexd:class_",M81)</f>
+        <v>celexd:class_4</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -40321,8 +40311,8 @@
         <v>4</v>
       </c>
       <c r="O82" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M82)</f>
-        <v>celexd:clc_4</v>
+        <f aca="false">CONCATENATE("celexd:class_",M82)</f>
+        <v>celexd:class_4</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -40365,11 +40355,11 @@
         <v>4</v>
       </c>
       <c r="O83" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M83)</f>
-        <v>celexd:clc_4</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">CONCATENATE("celexd:class_",M83)</f>
+        <v>celexd:class_4</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="2" t="str">
         <f aca="false">CONCATENATE("celexd:c_",B84)</f>
         <v>celexd:c_5_AA</v>
@@ -40400,8 +40390,8 @@
         <v>5</v>
       </c>
       <c r="O84" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M84)</f>
-        <v>celexd:clc_5_ECA</v>
+        <f aca="false">CONCATENATE("celexd:class_",M84)</f>
+        <v>celexd:class_5_ECA</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -40444,11 +40434,11 @@
         <v>5</v>
       </c>
       <c r="O85" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M85)</f>
-        <v>celexd:clc_5_ECA</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">CONCATENATE("celexd:class_",M85)</f>
+        <v>celexd:class_5_ECA</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="2" t="str">
         <f aca="false">CONCATENATE("celexd:c_",B86)</f>
         <v>celexd:c_5_AB</v>
@@ -40479,8 +40469,8 @@
         <v>5</v>
       </c>
       <c r="O86" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M86)</f>
-        <v>celexd:clc_5_ECB</v>
+        <f aca="false">CONCATENATE("celexd:class_",M86)</f>
+        <v>celexd:class_5_ECB</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -40523,8 +40513,8 @@
         <v>5</v>
       </c>
       <c r="O87" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M87)</f>
-        <v>celexd:clc_5_ECB</v>
+        <f aca="false">CONCATENATE("celexd:class_",M87)</f>
+        <v>celexd:class_5_ECB</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -40558,8 +40548,8 @@
         <v>5</v>
       </c>
       <c r="O88" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M88)</f>
-        <v>celexd:clc_5_EESC</v>
+        <f aca="false">CONCATENATE("celexd:class_",M88)</f>
+        <v>celexd:class_5_EESC</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -40605,8 +40595,8 @@
         <v>5</v>
       </c>
       <c r="O89" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M89)</f>
-        <v>celexd:clc_5_EESC</v>
+        <f aca="false">CONCATENATE("celexd:class_",M89)</f>
+        <v>celexd:class_5_EESC</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -40640,8 +40630,8 @@
         <v>5</v>
       </c>
       <c r="O90" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M90)</f>
-        <v>celexd:clc_5_EESC</v>
+        <f aca="false">CONCATENATE("celexd:class_",M90)</f>
+        <v>celexd:class_5_EESC</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -40687,8 +40677,8 @@
         <v>5</v>
       </c>
       <c r="O91" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M91)</f>
-        <v>celexd:clc_5_EESC</v>
+        <f aca="false">CONCATENATE("celexd:class_",M91)</f>
+        <v>celexd:class_5_EESC</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -40725,8 +40715,8 @@
         <v>5</v>
       </c>
       <c r="O92" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M92)</f>
-        <v>celexd:clc_5_CONSIL</v>
+        <f aca="false">CONCATENATE("celexd:class_",M92)</f>
+        <v>celexd:class_5_CONSIL</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -40772,11 +40762,11 @@
         <v>5</v>
       </c>
       <c r="O93" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M93)</f>
-        <v>celexd:clc_5_CONSIL</v>
-      </c>
-    </row>
-    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">CONCATENATE("celexd:class_",M93)</f>
+        <v>celexd:class_5_CONSIL</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="2" t="str">
         <f aca="false">CONCATENATE("celexd:c_",B94)</f>
         <v>celexd:c_5_AK</v>
@@ -40807,8 +40797,8 @@
         <v>5</v>
       </c>
       <c r="O94" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M94)</f>
-        <v>celexd:clc_5_ECSC</v>
+        <f aca="false">CONCATENATE("celexd:class_",M94)</f>
+        <v>celexd:class_5_ECSC</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -40851,8 +40841,8 @@
         <v>5</v>
       </c>
       <c r="O95" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M95)</f>
-        <v>celexd:clc_5_ECSC</v>
+        <f aca="false">CONCATENATE("celexd:class_",M95)</f>
+        <v>celexd:class_5_ECSC</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -40886,8 +40876,8 @@
         <v>5</v>
       </c>
       <c r="O96" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M96)</f>
-        <v>celexd:clc_5_EP</v>
+        <f aca="false">CONCATENATE("celexd:class_",M96)</f>
+        <v>celexd:class_5_EP</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -40933,8 +40923,8 @@
         <v>5</v>
       </c>
       <c r="O97" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M97)</f>
-        <v>celexd:clc_5_EP</v>
+        <f aca="false">CONCATENATE("celexd:class_",M97)</f>
+        <v>celexd:class_5_EP</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -40980,8 +40970,8 @@
         <v>5</v>
       </c>
       <c r="O98" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M98)</f>
-        <v>celexd:clc_5_EP</v>
+        <f aca="false">CONCATENATE("celexd:class_",M98)</f>
+        <v>celexd:class_5_EP</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41018,8 +41008,8 @@
         <v>5</v>
       </c>
       <c r="O99" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M99)</f>
-        <v>celexd:clc_5_COR</v>
+        <f aca="false">CONCATENATE("celexd:class_",M99)</f>
+        <v>celexd:class_5_COR</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41062,8 +41052,8 @@
         <v>5</v>
       </c>
       <c r="O100" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M100)</f>
-        <v>celexd:clc_5_COR</v>
+        <f aca="false">CONCATENATE("celexd:class_",M100)</f>
+        <v>celexd:class_5_COR</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="782.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41100,8 +41090,8 @@
         <v>5</v>
       </c>
       <c r="O101" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M101)</f>
-        <v>celexd:clc_5_OTHER</v>
+        <f aca="false">CONCATENATE("celexd:class_",M101)</f>
+        <v>celexd:class_5_OTHER</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41144,8 +41134,8 @@
         <v>5</v>
       </c>
       <c r="O102" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M102)</f>
-        <v>celexd:clc_5_OTHER</v>
+        <f aca="false">CONCATENATE("celexd:class_",M102)</f>
+        <v>celexd:class_5_OTHER</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41182,8 +41172,8 @@
         <v>5</v>
       </c>
       <c r="O103" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M103)</f>
-        <v>celexd:clc_5_OTHER</v>
+        <f aca="false">CONCATENATE("celexd:class_",M103)</f>
+        <v>celexd:class_5_OTHER</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41226,8 +41216,8 @@
         <v>5</v>
       </c>
       <c r="O104" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M104)</f>
-        <v>celexd:clc_5_OTHER</v>
+        <f aca="false">CONCATENATE("celexd:class_",M104)</f>
+        <v>celexd:class_5_OTHER</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41261,8 +41251,8 @@
         <v>5</v>
       </c>
       <c r="O105" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M105)</f>
-        <v>celexd:clc_5_EP</v>
+        <f aca="false">CONCATENATE("celexd:class_",M105)</f>
+        <v>celexd:class_5_EP</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41305,8 +41295,8 @@
         <v>5</v>
       </c>
       <c r="O106" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M106)</f>
-        <v>celexd:clc_5_EP</v>
+        <f aca="false">CONCATENATE("celexd:class_",M106)</f>
+        <v>celexd:class_5_EP</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41352,8 +41342,8 @@
         <v>5</v>
       </c>
       <c r="O107" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M107)</f>
-        <v>celexd:clc_5_EP</v>
+        <f aca="false">CONCATENATE("celexd:class_",M107)</f>
+        <v>celexd:class_5_EP</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41387,8 +41377,8 @@
         <v>5</v>
       </c>
       <c r="O108" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M108)</f>
-        <v>celexd:clc_5_COM</v>
+        <f aca="false">CONCATENATE("celexd:class_",M108)</f>
+        <v>celexd:class_5_COM</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41431,8 +41421,8 @@
         <v>5</v>
       </c>
       <c r="O109" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M109)</f>
-        <v>celexd:clc_5_COM</v>
+        <f aca="false">CONCATENATE("celexd:class_",M109)</f>
+        <v>celexd:class_5_COM</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41469,8 +41459,8 @@
         <v>5</v>
       </c>
       <c r="O110" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M110)</f>
-        <v>celexd:clc_5_COM</v>
+        <f aca="false">CONCATENATE("celexd:class_",M110)</f>
+        <v>celexd:class_5_COM</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41504,8 +41494,8 @@
         <v>5</v>
       </c>
       <c r="O111" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M111)</f>
-        <v>celexd:clc_5_EP</v>
+        <f aca="false">CONCATENATE("celexd:class_",M111)</f>
+        <v>celexd:class_5_EP</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41548,11 +41538,11 @@
         <v>5</v>
       </c>
       <c r="O112" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M112)</f>
-        <v>celexd:clc_5_EP</v>
-      </c>
-    </row>
-    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">CONCATENATE("celexd:class_",M112)</f>
+        <v>celexd:class_5_EP</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="2" t="str">
         <f aca="false">CONCATENATE("celexd:c_",B113)</f>
         <v>celexd:c_5_EC</v>
@@ -41583,8 +41573,8 @@
         <v>5</v>
       </c>
       <c r="O113" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M113)</f>
-        <v>celexd:clc_5_COM</v>
+        <f aca="false">CONCATENATE("celexd:class_",M113)</f>
+        <v>celexd:class_5_COM</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41627,11 +41617,11 @@
         <v>5</v>
       </c>
       <c r="O114" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M114)</f>
-        <v>celexd:clc_5_COM</v>
-      </c>
-    </row>
-    <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">CONCATENATE("celexd:class_",M114)</f>
+        <v>celexd:class_5_COM</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="2" t="str">
         <f aca="false">CONCATENATE("celexd:c_",B115)</f>
         <v>celexd:c_5_FC</v>
@@ -41662,8 +41652,8 @@
         <v>5</v>
       </c>
       <c r="O115" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M115)</f>
-        <v>celexd:clc_5_COM</v>
+        <f aca="false">CONCATENATE("celexd:class_",M115)</f>
+        <v>celexd:class_5_COM</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41706,11 +41696,11 @@
         <v>5</v>
       </c>
       <c r="O116" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M116)</f>
-        <v>celexd:clc_5_COM</v>
-      </c>
-    </row>
-    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">CONCATENATE("celexd:class_",M116)</f>
+        <v>celexd:class_5_COM</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="2" t="str">
         <f aca="false">CONCATENATE("celexd:c_",B117)</f>
         <v>celexd:c_5_GC</v>
@@ -41741,8 +41731,8 @@
         <v>5</v>
       </c>
       <c r="O117" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M117)</f>
-        <v>celexd:clc_5_COM</v>
+        <f aca="false">CONCATENATE("celexd:class_",M117)</f>
+        <v>celexd:class_5_COM</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41785,8 +41775,8 @@
         <v>5</v>
       </c>
       <c r="O118" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M118)</f>
-        <v>celexd:clc_5_COM</v>
+        <f aca="false">CONCATENATE("celexd:class_",M118)</f>
+        <v>celexd:class_5_COM</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41820,8 +41810,8 @@
         <v>5</v>
       </c>
       <c r="O119" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M119)</f>
-        <v>celexd:clc_5_ECB</v>
+        <f aca="false">CONCATENATE("celexd:class_",M119)</f>
+        <v>celexd:class_5_ECB</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41864,8 +41854,8 @@
         <v>5</v>
       </c>
       <c r="O120" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M120)</f>
-        <v>celexd:clc_5_ECB</v>
+        <f aca="false">CONCATENATE("celexd:class_",M120)</f>
+        <v>celexd:class_5_ECB</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41899,8 +41889,8 @@
         <v>5</v>
       </c>
       <c r="O121" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M121)</f>
-        <v>celexd:clc_5_EESC</v>
+        <f aca="false">CONCATENATE("celexd:class_",M121)</f>
+        <v>celexd:class_5_EESC</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41946,8 +41936,8 @@
         <v>5</v>
       </c>
       <c r="O122" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M122)</f>
-        <v>celexd:clc_5_EESC</v>
+        <f aca="false">CONCATENATE("celexd:class_",M122)</f>
+        <v>celexd:class_5_EESC</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41981,8 +41971,8 @@
         <v>5</v>
       </c>
       <c r="O123" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M123)</f>
-        <v>celexd:clc_5_CONSIL</v>
+        <f aca="false">CONCATENATE("celexd:class_",M123)</f>
+        <v>celexd:class_5_CONSIL</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -42025,8 +42015,8 @@
         <v>5</v>
       </c>
       <c r="O124" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M124)</f>
-        <v>celexd:clc_5_CONSIL</v>
+        <f aca="false">CONCATENATE("celexd:class_",M124)</f>
+        <v>celexd:class_5_CONSIL</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -42060,8 +42050,8 @@
         <v>5</v>
       </c>
       <c r="O125" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M125)</f>
-        <v>celexd:clc_5_EP</v>
+        <f aca="false">CONCATENATE("celexd:class_",M125)</f>
+        <v>celexd:class_5_EP</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -42104,8 +42094,8 @@
         <v>5</v>
       </c>
       <c r="O126" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M126)</f>
-        <v>celexd:clc_5_EP</v>
+        <f aca="false">CONCATENATE("celexd:class_",M126)</f>
+        <v>celexd:class_5_EP</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -42142,8 +42132,8 @@
         <v>5</v>
       </c>
       <c r="O127" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M127)</f>
-        <v>celexd:clc_5_COR</v>
+        <f aca="false">CONCATENATE("celexd:class_",M127)</f>
+        <v>celexd:class_5_COR</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -42186,11 +42176,11 @@
         <v>5</v>
       </c>
       <c r="O128" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M128)</f>
-        <v>celexd:clc_5_COR</v>
-      </c>
-    </row>
-    <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">CONCATENATE("celexd:class_",M128)</f>
+        <v>celexd:class_5_COR</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="2" t="str">
         <f aca="false">CONCATENATE("celexd:c_",B129)</f>
         <v>celexd:c_5_JC</v>
@@ -42221,8 +42211,8 @@
         <v>5</v>
       </c>
       <c r="O129" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M129)</f>
-        <v>celexd:clc_5_COM</v>
+        <f aca="false">CONCATENATE("celexd:class_",M129)</f>
+        <v>celexd:class_5_COM</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -42268,8 +42258,8 @@
         <v>5</v>
       </c>
       <c r="O130" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M130)</f>
-        <v>celexd:clc_5_COM</v>
+        <f aca="false">CONCATENATE("celexd:class_",M130)</f>
+        <v>celexd:class_5_COM</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -42306,8 +42296,8 @@
         <v>5</v>
       </c>
       <c r="O131" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M131)</f>
-        <v>celexd:clc_5_CONSIL</v>
+        <f aca="false">CONCATENATE("celexd:class_",M131)</f>
+        <v>celexd:class_5_CONSIL</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -42347,8 +42337,8 @@
         <v>5</v>
       </c>
       <c r="O132" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M132)</f>
-        <v>celexd:clc_5_CONSIL</v>
+        <f aca="false">CONCATENATE("celexd:class_",M132)</f>
+        <v>celexd:class_5_CONSIL</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -42385,8 +42375,8 @@
         <v>5</v>
       </c>
       <c r="O133" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M133)</f>
-        <v>celexd:clc_5_OTHER</v>
+        <f aca="false">CONCATENATE("celexd:class_",M133)</f>
+        <v>celexd:class_5_OTHER</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -42429,8 +42419,8 @@
         <v>5</v>
       </c>
       <c r="O134" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M134)</f>
-        <v>celexd:clc_5_OTHER</v>
+        <f aca="false">CONCATENATE("celexd:class_",M134)</f>
+        <v>celexd:class_5_OTHER</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -42473,8 +42463,8 @@
         <v>5</v>
       </c>
       <c r="O135" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M135)</f>
-        <v>celexd:clc_5_COM</v>
+        <f aca="false">CONCATENATE("celexd:class_",M135)</f>
+        <v>celexd:class_5_COM</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -42517,8 +42507,8 @@
         <v>5</v>
       </c>
       <c r="O136" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M136)</f>
-        <v>celexd:clc_5_COM</v>
+        <f aca="false">CONCATENATE("celexd:class_",M136)</f>
+        <v>celexd:class_5_COM</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -42561,8 +42551,8 @@
         <v>5</v>
       </c>
       <c r="O137" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M137)</f>
-        <v>celexd:clc_5_COM</v>
+        <f aca="false">CONCATENATE("celexd:class_",M137)</f>
+        <v>celexd:class_5_COM</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -42605,8 +42595,8 @@
         <v>5</v>
       </c>
       <c r="O138" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M138)</f>
-        <v>celexd:clc_5_ECA</v>
+        <f aca="false">CONCATENATE("celexd:class_",M138)</f>
+        <v>celexd:class_5_ECA</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -42643,8 +42633,8 @@
         <v>5</v>
       </c>
       <c r="O139" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M139)</f>
-        <v>celexd:clc_5_ECA</v>
+        <f aca="false">CONCATENATE("celexd:class_",M139)</f>
+        <v>celexd:class_5_ECA</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -42687,8 +42677,8 @@
         <v>5</v>
       </c>
       <c r="O140" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M140)</f>
-        <v>celexd:clc_5_ECA</v>
+        <f aca="false">CONCATENATE("celexd:class_",M140)</f>
+        <v>celexd:class_5_ECA</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -42731,11 +42721,11 @@
         <v>5</v>
       </c>
       <c r="O141" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M141)</f>
-        <v>celexd:clc_5_COM</v>
-      </c>
-    </row>
-    <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">CONCATENATE("celexd:class_",M141)</f>
+        <v>celexd:class_5_COM</v>
+      </c>
+    </row>
+    <row r="142" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="2" t="str">
         <f aca="false">CONCATENATE("celexd:c_",B142)</f>
         <v>celexd:c_5_SC</v>
@@ -42766,8 +42756,8 @@
         <v>5</v>
       </c>
       <c r="O142" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M142)</f>
-        <v>celexd:clc_5_COM</v>
+        <f aca="false">CONCATENATE("celexd:class_",M142)</f>
+        <v>celexd:class_5_COM</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -42810,11 +42800,11 @@
         <v>5</v>
       </c>
       <c r="O143" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M143)</f>
-        <v>celexd:clc_5_COM</v>
-      </c>
-    </row>
-    <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">CONCATENATE("celexd:class_",M143)</f>
+        <v>celexd:class_5_COM</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="2" t="str">
         <f aca="false">CONCATENATE("celexd:c_",B144)</f>
         <v>celexd:c_5_SC_OJC</v>
@@ -42848,11 +42838,11 @@
         <v>5</v>
       </c>
       <c r="O144" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M144)</f>
-        <v>celexd:clc_5_COM</v>
-      </c>
-    </row>
-    <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">CONCATENATE("celexd:class_",M144)</f>
+        <v>celexd:class_5_COM</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="2" t="str">
         <f aca="false">CONCATENATE("celexd:c_",B145)</f>
         <v>celexd:c_5_SC_OJL</v>
@@ -42886,11 +42876,11 @@
         <v>5</v>
       </c>
       <c r="O145" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M145)</f>
-        <v>celexd:clc_5_ECA</v>
-      </c>
-    </row>
-    <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">CONCATENATE("celexd:class_",M145)</f>
+        <v>celexd:class_5_ECA</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="2" t="str">
         <f aca="false">CONCATENATE("celexd:c_",B146)</f>
         <v>celexd:c_5_TA</v>
@@ -42921,8 +42911,8 @@
         <v>5</v>
       </c>
       <c r="O146" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M146)</f>
-        <v>celexd:clc_5_ECA</v>
+        <f aca="false">CONCATENATE("celexd:class_",M146)</f>
+        <v>celexd:class_5_ECA</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -42965,11 +42955,11 @@
         <v>5</v>
       </c>
       <c r="O147" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M147)</f>
-        <v>celexd:clc_5_ECA</v>
-      </c>
-    </row>
-    <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">CONCATENATE("celexd:class_",M147)</f>
+        <v>celexd:class_5_ECA</v>
+      </c>
+    </row>
+    <row r="148" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="2" t="str">
         <f aca="false">CONCATENATE("celexd:c_",B148)</f>
         <v>celexd:c_5_XA</v>
@@ -43000,8 +42990,8 @@
         <v>5</v>
       </c>
       <c r="O148" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M148)</f>
-        <v>celexd:clc_5_ECA</v>
+        <f aca="false">CONCATENATE("celexd:class_",M148)</f>
+        <v>celexd:class_5_ECA</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43044,11 +43034,11 @@
         <v>5</v>
       </c>
       <c r="O149" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M149)</f>
-        <v>celexd:clc_5_ECB</v>
-      </c>
-    </row>
-    <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">CONCATENATE("celexd:class_",M149)</f>
+        <v>celexd:class_5_ECB</v>
+      </c>
+    </row>
+    <row r="150" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="2" t="str">
         <f aca="false">CONCATENATE("celexd:c_",B150)</f>
         <v>celexd:c_5_XB</v>
@@ -43079,8 +43069,8 @@
         <v>5</v>
       </c>
       <c r="O150" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M150)</f>
-        <v>celexd:clc_5_ECB</v>
+        <f aca="false">CONCATENATE("celexd:class_",M150)</f>
+        <v>celexd:class_5_ECB</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43123,11 +43113,11 @@
         <v>5</v>
       </c>
       <c r="O151" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M151)</f>
-        <v>celexd:clc_5_COM</v>
-      </c>
-    </row>
-    <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">CONCATENATE("celexd:class_",M151)</f>
+        <v>celexd:class_5_COM</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="2" t="str">
         <f aca="false">CONCATENATE("celexd:c_",B152)</f>
         <v>celexd:c_5_XC</v>
@@ -43158,8 +43148,8 @@
         <v>5</v>
       </c>
       <c r="O152" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M152)</f>
-        <v>celexd:clc_5_COM</v>
+        <f aca="false">CONCATENATE("celexd:class_",M152)</f>
+        <v>celexd:class_5_COM</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43202,11 +43192,11 @@
         <v>5</v>
       </c>
       <c r="O153" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M153)</f>
-        <v>celexd:clc_5_COM</v>
-      </c>
-    </row>
-    <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">CONCATENATE("celexd:class_",M153)</f>
+        <v>celexd:class_5_COM</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="2" t="str">
         <f aca="false">CONCATENATE("celexd:c_",B154)</f>
         <v>celexd:c_5_XC_OJL</v>
@@ -43249,8 +43239,8 @@
         <v>5</v>
       </c>
       <c r="O154" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M154)</f>
-        <v>celexd:clc_5_EESC</v>
+        <f aca="false">CONCATENATE("celexd:class_",M154)</f>
+        <v>celexd:class_5_EESC</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43284,8 +43274,8 @@
         <v>5</v>
       </c>
       <c r="O155" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M155)</f>
-        <v>celexd:clc_5_EESC</v>
+        <f aca="false">CONCATENATE("celexd:class_",M155)</f>
+        <v>celexd:class_5_EESC</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43331,8 +43321,8 @@
         <v>5</v>
       </c>
       <c r="O156" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M156)</f>
-        <v>celexd:clc_5_CONSIL</v>
+        <f aca="false">CONCATENATE("celexd:class_",M156)</f>
+        <v>celexd:class_5_CONSIL</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43366,8 +43356,8 @@
         <v>5</v>
       </c>
       <c r="O157" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M157)</f>
-        <v>celexd:clc_5_CONSIL</v>
+        <f aca="false">CONCATENATE("celexd:class_",M157)</f>
+        <v>celexd:class_5_CONSIL</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43410,8 +43400,8 @@
         <v>5</v>
       </c>
       <c r="O158" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M158)</f>
-        <v>celexd:clc_5_CONSIL</v>
+        <f aca="false">CONCATENATE("celexd:class_",M158)</f>
+        <v>celexd:class_5_CONSIL</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43457,11 +43447,11 @@
         <v>5</v>
       </c>
       <c r="O159" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M159)</f>
-        <v>celexd:clc_5_ECSC</v>
-      </c>
-    </row>
-    <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">CONCATENATE("celexd:class_",M159)</f>
+        <v>celexd:class_5_ECSC</v>
+      </c>
+    </row>
+    <row r="160" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="2" t="str">
         <f aca="false">CONCATENATE("celexd:c_",B160)</f>
         <v>celexd:c_5_XK</v>
@@ -43492,8 +43482,8 @@
         <v>5</v>
       </c>
       <c r="O160" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M160)</f>
-        <v>celexd:clc_5_ECSC</v>
+        <f aca="false">CONCATENATE("celexd:class_",M160)</f>
+        <v>celexd:class_5_ECSC</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43536,8 +43526,8 @@
         <v>5</v>
       </c>
       <c r="O161" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M161)</f>
-        <v>celexd:clc_5_EP</v>
+        <f aca="false">CONCATENATE("celexd:class_",M161)</f>
+        <v>celexd:class_5_EP</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43571,8 +43561,8 @@
         <v>5</v>
       </c>
       <c r="O162" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M162)</f>
-        <v>celexd:clc_5_EP</v>
+        <f aca="false">CONCATENATE("celexd:class_",M162)</f>
+        <v>celexd:class_5_EP</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43615,8 +43605,8 @@
         <v>5</v>
       </c>
       <c r="O163" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M163)</f>
-        <v>celexd:clc_5_COR</v>
+        <f aca="false">CONCATENATE("celexd:class_",M163)</f>
+        <v>celexd:class_5_COR</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43650,8 +43640,8 @@
         <v>5</v>
       </c>
       <c r="O164" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M164)</f>
-        <v>celexd:clc_5_COR</v>
+        <f aca="false">CONCATENATE("celexd:class_",M164)</f>
+        <v>celexd:class_5_COR</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43697,8 +43687,8 @@
         <v>5</v>
       </c>
       <c r="O165" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M165)</f>
-        <v>celexd:clc_5_OTHER</v>
+        <f aca="false">CONCATENATE("celexd:class_",M165)</f>
+        <v>celexd:class_5_OTHER</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43732,8 +43722,8 @@
         <v>5</v>
       </c>
       <c r="O166" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M166)</f>
-        <v>celexd:clc_5_OTHER</v>
+        <f aca="false">CONCATENATE("celexd:class_",M166)</f>
+        <v>celexd:class_5_OTHER</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43779,8 +43769,8 @@
         <v>5</v>
       </c>
       <c r="O167" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M167)</f>
-        <v>celexd:clc_5_OTHER</v>
+        <f aca="false">CONCATENATE("celexd:class_",M167)</f>
+        <v>celexd:class_5_OTHER</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43823,8 +43813,8 @@
         <v>6</v>
       </c>
       <c r="O168" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M168)</f>
-        <v>celexd:clc_6_CJ</v>
+        <f aca="false">CONCATENATE("celexd:class_",M168)</f>
+        <v>celexd:class_6_CJ</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43858,8 +43848,8 @@
         <v>6</v>
       </c>
       <c r="O169" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M169)</f>
-        <v>celexd:clc_6_CJ</v>
+        <f aca="false">CONCATENATE("celexd:class_",M169)</f>
+        <v>celexd:class_6_CJ</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43902,8 +43892,8 @@
         <v>6</v>
       </c>
       <c r="O170" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M170)</f>
-        <v>celexd:clc_6_CJ</v>
+        <f aca="false">CONCATENATE("celexd:class_",M170)</f>
+        <v>celexd:class_6_CJ</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43937,8 +43927,8 @@
         <v>6</v>
       </c>
       <c r="O171" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M171)</f>
-        <v>celexd:clc_6_CJ</v>
+        <f aca="false">CONCATENATE("celexd:class_",M171)</f>
+        <v>celexd:class_6_CJ</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43981,8 +43971,8 @@
         <v>6</v>
       </c>
       <c r="O172" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M172)</f>
-        <v>celexd:clc_6_CJ</v>
+        <f aca="false">CONCATENATE("celexd:class_",M172)</f>
+        <v>celexd:class_6_CJ</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -44016,8 +44006,8 @@
         <v>6</v>
       </c>
       <c r="O173" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M173)</f>
-        <v>celexd:clc_6_CJ</v>
+        <f aca="false">CONCATENATE("celexd:class_",M173)</f>
+        <v>celexd:class_6_CJ</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -44060,8 +44050,8 @@
         <v>6</v>
       </c>
       <c r="O174" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M174)</f>
-        <v>celexd:clc_6_CJ</v>
+        <f aca="false">CONCATENATE("celexd:class_",M174)</f>
+        <v>celexd:class_6_CJ</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -44095,8 +44085,8 @@
         <v>6</v>
       </c>
       <c r="O175" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M175)</f>
-        <v>celexd:clc_6_CJ</v>
+        <f aca="false">CONCATENATE("celexd:class_",M175)</f>
+        <v>celexd:class_6_CJ</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -44139,8 +44129,8 @@
         <v>6</v>
       </c>
       <c r="O176" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M176)</f>
-        <v>celexd:clc_6_CJ</v>
+        <f aca="false">CONCATENATE("celexd:class_",M176)</f>
+        <v>celexd:class_6_CJ</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -44174,8 +44164,8 @@
         <v>6</v>
       </c>
       <c r="O177" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M177)</f>
-        <v>celexd:clc_6_CJ</v>
+        <f aca="false">CONCATENATE("celexd:class_",M177)</f>
+        <v>celexd:class_6_CJ</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -44218,8 +44208,8 @@
         <v>6</v>
       </c>
       <c r="O178" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M178)</f>
-        <v>celexd:clc_6_CJ</v>
+        <f aca="false">CONCATENATE("celexd:class_",M178)</f>
+        <v>celexd:class_6_CJ</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -44253,8 +44243,8 @@
         <v>6</v>
       </c>
       <c r="O179" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M179)</f>
-        <v>celexd:clc_6_CJ</v>
+        <f aca="false">CONCATENATE("celexd:class_",M179)</f>
+        <v>celexd:class_6_CJ</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -44297,8 +44287,8 @@
         <v>6</v>
       </c>
       <c r="O180" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M180)</f>
-        <v>celexd:clc_6_CJ</v>
+        <f aca="false">CONCATENATE("celexd:class_",M180)</f>
+        <v>celexd:class_6_CJ</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -44332,8 +44322,8 @@
         <v>6</v>
       </c>
       <c r="O181" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M181)</f>
-        <v>celexd:clc_6_CJ</v>
+        <f aca="false">CONCATENATE("celexd:class_",M181)</f>
+        <v>celexd:class_6_CJ</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -44376,8 +44366,8 @@
         <v>6</v>
       </c>
       <c r="O182" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M182)</f>
-        <v>celexd:clc_6_CJ</v>
+        <f aca="false">CONCATENATE("celexd:class_",M182)</f>
+        <v>celexd:class_6_CJ</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -44411,8 +44401,8 @@
         <v>6</v>
       </c>
       <c r="O183" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M183)</f>
-        <v>celexd:clc_6_CJ</v>
+        <f aca="false">CONCATENATE("celexd:class_",M183)</f>
+        <v>celexd:class_6_CJ</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -44455,8 +44445,8 @@
         <v>6</v>
       </c>
       <c r="O184" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M184)</f>
-        <v>celexd:clc_6_CJ</v>
+        <f aca="false">CONCATENATE("celexd:class_",M184)</f>
+        <v>celexd:class_6_CJ</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -44490,8 +44480,8 @@
         <v>6</v>
       </c>
       <c r="O185" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M185)</f>
-        <v>celexd:clc_6_CJ</v>
+        <f aca="false">CONCATENATE("celexd:class_",M185)</f>
+        <v>celexd:class_6_CJ</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -44534,8 +44524,8 @@
         <v>6</v>
       </c>
       <c r="O186" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M186)</f>
-        <v>celexd:clc_6_CJ</v>
+        <f aca="false">CONCATENATE("celexd:class_",M186)</f>
+        <v>celexd:class_6_CJ</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -44569,8 +44559,8 @@
         <v>6</v>
       </c>
       <c r="O187" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M187)</f>
-        <v>celexd:clc_6_CJ</v>
+        <f aca="false">CONCATENATE("celexd:class_",M187)</f>
+        <v>celexd:class_6_CJ</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -44613,8 +44603,8 @@
         <v>6</v>
       </c>
       <c r="O188" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M188)</f>
-        <v>celexd:clc_6_CJ</v>
+        <f aca="false">CONCATENATE("celexd:class_",M188)</f>
+        <v>celexd:class_6_CJ</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -44648,8 +44638,8 @@
         <v>6</v>
       </c>
       <c r="O189" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M189)</f>
-        <v>celexd:clc_6_CJ</v>
+        <f aca="false">CONCATENATE("celexd:class_",M189)</f>
+        <v>celexd:class_6_CJ</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -44692,8 +44682,8 @@
         <v>6</v>
       </c>
       <c r="O190" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M190)</f>
-        <v>celexd:clc_6_CJ</v>
+        <f aca="false">CONCATENATE("celexd:class_",M190)</f>
+        <v>celexd:class_6_CJ</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -44727,8 +44717,8 @@
         <v>6</v>
       </c>
       <c r="O191" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M191)</f>
-        <v>celexd:clc_6_CJ</v>
+        <f aca="false">CONCATENATE("celexd:class_",M191)</f>
+        <v>celexd:class_6_CJ</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -44771,8 +44761,8 @@
         <v>6</v>
       </c>
       <c r="O192" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M192)</f>
-        <v>celexd:clc_6_CJ</v>
+        <f aca="false">CONCATENATE("celexd:class_",M192)</f>
+        <v>celexd:class_6_CJ</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -44806,8 +44796,8 @@
         <v>6</v>
       </c>
       <c r="O193" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M193)</f>
-        <v>celexd:clc_6_CJ</v>
+        <f aca="false">CONCATENATE("celexd:class_",M193)</f>
+        <v>celexd:class_6_CJ</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -44850,8 +44840,8 @@
         <v>6</v>
       </c>
       <c r="O194" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M194)</f>
-        <v>celexd:clc_6_CJ</v>
+        <f aca="false">CONCATENATE("celexd:class_",M194)</f>
+        <v>celexd:class_6_CJ</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -44885,8 +44875,8 @@
         <v>6</v>
       </c>
       <c r="O195" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M195)</f>
-        <v>celexd:clc_6_CJ</v>
+        <f aca="false">CONCATENATE("celexd:class_",M195)</f>
+        <v>celexd:class_6_CJ</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -44929,8 +44919,8 @@
         <v>6</v>
       </c>
       <c r="O196" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M196)</f>
-        <v>celexd:clc_6_CST</v>
+        <f aca="false">CONCATENATE("celexd:class_",M196)</f>
+        <v>celexd:class_6_CST</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -44964,8 +44954,8 @@
         <v>6</v>
       </c>
       <c r="O197" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M197)</f>
-        <v>celexd:clc_6_CST</v>
+        <f aca="false">CONCATENATE("celexd:class_",M197)</f>
+        <v>celexd:class_6_CST</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45008,8 +44998,8 @@
         <v>6</v>
       </c>
       <c r="O198" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M198)</f>
-        <v>celexd:clc_6_CST</v>
+        <f aca="false">CONCATENATE("celexd:class_",M198)</f>
+        <v>celexd:class_6_CST</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45043,8 +45033,8 @@
         <v>6</v>
       </c>
       <c r="O199" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M199)</f>
-        <v>celexd:clc_6_CST</v>
+        <f aca="false">CONCATENATE("celexd:class_",M199)</f>
+        <v>celexd:class_6_CST</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45087,8 +45077,8 @@
         <v>6</v>
       </c>
       <c r="O200" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M200)</f>
-        <v>celexd:clc_6_CST</v>
+        <f aca="false">CONCATENATE("celexd:class_",M200)</f>
+        <v>celexd:class_6_CST</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45122,8 +45112,8 @@
         <v>6</v>
       </c>
       <c r="O201" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M201)</f>
-        <v>celexd:clc_6_CST</v>
+        <f aca="false">CONCATENATE("celexd:class_",M201)</f>
+        <v>celexd:class_6_CST</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45166,8 +45156,8 @@
         <v>6</v>
       </c>
       <c r="O202" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M202)</f>
-        <v>celexd:clc_6_CST</v>
+        <f aca="false">CONCATENATE("celexd:class_",M202)</f>
+        <v>celexd:class_6_CST</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45201,8 +45191,8 @@
         <v>6</v>
       </c>
       <c r="O203" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M203)</f>
-        <v>celexd:clc_6_CST</v>
+        <f aca="false">CONCATENATE("celexd:class_",M203)</f>
+        <v>celexd:class_6_CST</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45245,8 +45235,8 @@
         <v>6</v>
       </c>
       <c r="O204" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M204)</f>
-        <v>celexd:clc_6_CST</v>
+        <f aca="false">CONCATENATE("celexd:class_",M204)</f>
+        <v>celexd:class_6_CST</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45280,8 +45270,8 @@
         <v>6</v>
       </c>
       <c r="O205" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M205)</f>
-        <v>celexd:clc_6_CST</v>
+        <f aca="false">CONCATENATE("celexd:class_",M205)</f>
+        <v>celexd:class_6_CST</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45324,8 +45314,8 @@
         <v>6</v>
       </c>
       <c r="O206" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M206)</f>
-        <v>celexd:clc_6_CST</v>
+        <f aca="false">CONCATENATE("celexd:class_",M206)</f>
+        <v>celexd:class_6_CST</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45359,11 +45349,11 @@
         <v>6</v>
       </c>
       <c r="O207" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M207)</f>
-        <v>celexd:clc_6_CST</v>
-      </c>
-    </row>
-    <row r="208" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">CONCATENATE("celexd:class_",M207)</f>
+        <v>celexd:class_6_CST</v>
+      </c>
+    </row>
+    <row r="208" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="2" t="str">
         <f aca="false">CONCATENATE("celexd:c_",B208)</f>
         <v>celexd:c_6_FT_EUR</v>
@@ -45400,11 +45390,11 @@
         <v>6</v>
       </c>
       <c r="O208" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M208)</f>
-        <v>celexd:clc_6_GCEU</v>
-      </c>
-    </row>
-    <row r="209" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">CONCATENATE("celexd:class_",M208)</f>
+        <v>celexd:class_6_GCEU</v>
+      </c>
+    </row>
+    <row r="209" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="2" t="str">
         <f aca="false">CONCATENATE("celexd:c_",B209)</f>
         <v>celexd:c_6_TA</v>
@@ -45435,8 +45425,8 @@
         <v>6</v>
       </c>
       <c r="O209" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M209)</f>
-        <v>celexd:clc_6_GCEU</v>
+        <f aca="false">CONCATENATE("celexd:class_",M209)</f>
+        <v>celexd:class_6_GCEU</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45479,11 +45469,11 @@
         <v>6</v>
       </c>
       <c r="O210" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M210)</f>
-        <v>celexd:clc_6_GCEU</v>
-      </c>
-    </row>
-    <row r="211" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">CONCATENATE("celexd:class_",M210)</f>
+        <v>celexd:class_6_GCEU</v>
+      </c>
+    </row>
+    <row r="211" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="2" t="str">
         <f aca="false">CONCATENATE("celexd:c_",B211)</f>
         <v>celexd:c_6_TB</v>
@@ -45514,8 +45504,8 @@
         <v>6</v>
       </c>
       <c r="O211" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M211)</f>
-        <v>celexd:clc_6_GCEU</v>
+        <f aca="false">CONCATENATE("celexd:class_",M211)</f>
+        <v>celexd:class_6_GCEU</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45558,11 +45548,11 @@
         <v>6</v>
       </c>
       <c r="O212" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M212)</f>
-        <v>celexd:clc_6_GCEU</v>
-      </c>
-    </row>
-    <row r="213" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">CONCATENATE("celexd:class_",M212)</f>
+        <v>celexd:class_6_GCEU</v>
+      </c>
+    </row>
+    <row r="213" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="2" t="str">
         <f aca="false">CONCATENATE("celexd:c_",B213)</f>
         <v>celexd:c_6_TC</v>
@@ -45593,8 +45583,8 @@
         <v>6</v>
       </c>
       <c r="O213" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M213)</f>
-        <v>celexd:clc_6_GCEU</v>
+        <f aca="false">CONCATENATE("celexd:class_",M213)</f>
+        <v>celexd:class_6_GCEU</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45637,11 +45627,11 @@
         <v>6</v>
       </c>
       <c r="O214" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M214)</f>
-        <v>celexd:clc_6_GCEU</v>
-      </c>
-    </row>
-    <row r="215" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">CONCATENATE("celexd:class_",M214)</f>
+        <v>celexd:class_6_GCEU</v>
+      </c>
+    </row>
+    <row r="215" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="2" t="str">
         <f aca="false">CONCATENATE("celexd:c_",B215)</f>
         <v>celexd:c_6_TJ</v>
@@ -45672,8 +45662,8 @@
         <v>6</v>
       </c>
       <c r="O215" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M215)</f>
-        <v>celexd:clc_6_GCEU</v>
+        <f aca="false">CONCATENATE("celexd:class_",M215)</f>
+        <v>celexd:class_6_GCEU</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45716,11 +45706,11 @@
         <v>6</v>
       </c>
       <c r="O216" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M216)</f>
-        <v>celexd:clc_6_GCEU</v>
-      </c>
-    </row>
-    <row r="217" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">CONCATENATE("celexd:class_",M216)</f>
+        <v>celexd:class_6_GCEU</v>
+      </c>
+    </row>
+    <row r="217" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="2" t="str">
         <f aca="false">CONCATENATE("celexd:c_",B217)</f>
         <v>celexd:c_6_TN</v>
@@ -45751,8 +45741,8 @@
         <v>6</v>
       </c>
       <c r="O217" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M217)</f>
-        <v>celexd:clc_6_GCEU</v>
+        <f aca="false">CONCATENATE("celexd:class_",M217)</f>
+        <v>celexd:class_6_GCEU</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45795,11 +45785,11 @@
         <v>6</v>
       </c>
       <c r="O218" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M218)</f>
-        <v>celexd:clc_6_GCEU</v>
-      </c>
-    </row>
-    <row r="219" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">CONCATENATE("celexd:class_",M218)</f>
+        <v>celexd:class_6_GCEU</v>
+      </c>
+    </row>
+    <row r="219" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="2" t="str">
         <f aca="false">CONCATENATE("celexd:c_",B219)</f>
         <v>celexd:c_6_TO</v>
@@ -45830,8 +45820,8 @@
         <v>6</v>
       </c>
       <c r="O219" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M219)</f>
-        <v>celexd:clc_6_GCEU</v>
+        <f aca="false">CONCATENATE("celexd:class_",M219)</f>
+        <v>celexd:class_6_GCEU</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45874,11 +45864,11 @@
         <v>6</v>
       </c>
       <c r="O220" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M220)</f>
-        <v>celexd:clc_6_GCEU</v>
-      </c>
-    </row>
-    <row r="221" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">CONCATENATE("celexd:class_",M220)</f>
+        <v>celexd:class_6_GCEU</v>
+      </c>
+    </row>
+    <row r="221" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="2" t="str">
         <f aca="false">CONCATENATE("celexd:c_",B221)</f>
         <v>celexd:c_6_TT</v>
@@ -45909,8 +45899,8 @@
         <v>6</v>
       </c>
       <c r="O221" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M221)</f>
-        <v>celexd:clc_6_GCEU</v>
+        <f aca="false">CONCATENATE("celexd:class_",M221)</f>
+        <v>celexd:class_6_GCEU</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45953,8 +45943,8 @@
         <v>6</v>
       </c>
       <c r="O222" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M222)</f>
-        <v>celexd:clc_6_GCEU</v>
+        <f aca="false">CONCATENATE("celexd:class_",M222)</f>
+        <v>celexd:class_6_GCEU</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45988,8 +45978,8 @@
         <v>8</v>
       </c>
       <c r="O223" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M223)</f>
-        <v>celexd:clc_8</v>
+        <f aca="false">CONCATENATE("celexd:class_",M223)</f>
+        <v>celexd:class_8</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -46020,8 +46010,8 @@
         <v>8</v>
       </c>
       <c r="O224" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M224)</f>
-        <v>celexd:clc_8</v>
+        <f aca="false">CONCATENATE("celexd:class_",M224)</f>
+        <v>celexd:class_8</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -46052,8 +46042,8 @@
         <v>8</v>
       </c>
       <c r="O225" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M225)</f>
-        <v>celexd:clc_8</v>
+        <f aca="false">CONCATENATE("celexd:class_",M225)</f>
+        <v>celexd:class_8</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -46084,8 +46074,8 @@
         <v>8</v>
       </c>
       <c r="O226" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M226)</f>
-        <v>celexd:clc_8</v>
+        <f aca="false">CONCATENATE("celexd:class_",M226)</f>
+        <v>celexd:class_8</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -46116,8 +46106,8 @@
         <v>8</v>
       </c>
       <c r="O227" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M227)</f>
-        <v>celexd:clc_8</v>
+        <f aca="false">CONCATENATE("celexd:class_",M227)</f>
+        <v>celexd:class_8</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -46148,8 +46138,8 @@
         <v>8</v>
       </c>
       <c r="O228" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M228)</f>
-        <v>celexd:clc_8</v>
+        <f aca="false">CONCATENATE("celexd:class_",M228)</f>
+        <v>celexd:class_8</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -46180,8 +46170,8 @@
         <v>8</v>
       </c>
       <c r="O229" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M229)</f>
-        <v>celexd:clc_8</v>
+        <f aca="false">CONCATENATE("celexd:class_",M229)</f>
+        <v>celexd:class_8</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -46212,8 +46202,8 @@
         <v>8</v>
       </c>
       <c r="O230" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M230)</f>
-        <v>celexd:clc_8</v>
+        <f aca="false">CONCATENATE("celexd:class_",M230)</f>
+        <v>celexd:class_8</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -46244,8 +46234,8 @@
         <v>8</v>
       </c>
       <c r="O231" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M231)</f>
-        <v>celexd:clc_8</v>
+        <f aca="false">CONCATENATE("celexd:class_",M231)</f>
+        <v>celexd:class_8</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -46276,8 +46266,8 @@
         <v>8</v>
       </c>
       <c r="O232" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M232)</f>
-        <v>celexd:clc_8</v>
+        <f aca="false">CONCATENATE("celexd:class_",M232)</f>
+        <v>celexd:class_8</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -46308,8 +46298,8 @@
         <v>8</v>
       </c>
       <c r="O233" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M233)</f>
-        <v>celexd:clc_8</v>
+        <f aca="false">CONCATENATE("celexd:class_",M233)</f>
+        <v>celexd:class_8</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -46340,8 +46330,8 @@
         <v>8</v>
       </c>
       <c r="O234" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M234)</f>
-        <v>celexd:clc_8</v>
+        <f aca="false">CONCATENATE("celexd:class_",M234)</f>
+        <v>celexd:class_8</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -46372,8 +46362,8 @@
         <v>8</v>
       </c>
       <c r="O235" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M235)</f>
-        <v>celexd:clc_8</v>
+        <f aca="false">CONCATENATE("celexd:class_",M235)</f>
+        <v>celexd:class_8</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -46404,8 +46394,8 @@
         <v>8</v>
       </c>
       <c r="O236" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M236)</f>
-        <v>celexd:clc_8</v>
+        <f aca="false">CONCATENATE("celexd:class_",M236)</f>
+        <v>celexd:class_8</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -46436,8 +46426,8 @@
         <v>8</v>
       </c>
       <c r="O237" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M237)</f>
-        <v>celexd:clc_8</v>
+        <f aca="false">CONCATENATE("celexd:class_",M237)</f>
+        <v>celexd:class_8</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -46468,8 +46458,8 @@
         <v>8</v>
       </c>
       <c r="O238" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M238)</f>
-        <v>celexd:clc_8</v>
+        <f aca="false">CONCATENATE("celexd:class_",M238)</f>
+        <v>celexd:class_8</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -46500,8 +46490,8 @@
         <v>8</v>
       </c>
       <c r="O239" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M239)</f>
-        <v>celexd:clc_8</v>
+        <f aca="false">CONCATENATE("celexd:class_",M239)</f>
+        <v>celexd:class_8</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -46532,8 +46522,8 @@
         <v>8</v>
       </c>
       <c r="O240" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M240)</f>
-        <v>celexd:clc_8</v>
+        <f aca="false">CONCATENATE("celexd:class_",M240)</f>
+        <v>celexd:class_8</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -46564,8 +46554,8 @@
         <v>8</v>
       </c>
       <c r="O241" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M241)</f>
-        <v>celexd:clc_8</v>
+        <f aca="false">CONCATENATE("celexd:class_",M241)</f>
+        <v>celexd:class_8</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -46596,8 +46586,8 @@
         <v>8</v>
       </c>
       <c r="O242" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M242)</f>
-        <v>celexd:clc_8</v>
+        <f aca="false">CONCATENATE("celexd:class_",M242)</f>
+        <v>celexd:class_8</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -46628,8 +46618,8 @@
         <v>8</v>
       </c>
       <c r="O243" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M243)</f>
-        <v>celexd:clc_8</v>
+        <f aca="false">CONCATENATE("celexd:class_",M243)</f>
+        <v>celexd:class_8</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -46660,8 +46650,8 @@
         <v>8</v>
       </c>
       <c r="O244" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M244)</f>
-        <v>celexd:clc_8</v>
+        <f aca="false">CONCATENATE("celexd:class_",M244)</f>
+        <v>celexd:class_8</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -46692,8 +46682,8 @@
         <v>8</v>
       </c>
       <c r="O245" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M245)</f>
-        <v>celexd:clc_8</v>
+        <f aca="false">CONCATENATE("celexd:class_",M245)</f>
+        <v>celexd:class_8</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -46724,8 +46714,8 @@
         <v>8</v>
       </c>
       <c r="O246" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M246)</f>
-        <v>celexd:clc_8</v>
+        <f aca="false">CONCATENATE("celexd:class_",M246)</f>
+        <v>celexd:class_8</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -46756,8 +46746,8 @@
         <v>8</v>
       </c>
       <c r="O247" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M247)</f>
-        <v>celexd:clc_8</v>
+        <f aca="false">CONCATENATE("celexd:class_",M247)</f>
+        <v>celexd:class_8</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -46788,8 +46778,8 @@
         <v>8</v>
       </c>
       <c r="O248" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M248)</f>
-        <v>celexd:clc_8</v>
+        <f aca="false">CONCATENATE("celexd:class_",M248)</f>
+        <v>celexd:class_8</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -46820,8 +46810,8 @@
         <v>8</v>
       </c>
       <c r="O249" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M249)</f>
-        <v>celexd:clc_8</v>
+        <f aca="false">CONCATENATE("celexd:class_",M249)</f>
+        <v>celexd:class_8</v>
       </c>
     </row>
     <row r="250" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -46852,8 +46842,8 @@
         <v>8</v>
       </c>
       <c r="O250" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M250)</f>
-        <v>celexd:clc_8</v>
+        <f aca="false">CONCATENATE("celexd:class_",M250)</f>
+        <v>celexd:class_8</v>
       </c>
     </row>
     <row r="251" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -46884,8 +46874,8 @@
         <v>8</v>
       </c>
       <c r="O251" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M251)</f>
-        <v>celexd:clc_8</v>
+        <f aca="false">CONCATENATE("celexd:class_",M251)</f>
+        <v>celexd:class_8</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -46906,7 +46896,7 @@
       <c r="E252" s="2" t="s">
         <v>2131</v>
       </c>
-      <c r="F252" s="29" t="s">
+      <c r="F252" s="28" t="s">
         <v>2132</v>
       </c>
       <c r="H252" s="2" t="n">
@@ -46919,8 +46909,8 @@
         <v>9</v>
       </c>
       <c r="O252" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M252)</f>
-        <v>celexd:clc_9</v>
+        <f aca="false">CONCATENATE("celexd:class_",M252)</f>
+        <v>celexd:class_9</v>
       </c>
     </row>
     <row r="253" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -46954,8 +46944,8 @@
         <v>9</v>
       </c>
       <c r="O253" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M253)</f>
-        <v>celexd:clc_9</v>
+        <f aca="false">CONCATENATE("celexd:class_",M253)</f>
+        <v>celexd:class_9</v>
       </c>
     </row>
     <row r="254" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -46989,8 +46979,8 @@
         <v>9</v>
       </c>
       <c r="O254" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M254)</f>
-        <v>celexd:clc_9</v>
+        <f aca="false">CONCATENATE("celexd:class_",M254)</f>
+        <v>celexd:class_9</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -47015,8 +47005,8 @@
         <v>1464</v>
       </c>
       <c r="O255" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M255)</f>
-        <v>celexd:clc_C</v>
+        <f aca="false">CONCATENATE("celexd:class_",M255)</f>
+        <v>celexd:class_C</v>
       </c>
     </row>
     <row r="256" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -47041,8 +47031,8 @@
         <v>1486</v>
       </c>
       <c r="O256" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M256)</f>
-        <v>celexd:clc_E</v>
+        <f aca="false">CONCATENATE("celexd:class_",M256)</f>
+        <v>celexd:class_E</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -47073,8 +47063,8 @@
         <v>1486</v>
       </c>
       <c r="O257" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M257)</f>
-        <v>celexd:clc_E</v>
+        <f aca="false">CONCATENATE("celexd:class_",M257)</f>
+        <v>celexd:class_E</v>
       </c>
     </row>
     <row r="258" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -47114,8 +47104,8 @@
         <v>1486</v>
       </c>
       <c r="O258" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M258)</f>
-        <v>celexd:clc_E</v>
+        <f aca="false">CONCATENATE("celexd:class_",M258)</f>
+        <v>celexd:class_E</v>
       </c>
     </row>
     <row r="259" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -47158,8 +47148,8 @@
         <v>1486</v>
       </c>
       <c r="O259" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M259)</f>
-        <v>celexd:clc_E</v>
+        <f aca="false">CONCATENATE("celexd:class_",M259)</f>
+        <v>celexd:class_E</v>
       </c>
     </row>
     <row r="260" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -47190,8 +47180,8 @@
         <v>1486</v>
       </c>
       <c r="O260" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M260)</f>
-        <v>celexd:clc_E</v>
+        <f aca="false">CONCATENATE("celexd:class_",M260)</f>
+        <v>celexd:class_E</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -47231,8 +47221,8 @@
         <v>1486</v>
       </c>
       <c r="O261" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M261)</f>
-        <v>celexd:clc_E</v>
+        <f aca="false">CONCATENATE("celexd:class_",M261)</f>
+        <v>celexd:class_E</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -47272,8 +47262,8 @@
         <v>1486</v>
       </c>
       <c r="O262" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M262)</f>
-        <v>celexd:clc_E</v>
+        <f aca="false">CONCATENATE("celexd:class_",M262)</f>
+        <v>celexd:class_E</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -47304,8 +47294,8 @@
         <v>1486</v>
       </c>
       <c r="O263" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M263)</f>
-        <v>celexd:clc_E</v>
+        <f aca="false">CONCATENATE("celexd:class_",M263)</f>
+        <v>celexd:class_E</v>
       </c>
     </row>
     <row r="264" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -47345,8 +47335,8 @@
         <v>1486</v>
       </c>
       <c r="O264" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M264)</f>
-        <v>celexd:clc_E</v>
+        <f aca="false">CONCATENATE("celexd:class_",M264)</f>
+        <v>celexd:class_E</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -47386,8 +47376,8 @@
         <v>1486</v>
       </c>
       <c r="O265" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M265)</f>
-        <v>celexd:clc_E</v>
+        <f aca="false">CONCATENATE("celexd:class_",M265)</f>
+        <v>celexd:class_E</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -47418,8 +47408,8 @@
         <v>1486</v>
       </c>
       <c r="O266" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M266)</f>
-        <v>celexd:clc_E</v>
+        <f aca="false">CONCATENATE("celexd:class_",M266)</f>
+        <v>celexd:class_E</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -47459,8 +47449,8 @@
         <v>1486</v>
       </c>
       <c r="O267" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M267)</f>
-        <v>celexd:clc_E</v>
+        <f aca="false">CONCATENATE("celexd:class_",M267)</f>
+        <v>celexd:class_E</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -47503,8 +47493,8 @@
         <v>1486</v>
       </c>
       <c r="O268" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M268)</f>
-        <v>celexd:clc_E</v>
+        <f aca="false">CONCATENATE("celexd:class_",M268)</f>
+        <v>celexd:class_E</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -47535,8 +47525,8 @@
         <v>1486</v>
       </c>
       <c r="O269" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M269)</f>
-        <v>celexd:clc_E</v>
+        <f aca="false">CONCATENATE("celexd:class_",M269)</f>
+        <v>celexd:class_E</v>
       </c>
     </row>
     <row r="270" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -47570,8 +47560,8 @@
         <v>1486</v>
       </c>
       <c r="O270" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M270)</f>
-        <v>celexd:clc_E</v>
+        <f aca="false">CONCATENATE("celexd:class_",M270)</f>
+        <v>celexd:class_E</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -47605,8 +47595,8 @@
         <v>1486</v>
       </c>
       <c r="O271" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M271)</f>
-        <v>celexd:clc_E</v>
+        <f aca="false">CONCATENATE("celexd:class_",M271)</f>
+        <v>celexd:class_E</v>
       </c>
     </row>
     <row r="272" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -47637,8 +47627,8 @@
         <v>1486</v>
       </c>
       <c r="O272" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M272)</f>
-        <v>celexd:clc_E</v>
+        <f aca="false">CONCATENATE("celexd:class_",M272)</f>
+        <v>celexd:class_E</v>
       </c>
     </row>
     <row r="273" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -47678,8 +47668,8 @@
         <v>1486</v>
       </c>
       <c r="O273" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M273)</f>
-        <v>celexd:clc_E</v>
+        <f aca="false">CONCATENATE("celexd:class_",M273)</f>
+        <v>celexd:class_E</v>
       </c>
     </row>
     <row r="274" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -47710,8 +47700,8 @@
         <v>1486</v>
       </c>
       <c r="O274" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M274)</f>
-        <v>celexd:clc_E</v>
+        <f aca="false">CONCATENATE("celexd:class_",M274)</f>
+        <v>celexd:class_E</v>
       </c>
     </row>
     <row r="275" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -47751,8 +47741,8 @@
         <v>1486</v>
       </c>
       <c r="O275" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M275)</f>
-        <v>celexd:clc_E</v>
+        <f aca="false">CONCATENATE("celexd:class_",M275)</f>
+        <v>celexd:class_E</v>
       </c>
     </row>
     <row r="276" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -47795,8 +47785,8 @@
         <v>1486</v>
       </c>
       <c r="O276" s="23" t="str">
-        <f aca="false">CONCATENATE("celexd:clc_",M276)</f>
-        <v>celexd:clc_E</v>
+        <f aca="false">CONCATENATE("celexd:class_",M276)</f>
+        <v>celexd:class_E</v>
       </c>
     </row>
   </sheetData>
@@ -47820,13 +47810,13 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="30" width="23.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="29" width="23.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.42"/>
@@ -47838,7 +47828,7 @@
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="30" t="s">
         <v>37</v>
       </c>
       <c r="C1" s="5" t="s">
@@ -47865,10 +47855,10 @@
         <f aca="false">CONCATENATE("celex_classif:class_",B2)</f>
         <v>celex_classif:class_1</v>
       </c>
-      <c r="B2" s="30" t="n">
+      <c r="B2" s="29" t="n">
         <v>1</v>
       </c>
-      <c r="C2" s="28" t="str">
+      <c r="C2" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D2)),CONCATENATE("celex_classif:class_",D2),""  )</f>
         <v/>
       </c>
@@ -47884,10 +47874,10 @@
         <f aca="false">CONCATENATE("celex_classif:class_",B3)</f>
         <v>celex_classif:class_2</v>
       </c>
-      <c r="B3" s="30" t="n">
+      <c r="B3" s="29" t="n">
         <v>2</v>
       </c>
-      <c r="C3" s="28" t="str">
+      <c r="C3" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D3)),CONCATENATE("celex_classif:class_",D3),""  )</f>
         <v/>
       </c>
@@ -47903,10 +47893,10 @@
         <f aca="false">CONCATENATE("celex_classif:class_",B4)</f>
         <v>celex_classif:class_3</v>
       </c>
-      <c r="B4" s="30" t="n">
+      <c r="B4" s="29" t="n">
         <v>3</v>
       </c>
-      <c r="C4" s="28" t="str">
+      <c r="C4" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D4)),CONCATENATE("celex_classif:class_",D4),""  )</f>
         <v/>
       </c>
@@ -47922,10 +47912,10 @@
         <f aca="false">CONCATENATE("celex_classif:class_",B5)</f>
         <v>celex_classif:class_5</v>
       </c>
-      <c r="B5" s="30" t="n">
+      <c r="B5" s="29" t="n">
         <v>5</v>
       </c>
-      <c r="C5" s="28" t="str">
+      <c r="C5" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D5)),CONCATENATE("celex_classif:class_",D5),""  )</f>
         <v/>
       </c>
@@ -47941,10 +47931,10 @@
         <f aca="false">CONCATENATE("celex_classif:class_",B6)</f>
         <v>celex_classif:class_5</v>
       </c>
-      <c r="B6" s="30" t="n">
+      <c r="B6" s="29" t="n">
         <v>5</v>
       </c>
-      <c r="C6" s="28" t="str">
+      <c r="C6" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D6)),CONCATENATE("celex_classif:class_",D6),""  )</f>
         <v/>
       </c>
@@ -47960,10 +47950,10 @@
         <f aca="false">CONCATENATE("celex_classif:class_",B7)</f>
         <v>celex_classif:class_5_CONSIL</v>
       </c>
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="29" t="s">
         <v>1650</v>
       </c>
-      <c r="C7" s="28" t="str">
+      <c r="C7" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D7)),CONCATENATE("celex_classif:class_",D7),""  )</f>
         <v>celex_classif:class_5</v>
       </c>
@@ -47982,10 +47972,10 @@
         <f aca="false">CONCATENATE("celex_classif:class_",B8)</f>
         <v>celex_classif:class_5_COM</v>
       </c>
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="29" t="s">
         <v>1709</v>
       </c>
-      <c r="C8" s="28" t="str">
+      <c r="C8" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D8)),CONCATENATE("celex_classif:class_",D8),""  )</f>
         <v>celex_classif:class_5</v>
       </c>
@@ -48004,10 +47994,10 @@
         <f aca="false">CONCATENATE("celex_classif:class_",B9)</f>
         <v>celex_classif:class_5_EP</v>
       </c>
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="29" t="s">
         <v>1663</v>
       </c>
-      <c r="C9" s="28" t="str">
+      <c r="C9" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D9)),CONCATENATE("celex_classif:class_",D9),""  )</f>
         <v>celex_classif:class_5</v>
       </c>
@@ -48026,10 +48016,10 @@
         <f aca="false">CONCATENATE("celex_classif:class_",B10)</f>
         <v>celex_classif:class_5_ECA</v>
       </c>
-      <c r="B10" s="30" t="s">
+      <c r="B10" s="29" t="s">
         <v>1617</v>
       </c>
-      <c r="C10" s="28" t="str">
+      <c r="C10" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D10)),CONCATENATE("celex_classif:class_",D10),""  )</f>
         <v>celex_classif:class_5</v>
       </c>
@@ -48048,10 +48038,10 @@
         <f aca="false">CONCATENATE("celex_classif:class_",B11)</f>
         <v>celex_classif:class_5_ECB</v>
       </c>
-      <c r="B11" s="30" t="s">
+      <c r="B11" s="29" t="s">
         <v>1625</v>
       </c>
-      <c r="C11" s="28" t="str">
+      <c r="C11" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D11)),CONCATENATE("celex_classif:class_",D11),""  )</f>
         <v>celex_classif:class_5</v>
       </c>
@@ -48070,10 +48060,10 @@
         <f aca="false">CONCATENATE("celex_classif:class_",B12)</f>
         <v>celex_classif:class_5_EESC</v>
       </c>
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="29" t="s">
         <v>1633</v>
       </c>
-      <c r="C12" s="28" t="str">
+      <c r="C12" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D12)),CONCATENATE("celex_classif:class_",D12),""  )</f>
         <v>celex_classif:class_5</v>
       </c>
@@ -48092,10 +48082,10 @@
         <f aca="false">CONCATENATE("celex_classif:class_",B13)</f>
         <v>celex_classif:class_5_COR</v>
       </c>
-      <c r="B13" s="30" t="s">
+      <c r="B13" s="29" t="s">
         <v>1677</v>
       </c>
-      <c r="C13" s="28" t="str">
+      <c r="C13" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D13)),CONCATENATE("celex_classif:class_",D13),""  )</f>
         <v>celex_classif:class_5</v>
       </c>
@@ -48114,10 +48104,10 @@
         <f aca="false">CONCATENATE("celex_classif:class_",B14)</f>
         <v>celex_classif:class_5_ECSC</v>
       </c>
-      <c r="B14" s="30" t="s">
+      <c r="B14" s="29" t="s">
         <v>1657</v>
       </c>
-      <c r="C14" s="28" t="str">
+      <c r="C14" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D14)),CONCATENATE("celex_classif:class_",D14),""  )</f>
         <v>celex_classif:class_5</v>
       </c>
@@ -48136,10 +48126,10 @@
         <f aca="false">CONCATENATE("celex_classif:class_",B15)</f>
         <v>celex_classif:class_5_OTHER</v>
       </c>
-      <c r="B15" s="30" t="s">
+      <c r="B15" s="29" t="s">
         <v>1685</v>
       </c>
-      <c r="C15" s="28" t="str">
+      <c r="C15" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D15)),CONCATENATE("celex_classif:class_",D15),""  )</f>
         <v>celex_classif:class_5</v>
       </c>
@@ -48158,10 +48148,10 @@
         <f aca="false">CONCATENATE("celex_classif:class_",B16)</f>
         <v>celex_classif:class_6</v>
       </c>
-      <c r="B16" s="30" t="n">
+      <c r="B16" s="29" t="n">
         <v>6</v>
       </c>
-      <c r="C16" s="28" t="str">
+      <c r="C16" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D16)),CONCATENATE("celex_classif:class_",D16),""  )</f>
         <v/>
       </c>
@@ -48177,10 +48167,10 @@
         <f aca="false">CONCATENATE("celex_classif:class_",B17)</f>
         <v>celex_classif:class_6_CJ</v>
       </c>
-      <c r="B17" s="30" t="s">
+      <c r="B17" s="29" t="s">
         <v>1908</v>
       </c>
-      <c r="C17" s="28" t="str">
+      <c r="C17" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D17)),CONCATENATE("celex_classif:class_",D17),""  )</f>
         <v>celex_classif:class_6</v>
       </c>
@@ -48199,10 +48189,10 @@
         <f aca="false">CONCATENATE("celex_classif:class_",B18)</f>
         <v>celex_classif:class_6_GCEU</v>
       </c>
-      <c r="B18" s="30" t="s">
+      <c r="B18" s="29" t="s">
         <v>2016</v>
       </c>
-      <c r="C18" s="28" t="str">
+      <c r="C18" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D18)),CONCATENATE("celex_classif:class_",D18),""  )</f>
         <v>celex_classif:class_6</v>
       </c>
@@ -48221,10 +48211,10 @@
         <f aca="false">CONCATENATE("celex_classif:class_",B19)</f>
         <v>celex_classif:class_6_CST</v>
       </c>
-      <c r="B19" s="30" t="s">
+      <c r="B19" s="29" t="s">
         <v>1991</v>
       </c>
-      <c r="C19" s="28" t="str">
+      <c r="C19" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D19)),CONCATENATE("celex_classif:class_",D19),""  )</f>
         <v>celex_classif:class_6</v>
       </c>
@@ -48243,10 +48233,10 @@
         <f aca="false">CONCATENATE("celex_classif:class_",B20)</f>
         <v>celex_classif:class_7</v>
       </c>
-      <c r="B20" s="30" t="n">
+      <c r="B20" s="29" t="n">
         <v>7</v>
       </c>
-      <c r="C20" s="28" t="str">
+      <c r="C20" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D20)),CONCATENATE("celex_classif:class_",D20),""  )</f>
         <v/>
       </c>
@@ -48262,10 +48252,10 @@
         <f aca="false">CONCATENATE("celex_classif:class_",B21)</f>
         <v>celex_classif:class_8</v>
       </c>
-      <c r="B21" s="30" t="n">
+      <c r="B21" s="29" t="n">
         <v>8</v>
       </c>
-      <c r="C21" s="28" t="str">
+      <c r="C21" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D21)),CONCATENATE("celex_classif:class_",D21),""  )</f>
         <v/>
       </c>
@@ -48281,10 +48271,10 @@
         <f aca="false">CONCATENATE("celex_classif:class_",B22)</f>
         <v>celex_classif:class_9</v>
       </c>
-      <c r="B22" s="30" t="n">
+      <c r="B22" s="29" t="n">
         <v>9</v>
       </c>
-      <c r="C22" s="28" t="str">
+      <c r="C22" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D22)),CONCATENATE("celex_classif:class_",D22),""  )</f>
         <v/>
       </c>
@@ -48300,10 +48290,10 @@
         <f aca="false">CONCATENATE("celex_classif:class_",B23)</f>
         <v>celex_classif:class_E</v>
       </c>
-      <c r="B23" s="30" t="s">
+      <c r="B23" s="29" t="s">
         <v>1486</v>
       </c>
-      <c r="C23" s="28" t="str">
+      <c r="C23" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D23)),CONCATENATE("celex_classif:class_",D23),""  )</f>
         <v/>
       </c>
@@ -48319,10 +48309,10 @@
         <f aca="false">CONCATENATE("celex_classif:class_",B24)</f>
         <v>celex_classif:class_C</v>
       </c>
-      <c r="B24" s="30" t="s">
+      <c r="B24" s="29" t="s">
         <v>1464</v>
       </c>
-      <c r="C24" s="28" t="str">
+      <c r="C24" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D24)),CONCATENATE("celex_classif:class_",D24),""  )</f>
         <v/>
       </c>
@@ -48338,10 +48328,10 @@
         <f aca="false">CONCATENATE("celex_classif:class_",B25)</f>
         <v>celex_classif:class_0</v>
       </c>
-      <c r="B25" s="30" t="n">
+      <c r="B25" s="29" t="n">
         <v>0</v>
       </c>
-      <c r="C25" s="28" t="str">
+      <c r="C25" s="21" t="str">
         <f aca="false">IF(NOT(ISBLANK(D25)),CONCATENATE("celex_classif:class_",D25),""  )</f>
         <v/>
       </c>
@@ -48374,7 +48364,7 @@
       <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.19140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.2109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="61.24"/>
@@ -48514,7 +48504,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="28" t="s">
+      <c r="A18" s="21" t="s">
         <v>2245</v>
       </c>
       <c r="B18" s="0" t="s">
@@ -48546,7 +48536,7 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="28" t="s">
+      <c r="A22" s="21" t="s">
         <v>2251</v>
       </c>
       <c r="B22" s="0" t="s">
@@ -48832,7 +48822,7 @@
       <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.19140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.2109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="80.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.28"/>

</xml_diff>

<commit_message>
corrected non-unicode characters in teh Excel file
</commit_message>
<xml_diff>
--- a/resources/input_workbook/LAM_metadata_20200903_JKU.xlsx
+++ b/resources/input_workbook/LAM_metadata_20200903_JKU.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="LAM properties" sheetId="1" state="visible" r:id="rId2"/>
@@ -2338,7 +2338,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">If descriptors are incorrectly used (not relevant, out of context), the query system will retrieve several but irrelevant documents, there will be a 'noise'  In that case, incorrect descriptors have to be deleted. 
+      <t xml:space="preserve">If descriptors are incorrectly used (not relevant, out of context), the query system will retrieve several but irrelevant documents, there will be a 'noise' In that case, incorrect descriptors have to be deleted. 
 The use of incorrect descriptors is due to: 
 • either the misunderstanding of the content of the document
 • or to the defect in examining the contextual and semantic environment of the selected descriptor (non-preferred terms, related terms, hierarchy, notes) which may lead to the misunderstanding of the selected descriptor
@@ -9901,7 +9901,7 @@
       </rPr>
       <t xml:space="preserve">In force indicator is applicable only to certain acts (EU legal acts - legislative and non-legislative acts, treaties, international agreements plus some other cases).
 This field is generated automatically, based on the end of validity date and date of effect. Values are true or false.
-If there is at least one IF ≤ TODAY and at least one EV ≥ TODAY is present in the notice, true is inserted. 
+If there is at least one IF &lt; TODAY and at least one EV &gt; TODAY is present in the notice, true is inserted. 
 If date of entry into force is not yet known (0001-01-01; e.g. cases where it is linked to the date of notification), false is inserted. 
 Ephemeral notices are excluded (value EPH present in manifestation_official-journal_part_durability):
 </t>
@@ -19876,9 +19876,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>218880</xdr:colOff>
+      <xdr:colOff>218520</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>668520</xdr:rowOff>
+      <xdr:rowOff>668160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -19888,7 +19888,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="7829280" cy="8162640"/>
+          <a:ext cx="7828920" cy="8162280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -19923,7 +19923,7 @@
       <xdr:col>27</xdr:col>
       <xdr:colOff>636120</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>2036160</xdr:rowOff>
+      <xdr:rowOff>2035800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -19933,7 +19933,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="10038240" cy="9530280"/>
+          <a:ext cx="10038240" cy="9529920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -19971,9 +19971,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>452880</xdr:colOff>
+      <xdr:colOff>452520</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>172440</xdr:rowOff>
+      <xdr:rowOff>172080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -19983,7 +19983,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="17857440" cy="4626720"/>
+          <a:ext cx="17857800" cy="4626360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -20022,10 +20022,10 @@
   </sheetPr>
   <dimension ref="A1:AK118"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="AJ2" activeCellId="0" sqref="AJ2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AD1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="AD1" activeCellId="0" sqref="AD1"/>
+      <selection pane="bottomLeft" activeCell="AD31" activeCellId="0" sqref="AD31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="2"/>
@@ -20840,7 +20840,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="3276.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B15)</f>
         <v>lamd:md_DC</v>
@@ -21889,7 +21889,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="393.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B31)</f>
         <v>lamd:md_VV</v>
@@ -28055,10 +28055,10 @@
   <dimension ref="A1:J49"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.2265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.7"/>
@@ -36583,7 +36583,7 @@
       <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.1"/>
@@ -47807,7 +47807,7 @@
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="29" width="23.42"/>
@@ -48354,11 +48354,11 @@
   </sheetPr>
   <dimension ref="A1:B1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.2265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="61.24"/>
@@ -48802,7 +48802,7 @@
       <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.2265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="80.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.28"/>

</xml_diff>